<commit_message>
Adjusting the mobile port
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="2186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2266" uniqueCount="2192">
   <si>
     <t>myself</t>
   </si>
@@ -8408,6 +8408,30 @@
   </si>
   <si>
     <t>VALUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userNameEmpty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passwordEmpty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The password cannot be empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The username cannot be empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginSuccessfully</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login Successfully</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8808,10 +8832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -8854,7 +8878,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -8864,323 +8888,323 @@
         <v>971</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="12" t="s">
+        <v>2186</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>972</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>2187</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>1962</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>1963</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>2190</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>2191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>1802</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>1801</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>1804</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>1803</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>1621</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>1620</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>1942</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>1941</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>2040</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>2039</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>977</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>978</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>980</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>1988</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>2020</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>2021</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -9188,10 +9212,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>982</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -9199,10 +9223,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>983</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -9210,10 +9234,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>141</v>
+        <v>2020</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>984</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -9221,10 +9245,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>367</v>
+        <v>52</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -9232,10 +9256,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>368</v>
+        <v>119</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -9243,10 +9267,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -9254,10 +9278,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>299</v>
+        <v>367</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -9265,10 +9289,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>298</v>
+        <v>368</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -9276,10 +9300,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -9287,10 +9311,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>137</v>
+        <v>299</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>140</v>
+        <v>988</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -9298,10 +9322,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>138</v>
+        <v>298</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -9309,10 +9333,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -9320,10 +9344,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>993</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -9331,10 +9355,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -9342,10 +9366,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1966</v>
+        <v>139</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1967</v>
+        <v>992</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -9353,10 +9377,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>917</v>
+        <v>132</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -9364,10 +9388,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>918</v>
+        <v>142</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -9375,10 +9399,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>133</v>
+        <v>1966</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>997</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -9386,10 +9410,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>134</v>
+        <v>917</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -9397,10 +9421,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>135</v>
+        <v>918</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -9408,10 +9432,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>31</v>
+        <v>133</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -9419,10 +9443,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>2054</v>
+        <v>134</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>2055</v>
+        <v>998</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -9430,10 +9454,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>311</v>
+        <v>135</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1900</v>
+        <v>999</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -9441,10 +9465,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1898</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -9452,10 +9476,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>5</v>
+        <v>2054</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1899</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -9463,10 +9487,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>6</v>
+        <v>311</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -9474,10 +9498,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1901</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -9485,10 +9509,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>312</v>
+        <v>5</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1902</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -9496,10 +9520,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1902</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -9507,10 +9531,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>231</v>
+        <v>7</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>234</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -9518,10 +9542,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>232</v>
+        <v>312</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>245</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -9529,10 +9553,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>233</v>
+        <v>23</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1001</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -9540,10 +9564,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -9551,10 +9575,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1968</v>
+        <v>232</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -9562,10 +9586,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -9573,10 +9597,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1003</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -9584,10 +9608,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>238</v>
+        <v>1968</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -9595,10 +9619,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -9606,10 +9630,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1713</v>
+        <v>237</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1712</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -9617,10 +9641,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1005</v>
+        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -9628,10 +9652,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -9639,10 +9663,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>242</v>
+        <v>1713</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1007</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -9650,10 +9674,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -9661,10 +9685,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -9672,10 +9696,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>216</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -9683,10 +9707,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>246</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -9694,10 +9718,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>215</v>
+        <v>244</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>247</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -9705,10 +9729,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>248</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -9716,10 +9740,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>253</v>
+        <v>214</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -9727,10 +9751,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>300</v>
+        <v>215</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1010</v>
+        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -9738,10 +9762,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>301</v>
+        <v>249</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1011</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -9749,10 +9773,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>302</v>
+        <v>253</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1012</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -9760,10 +9784,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>921</v>
+        <v>300</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>940</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -9771,10 +9795,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>922</v>
+        <v>301</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>939</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -9782,10 +9806,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>923</v>
+        <v>302</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>938</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -9793,10 +9817,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>937</v>
+        <v>940</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -9804,10 +9828,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -9815,10 +9839,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -9826,10 +9850,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -9837,10 +9861,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>931</v>
+        <v>936</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -9848,10 +9872,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -9859,10 +9883,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -9870,10 +9894,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>1999</v>
+        <v>928</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1998</v>
+        <v>931</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -9881,10 +9905,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>2002</v>
+        <v>929</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>2000</v>
+        <v>932</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -9892,26 +9916,44 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="12">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>1999</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="12">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>2002</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="12">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>2027</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>2026</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
@@ -9942,6 +9984,21 @@
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -22524,8 +22581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
System testing and improvement
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A6F37D-8BA6-4619-8E17-3D3F8DD5092D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A60EEB8-9AD2-4CEC-923A-8472120729F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3793" uniqueCount="3598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3793" uniqueCount="3597">
   <si>
     <t>myself</t>
   </si>
@@ -13258,9 +13258,6 @@
   <si>
     <t>生产井段</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Production well sections</t>
   </si>
   <si>
     <t>Production well sections</t>
@@ -13431,7 +13428,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13490,12 +13487,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -13575,7 +13566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -13614,7 +13605,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -15819,7 +15809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D330"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
@@ -20462,8 +20452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
   <dimension ref="A1:D638"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A619" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D638" sqref="D638"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20473,7 +20463,7 @@
     <col min="4" max="4" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="14" t="s">
         <v>1746</v>
       </c>
@@ -20483,8 +20473,8 @@
       <c r="C1" s="14" t="s">
         <v>1748</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>3555</v>
+      <c r="D1" s="14" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -26750,13 +26740,13 @@
         <v>448</v>
       </c>
       <c r="B449" s="5" t="s">
+        <v>3591</v>
+      </c>
+      <c r="C449" s="25" t="s">
         <v>3592</v>
       </c>
-      <c r="C449" s="26" t="s">
+      <c r="D449" s="25" t="s">
         <v>3593</v>
-      </c>
-      <c r="D449" s="26" t="s">
-        <v>3594</v>
       </c>
     </row>
     <row r="450" spans="1:4">
@@ -29129,13 +29119,13 @@
       <c r="A619" s="15">
         <v>618</v>
       </c>
-      <c r="B619" s="25" t="s">
-        <v>3573</v>
+      <c r="B619" s="24" t="s">
+        <v>3572</v>
       </c>
       <c r="C619" s="18" t="s">
         <v>3536</v>
       </c>
-      <c r="D619" s="25" t="s">
+      <c r="D619" s="24" t="s">
         <v>3537</v>
       </c>
     </row>
@@ -29144,7 +29134,7 @@
         <v>619</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
       <c r="C620" s="9" t="s">
         <v>3538</v>
@@ -29228,13 +29218,13 @@
         <v>625</v>
       </c>
       <c r="B626" s="1" t="s">
-        <v>3572</v>
+        <v>3571</v>
       </c>
       <c r="C626" s="1" t="s">
+        <v>3570</v>
+      </c>
+      <c r="D626" s="1" t="s">
         <v>3571</v>
-      </c>
-      <c r="D626" s="1" t="s">
-        <v>3572</v>
       </c>
     </row>
     <row r="627" spans="1:4">
@@ -29242,7 +29232,7 @@
         <v>626</v>
       </c>
       <c r="B627" s="1" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="C627" s="1" t="s">
         <v>3552</v>
@@ -29256,13 +29246,13 @@
         <v>627</v>
       </c>
       <c r="B628" s="1" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
       <c r="C628" s="1" t="s">
         <v>3554</v>
       </c>
       <c r="D628" s="1" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
     </row>
     <row r="629" spans="1:4">
@@ -29270,13 +29260,13 @@
         <v>628</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>3577</v>
+        <v>3576</v>
       </c>
       <c r="C629" s="1" t="s">
+        <v>3556</v>
+      </c>
+      <c r="D629" s="1" t="s">
         <v>3557</v>
-      </c>
-      <c r="D629" s="1" t="s">
-        <v>3558</v>
       </c>
     </row>
     <row r="630" spans="1:4">
@@ -29284,13 +29274,13 @@
         <v>629</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>3578</v>
+        <v>3577</v>
       </c>
       <c r="C630" s="1" t="s">
+        <v>3558</v>
+      </c>
+      <c r="D630" s="1" t="s">
         <v>3559</v>
-      </c>
-      <c r="D630" s="1" t="s">
-        <v>3560</v>
       </c>
     </row>
     <row r="631" spans="1:4">
@@ -29298,13 +29288,13 @@
         <v>630</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>3562</v>
+        <v>3561</v>
       </c>
       <c r="C631" s="18" t="s">
+        <v>3560</v>
+      </c>
+      <c r="D631" s="1" t="s">
         <v>3561</v>
-      </c>
-      <c r="D631" s="1" t="s">
-        <v>3562</v>
       </c>
     </row>
     <row r="632" spans="1:4">
@@ -29312,13 +29302,13 @@
         <v>631</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="C632" s="1" t="s">
+        <v>3562</v>
+      </c>
+      <c r="D632" s="1" t="s">
         <v>3563</v>
-      </c>
-      <c r="D632" s="1" t="s">
-        <v>3564</v>
       </c>
     </row>
     <row r="633" spans="1:4">
@@ -29326,13 +29316,13 @@
         <v>632</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="C633" s="1" t="s">
+        <v>3564</v>
+      </c>
+      <c r="D633" s="1" t="s">
         <v>3565</v>
-      </c>
-      <c r="D633" s="1" t="s">
-        <v>3566</v>
       </c>
     </row>
     <row r="634" spans="1:4">
@@ -29340,13 +29330,13 @@
         <v>633</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
       <c r="C634" s="1" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D634" s="1" t="s">
         <v>3567</v>
-      </c>
-      <c r="D634" s="1" t="s">
-        <v>3568</v>
       </c>
     </row>
     <row r="635" spans="1:4">
@@ -29354,13 +29344,13 @@
         <v>634</v>
       </c>
       <c r="B635" s="1" t="s">
-        <v>3582</v>
+        <v>3581</v>
       </c>
       <c r="C635" s="1" t="s">
+        <v>3568</v>
+      </c>
+      <c r="D635" s="1" t="s">
         <v>3569</v>
-      </c>
-      <c r="D635" s="1" t="s">
-        <v>3570</v>
       </c>
     </row>
     <row r="636" spans="1:4">
@@ -29368,10 +29358,10 @@
         <v>635</v>
       </c>
       <c r="B636" s="5" t="s">
+        <v>3586</v>
+      </c>
+      <c r="C636" s="18" t="s">
         <v>3587</v>
-      </c>
-      <c r="C636" s="18" t="s">
-        <v>3588</v>
       </c>
       <c r="D636" s="9" t="s">
         <v>480</v>
@@ -29382,13 +29372,13 @@
         <v>636</v>
       </c>
       <c r="B637" s="5" t="s">
+        <v>3588</v>
+      </c>
+      <c r="C637" s="18" t="s">
         <v>3589</v>
       </c>
-      <c r="C637" s="18" t="s">
+      <c r="D637" s="9" t="s">
         <v>3590</v>
-      </c>
-      <c r="D637" s="9" t="s">
-        <v>3591</v>
       </c>
     </row>
     <row r="638" spans="1:4">
@@ -29396,13 +29386,13 @@
         <v>637</v>
       </c>
       <c r="B638" s="5" t="s">
+        <v>3594</v>
+      </c>
+      <c r="C638" s="18" t="s">
         <v>3595</v>
       </c>
-      <c r="C638" s="18" t="s">
+      <c r="D638" s="9" t="s">
         <v>3596</v>
-      </c>
-      <c r="D638" s="9" t="s">
-        <v>3597</v>
       </c>
     </row>
   </sheetData>
@@ -30282,13 +30272,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>1517</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
@@ -30302,7 +30292,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>1516</v>
@@ -30322,13 +30312,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>1515</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
       <c r="E45" s="1">
         <v>2</v>
@@ -30342,10 +30332,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>3586</v>
+        <v>3585</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>3227</v>
@@ -30362,7 +30352,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>1698</v>
@@ -30389,7 +30379,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Improvement of additional fields in the agreement
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7518B970-27BE-4418-8C2D-891816A825D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F311AB1-069F-4C73-8923-20A2B80A8798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="3756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4003" uniqueCount="3776">
   <si>
     <t>myself</t>
   </si>
@@ -13206,14 +13206,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>油气生产智能监控系统 V9.6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>《油气生产智能监控系统 V9.6》主要在采集、控制的基础上，侧重油井智能分析。模块主要包括实时监控、历史查询、生产报表、故障查询、日志查询、计算维护、驱动配置、权限管理、设备管理、系统配置等。系统应用大数据分析方法，对工况、产量、液面、平衡、能耗等生产关键指标进行统计分析，及时发现生产不正常井，挖掘生产潜力井，提升对目标区块和单井的管控能力。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Intelligent monitoring system V9.6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -14180,6 +14172,91 @@
   </si>
   <si>
     <t>Dynamometer construction data-ground efficiency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>智能监控系统 V9.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《智能监控系统 V9.6》主要在采集、控制的基础上，侧重油井智能分析。模块主要包括实时监控、历史查询、生产报表、故障查询、日志查询、计算维护、驱动配置、权限管理、设备管理、系统配置等。系统应用大数据分析方法，对工况、产量、液面、平衡、能耗等生产关键指标进行统计分析，及时发现生产不正常井，挖掘生产潜力井，提升对目标区块和单井的管控能力。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拓展字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extended fields</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extendedField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOUROPERATION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>减法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乘法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>除法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subtraction</t>
+  </si>
+  <si>
+    <t>multiplication</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>addition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fourOperation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDITIONALCONDITIONS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非负</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-negative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>additionalConditions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>附加条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Additional conditions</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -16390,7 +16467,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16423,10 +16500,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>3754</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3509</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3511</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -16437,10 +16514,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>3755</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3510</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3512</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -16610,8 +16687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -17566,13 +17643,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>3672</v>
+        <v>3670</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>3667</v>
+        <v>3665</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>3677</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -17580,13 +17657,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>3673</v>
+        <v>3671</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>3668</v>
+        <v>3666</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>3678</v>
+        <v>3676</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -17594,13 +17671,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>3674</v>
+        <v>3672</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>3669</v>
+        <v>3667</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>3679</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -17608,13 +17685,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>3675</v>
+        <v>3673</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>3670</v>
+        <v>3668</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>3680</v>
+        <v>3678</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -17622,13 +17699,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>3676</v>
+        <v>3674</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>3671</v>
+        <v>3669</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>3681</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -19518,7 +19595,7 @@
         <v>1281</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>3516</v>
+        <v>3514</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -19532,7 +19609,7 @@
         <v>1282</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>3517</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -19546,7 +19623,7 @@
         <v>1283</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>3518</v>
+        <v>3516</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -19560,7 +19637,7 @@
         <v>1284</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>3519</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -19574,7 +19651,7 @@
         <v>1285</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>3520</v>
+        <v>3518</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -19588,7 +19665,7 @@
         <v>1286</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>3521</v>
+        <v>3519</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -19602,7 +19679,7 @@
         <v>1287</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>3522</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -19616,7 +19693,7 @@
         <v>1288</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>3523</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -19644,7 +19721,7 @@
         <v>1289</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>3524</v>
+        <v>3522</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -19658,7 +19735,7 @@
         <v>1290</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>3525</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -19756,7 +19833,7 @@
         <v>1846</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>3526</v>
+        <v>3524</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -19770,7 +19847,7 @@
         <v>1847</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>3527</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -19798,7 +19875,7 @@
         <v>1849</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>3528</v>
+        <v>3526</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -19806,13 +19883,13 @@
         <v>227</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>3534</v>
+        <v>3532</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>3529</v>
+        <v>3527</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>3532</v>
+        <v>3530</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -19820,13 +19897,13 @@
         <v>228</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>3535</v>
+        <v>3533</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>3530</v>
+        <v>3528</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>3571</v>
+        <v>3569</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -19834,13 +19911,13 @@
         <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>3533</v>
+        <v>3531</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>3627</v>
+        <v>3625</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>3628</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -19848,13 +19925,13 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>3627</v>
+        <v>3625</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>3628</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -19862,13 +19939,13 @@
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>3537</v>
+        <v>3535</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>3531</v>
+        <v>3529</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>3572</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15" customHeight="1">
@@ -19876,13 +19953,13 @@
         <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>3538</v>
+        <v>3536</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>3569</v>
+        <v>3567</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>3573</v>
+        <v>3571</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -19890,13 +19967,13 @@
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>3540</v>
+        <v>3538</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>3574</v>
+        <v>3572</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>3575</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -19904,13 +19981,13 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>3539</v>
+        <v>3537</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>3576</v>
+        <v>3574</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>3577</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -19918,13 +19995,13 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>3541</v>
+        <v>3539</v>
       </c>
       <c r="C236" s="9" t="s">
-        <v>3578</v>
+        <v>3576</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>3579</v>
+        <v>3577</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -19932,13 +20009,13 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>3542</v>
+        <v>3540</v>
       </c>
       <c r="C237" s="9" t="s">
-        <v>3580</v>
+        <v>3578</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>3581</v>
+        <v>3579</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -19946,13 +20023,13 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>3543</v>
+        <v>3541</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>3582</v>
+        <v>3580</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>3583</v>
+        <v>3581</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -19960,13 +20037,13 @@
         <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>3544</v>
+        <v>3542</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>3584</v>
+        <v>3582</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>3585</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -19974,13 +20051,13 @@
         <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>3545</v>
+        <v>3543</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>3586</v>
+        <v>3584</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>3587</v>
+        <v>3585</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -19988,13 +20065,13 @@
         <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>3546</v>
+        <v>3544</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>3588</v>
+        <v>3586</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>3589</v>
+        <v>3587</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -20002,13 +20079,13 @@
         <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>3547</v>
+        <v>3545</v>
       </c>
       <c r="C242" s="9" t="s">
-        <v>3570</v>
+        <v>3568</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>3590</v>
+        <v>3588</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -20016,13 +20093,13 @@
         <v>242</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>3548</v>
+        <v>3546</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>3591</v>
+        <v>3589</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>3592</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -20030,13 +20107,13 @@
         <v>243</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>3549</v>
+        <v>3547</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>3593</v>
+        <v>3591</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>3594</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -20044,13 +20121,13 @@
         <v>244</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>3550</v>
+        <v>3548</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>3551</v>
+        <v>3549</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>3595</v>
+        <v>3593</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -20058,13 +20135,13 @@
         <v>245</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>3552</v>
+        <v>3550</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>3596</v>
+        <v>3594</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>3597</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -20072,13 +20149,13 @@
         <v>246</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>3553</v>
+        <v>3551</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>3598</v>
+        <v>3596</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>3599</v>
+        <v>3597</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -20086,13 +20163,13 @@
         <v>247</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>3554</v>
+        <v>3552</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>3600</v>
+        <v>3598</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>3601</v>
+        <v>3599</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -20100,13 +20177,13 @@
         <v>248</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>3555</v>
+        <v>3553</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>3602</v>
+        <v>3600</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>3603</v>
+        <v>3601</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -20114,13 +20191,13 @@
         <v>249</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>3556</v>
+        <v>3554</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>3604</v>
+        <v>3602</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>3605</v>
+        <v>3603</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -20128,13 +20205,13 @@
         <v>250</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>3557</v>
+        <v>3555</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>3606</v>
+        <v>3604</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>3607</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -20142,13 +20219,13 @@
         <v>251</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>3558</v>
+        <v>3556</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>3608</v>
+        <v>3606</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>3609</v>
+        <v>3607</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -20156,13 +20233,13 @@
         <v>252</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>3559</v>
+        <v>3557</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>3610</v>
+        <v>3608</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>3611</v>
+        <v>3609</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -20170,13 +20247,13 @@
         <v>253</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>3560</v>
+        <v>3558</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>3612</v>
+        <v>3610</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>3613</v>
+        <v>3611</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -20184,13 +20261,13 @@
         <v>254</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>3561</v>
+        <v>3559</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>3614</v>
+        <v>3612</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>3615</v>
+        <v>3613</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -20198,13 +20275,13 @@
         <v>255</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>3562</v>
+        <v>3560</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>3563</v>
+        <v>3561</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>3616</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -20212,13 +20289,13 @@
         <v>256</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>3564</v>
+        <v>3562</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>3617</v>
+        <v>3615</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>3618</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -20226,13 +20303,13 @@
         <v>257</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>3565</v>
+        <v>3563</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>3619</v>
+        <v>3617</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>3620</v>
+        <v>3618</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -20240,13 +20317,13 @@
         <v>258</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>3566</v>
+        <v>3564</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>3621</v>
+        <v>3619</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>3622</v>
+        <v>3620</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -20254,13 +20331,13 @@
         <v>259</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>3567</v>
+        <v>3565</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>3623</v>
+        <v>3621</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>3624</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -20268,13 +20345,13 @@
         <v>260</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>3568</v>
+        <v>3566</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>3625</v>
+        <v>3623</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>3626</v>
+        <v>3624</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -20288,7 +20365,7 @@
         <v>2486</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>3657</v>
+        <v>3655</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -20316,7 +20393,7 @@
         <v>2487</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>3658</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -20330,7 +20407,7 @@
         <v>2488</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>3659</v>
+        <v>3657</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -20400,7 +20477,7 @@
         <v>2489</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>3660</v>
+        <v>3658</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -20428,7 +20505,7 @@
         <v>2491</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>3661</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -20442,7 +20519,7 @@
         <v>2492</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>3662</v>
+        <v>3660</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -20456,7 +20533,7 @@
         <v>2493</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>3663</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -20470,7 +20547,7 @@
         <v>2494</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>3664</v>
+        <v>3662</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -20512,7 +20589,7 @@
         <v>2495</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>3665</v>
+        <v>3663</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -20526,7 +20603,7 @@
         <v>2496</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>3666</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -20554,7 +20631,7 @@
         <v>2497</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>3682</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -20568,7 +20645,7 @@
         <v>2498</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>3683</v>
+        <v>3681</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -20582,7 +20659,7 @@
         <v>2499</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>3684</v>
+        <v>3682</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -20596,7 +20673,7 @@
         <v>2563</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>3685</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -20610,7 +20687,7 @@
         <v>2564</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>3686</v>
+        <v>3684</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -20624,7 +20701,7 @@
         <v>2565</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>3687</v>
+        <v>3685</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -20638,7 +20715,7 @@
         <v>2566</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>3688</v>
+        <v>3686</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -20652,7 +20729,7 @@
         <v>2567</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>3689</v>
+        <v>3687</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -20666,7 +20743,7 @@
         <v>2568</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>3690</v>
+        <v>3688</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -20680,7 +20757,7 @@
         <v>2569</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>3691</v>
+        <v>3689</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -20694,7 +20771,7 @@
         <v>2570</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>3692</v>
+        <v>3690</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -20708,7 +20785,7 @@
         <v>2571</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>3693</v>
+        <v>3691</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -20722,7 +20799,7 @@
         <v>2572</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>3694</v>
+        <v>3692</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -20736,7 +20813,7 @@
         <v>2573</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>3695</v>
+        <v>3693</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -20750,7 +20827,7 @@
         <v>2574</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>3696</v>
+        <v>3694</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -20764,7 +20841,7 @@
         <v>2575</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>3697</v>
+        <v>3695</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -20778,7 +20855,7 @@
         <v>2576</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>3698</v>
+        <v>3696</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -20792,7 +20869,7 @@
         <v>2577</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>3699</v>
+        <v>3697</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -20806,7 +20883,7 @@
         <v>2578</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>3700</v>
+        <v>3698</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -20820,7 +20897,7 @@
         <v>2579</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>3701</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -20834,7 +20911,7 @@
         <v>2580</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>3702</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -20848,7 +20925,7 @@
         <v>2581</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>3703</v>
+        <v>3701</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -20862,7 +20939,7 @@
         <v>2582</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>3704</v>
+        <v>3702</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -20890,7 +20967,7 @@
         <v>2500</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>3705</v>
+        <v>3703</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -20904,7 +20981,7 @@
         <v>2501</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>3706</v>
+        <v>3704</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -20918,7 +20995,7 @@
         <v>2502</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>3707</v>
+        <v>3705</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -20932,7 +21009,7 @@
         <v>2503</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>3708</v>
+        <v>3706</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -20946,7 +21023,7 @@
         <v>2504</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>3709</v>
+        <v>3707</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -20960,7 +21037,7 @@
         <v>2505</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>3710</v>
+        <v>3708</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -20974,7 +21051,7 @@
         <v>2506</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>3711</v>
+        <v>3709</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -20988,7 +21065,7 @@
         <v>2507</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>3712</v>
+        <v>3710</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -21002,7 +21079,7 @@
         <v>2508</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>3713</v>
+        <v>3711</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -21016,7 +21093,7 @@
         <v>2509</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>3714</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -21030,7 +21107,7 @@
         <v>2510</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>3715</v>
+        <v>3713</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -21044,7 +21121,7 @@
         <v>2511</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>3716</v>
+        <v>3714</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -21156,7 +21233,7 @@
         <v>2519</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>3717</v>
+        <v>3715</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -21268,7 +21345,7 @@
         <v>2527</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>3718</v>
+        <v>3716</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -21282,7 +21359,7 @@
         <v>2528</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>3719</v>
+        <v>3717</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -21296,7 +21373,7 @@
         <v>2529</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>3720</v>
+        <v>3718</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -21310,7 +21387,7 @@
         <v>2530</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>3721</v>
+        <v>3719</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -21324,7 +21401,7 @@
         <v>2531</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>3722</v>
+        <v>3720</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -21335,10 +21412,10 @@
         <v>2104</v>
       </c>
       <c r="C337" s="22" t="s">
-        <v>3723</v>
+        <v>3721</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>3735</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -21349,10 +21426,10 @@
         <v>2105</v>
       </c>
       <c r="C338" s="22" t="s">
-        <v>3736</v>
+        <v>3734</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>3737</v>
+        <v>3735</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -21363,10 +21440,10 @@
         <v>2106</v>
       </c>
       <c r="C339" s="22" t="s">
-        <v>3754</v>
+        <v>3752</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>3755</v>
+        <v>3753</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -21377,10 +21454,10 @@
         <v>2107</v>
       </c>
       <c r="C340" s="22" t="s">
-        <v>3724</v>
+        <v>3722</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>3738</v>
+        <v>3736</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -21391,10 +21468,10 @@
         <v>2118</v>
       </c>
       <c r="C341" s="22" t="s">
-        <v>3725</v>
+        <v>3723</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>3739</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -21405,10 +21482,10 @@
         <v>2108</v>
       </c>
       <c r="C342" s="22" t="s">
-        <v>3730</v>
+        <v>3728</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>3740</v>
+        <v>3738</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -21419,10 +21496,10 @@
         <v>2109</v>
       </c>
       <c r="C343" s="22" t="s">
-        <v>3731</v>
+        <v>3729</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>3741</v>
+        <v>3739</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -21433,10 +21510,10 @@
         <v>2110</v>
       </c>
       <c r="C344" s="22" t="s">
-        <v>3732</v>
+        <v>3730</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>3742</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -21447,10 +21524,10 @@
         <v>2111</v>
       </c>
       <c r="C345" s="22" t="s">
-        <v>3733</v>
+        <v>3731</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>3743</v>
+        <v>3741</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -21461,10 +21538,10 @@
         <v>2112</v>
       </c>
       <c r="C346" s="22" t="s">
-        <v>3734</v>
+        <v>3732</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>3744</v>
+        <v>3742</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -21475,10 +21552,10 @@
         <v>2124</v>
       </c>
       <c r="C347" s="22" t="s">
-        <v>3726</v>
+        <v>3724</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>3745</v>
+        <v>3743</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -21489,10 +21566,10 @@
         <v>2125</v>
       </c>
       <c r="C348" s="22" t="s">
-        <v>3727</v>
+        <v>3725</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>3746</v>
+        <v>3744</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -21503,10 +21580,10 @@
         <v>2113</v>
       </c>
       <c r="C349" s="22" t="s">
-        <v>3728</v>
+        <v>3726</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>3747</v>
+        <v>3745</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -21517,10 +21594,10 @@
         <v>2171</v>
       </c>
       <c r="C350" s="22" t="s">
-        <v>3729</v>
+        <v>3727</v>
       </c>
       <c r="D350" s="22" t="s">
-        <v>3750</v>
+        <v>3748</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -21534,7 +21611,7 @@
         <v>2181</v>
       </c>
       <c r="D351" s="22" t="s">
-        <v>3514</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -21548,7 +21625,7 @@
         <v>2183</v>
       </c>
       <c r="D352" s="22" t="s">
-        <v>3515</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -21730,7 +21807,7 @@
         <v>2175</v>
       </c>
       <c r="D365" s="22" t="s">
-        <v>3751</v>
+        <v>3749</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -21744,7 +21821,7 @@
         <v>2177</v>
       </c>
       <c r="D366" s="22" t="s">
-        <v>3752</v>
+        <v>3750</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -21758,7 +21835,7 @@
         <v>2179</v>
       </c>
       <c r="D367" s="22" t="s">
-        <v>3753</v>
+        <v>3751</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -21786,7 +21863,7 @@
         <v>2188</v>
       </c>
       <c r="D369" s="9" t="s">
-        <v>3748</v>
+        <v>3746</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -21800,7 +21877,7 @@
         <v>2190</v>
       </c>
       <c r="D370" s="9" t="s">
-        <v>3749</v>
+        <v>3747</v>
       </c>
     </row>
   </sheetData>
@@ -21812,10 +21889,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D652"/>
+  <dimension ref="A1:D655"/>
   <sheetViews>
-    <sheetView topLeftCell="A566" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D585" sqref="D585"/>
+    <sheetView tabSelected="1" topLeftCell="A643" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B661" sqref="B661"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -25868,7 +25945,7 @@
         <v>1474</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>3513</v>
+        <v>3511</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -30951,6 +31028,48 @@
       </c>
       <c r="D652" s="9" t="s">
         <v>3454</v>
+      </c>
+    </row>
+    <row r="653" spans="1:4">
+      <c r="A653" s="15">
+        <v>652</v>
+      </c>
+      <c r="B653" s="5" t="s">
+        <v>3758</v>
+      </c>
+      <c r="C653" s="18" t="s">
+        <v>3756</v>
+      </c>
+      <c r="D653" s="9" t="s">
+        <v>3757</v>
+      </c>
+    </row>
+    <row r="654" spans="1:4">
+      <c r="A654" s="15">
+        <v>653</v>
+      </c>
+      <c r="B654" s="5" t="s">
+        <v>3769</v>
+      </c>
+      <c r="C654" s="18" t="s">
+        <v>3768</v>
+      </c>
+      <c r="D654" s="9" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4">
+      <c r="A655" s="15">
+        <v>654</v>
+      </c>
+      <c r="B655" s="5" t="s">
+        <v>3773</v>
+      </c>
+      <c r="C655" s="18" t="s">
+        <v>3774</v>
+      </c>
+      <c r="D655" s="9" t="s">
+        <v>3775</v>
       </c>
     </row>
   </sheetData>
@@ -30962,10 +31081,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -31930,17 +32049,17 @@
       <c r="A48" s="15">
         <v>47</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>3485</v>
+      <c r="B48" s="4" t="s">
+        <v>3440</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>3486</v>
+        <v>3756</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>3488</v>
+        <v>3757</v>
       </c>
       <c r="E48" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -31954,13 +32073,13 @@
         <v>3485</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>3487</v>
+        <v>3486</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>3190</v>
+        <v>3488</v>
       </c>
       <c r="E49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -31974,17 +32093,157 @@
         <v>3485</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>1300</v>
+        <v>3487</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>826</v>
+        <v>3190</v>
       </c>
       <c r="E50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="15">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>3485</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="E51" s="1">
+        <v>2</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="15">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>3759</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>3760</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>3767</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="15">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>3759</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>3761</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>3764</v>
+      </c>
+      <c r="E53" s="1">
+        <v>2</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="15">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3759</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>3765</v>
+      </c>
+      <c r="E54" s="1">
+        <v>3</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="15">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>3759</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>3766</v>
+      </c>
+      <c r="E55" s="1">
+        <v>4</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="15">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>3770</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>2712</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="15">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>3770</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>3771</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>3772</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -32058,7 +32317,7 @@
         <v>1838</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3629</v>
+        <v>3627</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>1887</v>
@@ -32110,7 +32369,7 @@
         <v>1819</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>3630</v>
+        <v>3628</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>1889</v>
@@ -32136,7 +32395,7 @@
         <v>1820</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3631</v>
+        <v>3629</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>1890</v>
@@ -32164,7 +32423,7 @@
         <v>1821</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3632</v>
+        <v>3630</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1891</v>
@@ -32192,7 +32451,7 @@
         <v>1839</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>3633</v>
+        <v>3631</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>1892</v>
@@ -32220,7 +32479,7 @@
         <v>1822</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>3634</v>
+        <v>3632</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>1893</v>
@@ -32248,7 +32507,7 @@
         <v>1823</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>3635</v>
+        <v>3633</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>1894</v>
@@ -32304,7 +32563,7 @@
         <v>1824</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>3636</v>
+        <v>3634</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>1896</v>
@@ -32332,7 +32591,7 @@
         <v>1825</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>3637</v>
+        <v>3635</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>1897</v>
@@ -32360,7 +32619,7 @@
         <v>1826</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>3638</v>
+        <v>3636</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>1898</v>
@@ -32388,7 +32647,7 @@
         <v>1827</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>3639</v>
+        <v>3637</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>1899</v>
@@ -32416,7 +32675,7 @@
         <v>1828</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>3640</v>
+        <v>3638</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>1900</v>
@@ -32444,7 +32703,7 @@
         <v>1829</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>3641</v>
+        <v>3639</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>1901</v>
@@ -32472,7 +32731,7 @@
         <v>1830</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>3642</v>
+        <v>3640</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>1902</v>
@@ -32500,7 +32759,7 @@
         <v>1831</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>3643</v>
+        <v>3641</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>1903</v>
@@ -32528,7 +32787,7 @@
         <v>1841</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>3644</v>
+        <v>3642</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>1904</v>
@@ -32556,7 +32815,7 @@
         <v>1832</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>3645</v>
+        <v>3643</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>1905</v>
@@ -32584,7 +32843,7 @@
         <v>1842</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>3646</v>
+        <v>3644</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>1901</v>
@@ -32612,7 +32871,7 @@
         <v>1833</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>3647</v>
+        <v>3645</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>1906</v>
@@ -32640,7 +32899,7 @@
         <v>1834</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>3648</v>
+        <v>3646</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>1907</v>
@@ -32668,7 +32927,7 @@
         <v>1844</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>3649</v>
+        <v>3647</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>1908</v>
@@ -32696,7 +32955,7 @@
         <v>1995</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>3650</v>
+        <v>3648</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>1909</v>
@@ -32724,7 +32983,7 @@
         <v>1994</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>3651</v>
+        <v>3649</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="1"/>
@@ -32748,7 +33007,7 @@
         <v>1992</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>3652</v>
+        <v>3650</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>1910</v>
@@ -32776,7 +33035,7 @@
         <v>1993</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>3653</v>
+        <v>3651</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="1"/>
@@ -32800,7 +33059,7 @@
         <v>1835</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>3654</v>
+        <v>3652</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>1911</v>
@@ -32828,7 +33087,7 @@
         <v>1836</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>3655</v>
+        <v>3653</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="1"/>
@@ -32852,7 +33111,7 @@
         <v>1837</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>3656</v>
+        <v>3654</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="1"/>

</xml_diff>

<commit_message>
The dictionary module has been improved.
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD8B17C-2FC5-46A7-991C-162B47681084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF0ED35-F818-4E9B-BF60-668963994AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4006" uniqueCount="3779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4009" uniqueCount="3782">
   <si>
     <t>myself</t>
   </si>
@@ -13107,17 +13107,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>基础字段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>驱动配置</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Base fields</t>
-  </si>
-  <si>
     <t>字段来源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -14269,6 +14262,26 @@
   </si>
   <si>
     <t>Double-click the cell to configure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Configure field</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>configureField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>固定字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed fields</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -16211,13 +16224,13 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>3498</v>
+        <v>3496</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>3499</v>
+        <v>3497</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>3504</v>
+        <v>3502</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -16225,13 +16238,13 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>3500</v>
+        <v>3498</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>3501</v>
+        <v>3499</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>3505</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -16239,13 +16252,13 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>3502</v>
+        <v>3500</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>3503</v>
+        <v>3501</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>3506</v>
+        <v>3504</v>
       </c>
     </row>
   </sheetData>
@@ -16512,10 +16525,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>3752</v>
+        <v>3750</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3507</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -16526,10 +16539,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>3753</v>
+        <v>3751</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3508</v>
+        <v>3506</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -17655,13 +17668,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>3668</v>
+        <v>3666</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>3663</v>
+        <v>3661</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>3673</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -17669,13 +17682,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>3669</v>
+        <v>3667</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>3664</v>
+        <v>3662</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>3674</v>
+        <v>3672</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -17683,13 +17696,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>3670</v>
+        <v>3668</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>3665</v>
+        <v>3663</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>3675</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -17697,13 +17710,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>3671</v>
+        <v>3669</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>3666</v>
+        <v>3664</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>3676</v>
+        <v>3674</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -17711,13 +17724,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>3672</v>
+        <v>3670</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>3667</v>
+        <v>3665</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>3677</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -19607,7 +19620,7 @@
         <v>1280</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>3512</v>
+        <v>3510</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -19621,7 +19634,7 @@
         <v>1281</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>3513</v>
+        <v>3511</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -19635,7 +19648,7 @@
         <v>1282</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>3514</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -19649,7 +19662,7 @@
         <v>1283</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>3515</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -19663,7 +19676,7 @@
         <v>1284</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>3516</v>
+        <v>3514</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -19677,7 +19690,7 @@
         <v>1285</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>3517</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -19691,7 +19704,7 @@
         <v>1286</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>3518</v>
+        <v>3516</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -19705,7 +19718,7 @@
         <v>1287</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>3519</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -19733,7 +19746,7 @@
         <v>1288</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>3520</v>
+        <v>3518</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -19747,7 +19760,7 @@
         <v>1289</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>3521</v>
+        <v>3519</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -19845,7 +19858,7 @@
         <v>1844</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>3522</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -19859,7 +19872,7 @@
         <v>1845</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>3523</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -19887,7 +19900,7 @@
         <v>1847</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>3524</v>
+        <v>3522</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -19895,13 +19908,13 @@
         <v>227</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>3530</v>
+        <v>3528</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>3525</v>
+        <v>3523</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>3528</v>
+        <v>3526</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -19909,13 +19922,13 @@
         <v>228</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>3531</v>
+        <v>3529</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>3526</v>
+        <v>3524</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>3567</v>
+        <v>3565</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -19923,13 +19936,13 @@
         <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>3529</v>
+        <v>3527</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>3623</v>
+        <v>3621</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>3624</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -19937,13 +19950,13 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>3532</v>
+        <v>3530</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>3623</v>
+        <v>3621</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>3624</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -19951,13 +19964,13 @@
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>3533</v>
+        <v>3531</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>3527</v>
+        <v>3525</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>3568</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15" customHeight="1">
@@ -19965,13 +19978,13 @@
         <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>3534</v>
+        <v>3532</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>3565</v>
+        <v>3563</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>3569</v>
+        <v>3567</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -19979,13 +19992,13 @@
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>3570</v>
+        <v>3568</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>3571</v>
+        <v>3569</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -19993,13 +20006,13 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>3535</v>
+        <v>3533</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>3572</v>
+        <v>3570</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>3573</v>
+        <v>3571</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -20007,13 +20020,13 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>3537</v>
+        <v>3535</v>
       </c>
       <c r="C236" s="9" t="s">
-        <v>3574</v>
+        <v>3572</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>3575</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -20021,13 +20034,13 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>3538</v>
+        <v>3536</v>
       </c>
       <c r="C237" s="9" t="s">
-        <v>3576</v>
+        <v>3574</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>3577</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -20035,13 +20048,13 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>3539</v>
+        <v>3537</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>3578</v>
+        <v>3576</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>3579</v>
+        <v>3577</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -20049,13 +20062,13 @@
         <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>3540</v>
+        <v>3538</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>3580</v>
+        <v>3578</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>3581</v>
+        <v>3579</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -20063,13 +20076,13 @@
         <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>3541</v>
+        <v>3539</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>3582</v>
+        <v>3580</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>3583</v>
+        <v>3581</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -20077,13 +20090,13 @@
         <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>3542</v>
+        <v>3540</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>3584</v>
+        <v>3582</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>3585</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -20091,13 +20104,13 @@
         <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>3543</v>
+        <v>3541</v>
       </c>
       <c r="C242" s="9" t="s">
-        <v>3566</v>
+        <v>3564</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>3586</v>
+        <v>3584</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -20105,13 +20118,13 @@
         <v>242</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>3544</v>
+        <v>3542</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>3587</v>
+        <v>3585</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>3588</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -20119,13 +20132,13 @@
         <v>243</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>3545</v>
+        <v>3543</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>3589</v>
+        <v>3587</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>3590</v>
+        <v>3588</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -20133,13 +20146,13 @@
         <v>244</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>3546</v>
+        <v>3544</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>3547</v>
+        <v>3545</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>3591</v>
+        <v>3589</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -20147,13 +20160,13 @@
         <v>245</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>3548</v>
+        <v>3546</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>3592</v>
+        <v>3590</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>3593</v>
+        <v>3591</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -20161,13 +20174,13 @@
         <v>246</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>3549</v>
+        <v>3547</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>3594</v>
+        <v>3592</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>3595</v>
+        <v>3593</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -20175,13 +20188,13 @@
         <v>247</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>3550</v>
+        <v>3548</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>3596</v>
+        <v>3594</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>3597</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -20189,13 +20202,13 @@
         <v>248</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>3551</v>
+        <v>3549</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>3598</v>
+        <v>3596</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>3599</v>
+        <v>3597</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -20203,13 +20216,13 @@
         <v>249</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>3552</v>
+        <v>3550</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>3600</v>
+        <v>3598</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>3601</v>
+        <v>3599</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -20217,13 +20230,13 @@
         <v>250</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>3553</v>
+        <v>3551</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>3602</v>
+        <v>3600</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>3603</v>
+        <v>3601</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -20231,13 +20244,13 @@
         <v>251</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>3554</v>
+        <v>3552</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>3604</v>
+        <v>3602</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>3605</v>
+        <v>3603</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -20245,13 +20258,13 @@
         <v>252</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>3555</v>
+        <v>3553</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>3606</v>
+        <v>3604</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>3607</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -20259,13 +20272,13 @@
         <v>253</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>3556</v>
+        <v>3554</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>3608</v>
+        <v>3606</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>3609</v>
+        <v>3607</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -20273,13 +20286,13 @@
         <v>254</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>3557</v>
+        <v>3555</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>3610</v>
+        <v>3608</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>3611</v>
+        <v>3609</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -20287,13 +20300,13 @@
         <v>255</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>3558</v>
+        <v>3556</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>3559</v>
+        <v>3557</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>3612</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -20301,13 +20314,13 @@
         <v>256</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>3560</v>
+        <v>3558</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>3613</v>
+        <v>3611</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>3614</v>
+        <v>3612</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -20315,13 +20328,13 @@
         <v>257</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>3561</v>
+        <v>3559</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>3615</v>
+        <v>3613</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>3616</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -20329,13 +20342,13 @@
         <v>258</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>3562</v>
+        <v>3560</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>3617</v>
+        <v>3615</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>3618</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -20343,13 +20356,13 @@
         <v>259</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>3563</v>
+        <v>3561</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>3619</v>
+        <v>3617</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>3620</v>
+        <v>3618</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -20357,13 +20370,13 @@
         <v>260</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>3564</v>
+        <v>3562</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>3621</v>
+        <v>3619</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>3622</v>
+        <v>3620</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -20377,7 +20390,7 @@
         <v>2484</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>3653</v>
+        <v>3651</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -20405,7 +20418,7 @@
         <v>2485</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>3654</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -20419,7 +20432,7 @@
         <v>2486</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>3655</v>
+        <v>3653</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -20489,7 +20502,7 @@
         <v>2487</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>3656</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -20517,7 +20530,7 @@
         <v>2489</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>3657</v>
+        <v>3655</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -20531,7 +20544,7 @@
         <v>2490</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>3658</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -20545,7 +20558,7 @@
         <v>2491</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>3659</v>
+        <v>3657</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -20559,7 +20572,7 @@
         <v>2492</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>3660</v>
+        <v>3658</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -20601,7 +20614,7 @@
         <v>2493</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>3661</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -20615,7 +20628,7 @@
         <v>2494</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>3662</v>
+        <v>3660</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -20643,7 +20656,7 @@
         <v>2495</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>3678</v>
+        <v>3676</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -20657,7 +20670,7 @@
         <v>2496</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>3679</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -20671,7 +20684,7 @@
         <v>2497</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>3680</v>
+        <v>3678</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -20685,7 +20698,7 @@
         <v>2561</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>3681</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -20699,7 +20712,7 @@
         <v>2562</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>3682</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -20713,7 +20726,7 @@
         <v>2563</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>3683</v>
+        <v>3681</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -20727,7 +20740,7 @@
         <v>2564</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>3684</v>
+        <v>3682</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -20741,7 +20754,7 @@
         <v>2565</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>3685</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -20755,7 +20768,7 @@
         <v>2566</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>3686</v>
+        <v>3684</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -20769,7 +20782,7 @@
         <v>2567</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>3687</v>
+        <v>3685</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -20783,7 +20796,7 @@
         <v>2568</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>3688</v>
+        <v>3686</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -20797,7 +20810,7 @@
         <v>2569</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>3689</v>
+        <v>3687</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -20811,7 +20824,7 @@
         <v>2570</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>3690</v>
+        <v>3688</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -20825,7 +20838,7 @@
         <v>2571</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>3691</v>
+        <v>3689</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -20839,7 +20852,7 @@
         <v>2572</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>3692</v>
+        <v>3690</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -20853,7 +20866,7 @@
         <v>2573</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>3693</v>
+        <v>3691</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -20867,7 +20880,7 @@
         <v>2574</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>3694</v>
+        <v>3692</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -20881,7 +20894,7 @@
         <v>2575</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>3695</v>
+        <v>3693</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -20895,7 +20908,7 @@
         <v>2576</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>3696</v>
+        <v>3694</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -20909,7 +20922,7 @@
         <v>2577</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>3697</v>
+        <v>3695</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -20923,7 +20936,7 @@
         <v>2578</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>3698</v>
+        <v>3696</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -20937,7 +20950,7 @@
         <v>2579</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>3699</v>
+        <v>3697</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -20951,7 +20964,7 @@
         <v>2580</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>3700</v>
+        <v>3698</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -20979,7 +20992,7 @@
         <v>2498</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>3701</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -20993,7 +21006,7 @@
         <v>2499</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>3702</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -21007,7 +21020,7 @@
         <v>2500</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>3703</v>
+        <v>3701</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -21021,7 +21034,7 @@
         <v>2501</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>3704</v>
+        <v>3702</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -21035,7 +21048,7 @@
         <v>2502</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>3705</v>
+        <v>3703</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -21049,7 +21062,7 @@
         <v>2503</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>3706</v>
+        <v>3704</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -21063,7 +21076,7 @@
         <v>2504</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>3707</v>
+        <v>3705</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -21077,7 +21090,7 @@
         <v>2505</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>3708</v>
+        <v>3706</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -21091,7 +21104,7 @@
         <v>2506</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>3709</v>
+        <v>3707</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -21105,7 +21118,7 @@
         <v>2507</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>3710</v>
+        <v>3708</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -21119,7 +21132,7 @@
         <v>2508</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>3711</v>
+        <v>3709</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -21133,7 +21146,7 @@
         <v>2509</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>3712</v>
+        <v>3710</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -21245,7 +21258,7 @@
         <v>2517</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>3713</v>
+        <v>3711</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -21357,7 +21370,7 @@
         <v>2525</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>3714</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -21371,7 +21384,7 @@
         <v>2526</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>3715</v>
+        <v>3713</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -21385,7 +21398,7 @@
         <v>2527</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>3716</v>
+        <v>3714</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -21399,7 +21412,7 @@
         <v>2528</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>3717</v>
+        <v>3715</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -21413,7 +21426,7 @@
         <v>2529</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>3718</v>
+        <v>3716</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -21424,10 +21437,10 @@
         <v>2102</v>
       </c>
       <c r="C337" s="22" t="s">
-        <v>3719</v>
+        <v>3717</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>3731</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -21438,10 +21451,10 @@
         <v>2103</v>
       </c>
       <c r="C338" s="22" t="s">
-        <v>3732</v>
+        <v>3730</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>3733</v>
+        <v>3731</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -21452,10 +21465,10 @@
         <v>2104</v>
       </c>
       <c r="C339" s="22" t="s">
-        <v>3750</v>
+        <v>3748</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>3751</v>
+        <v>3749</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -21466,10 +21479,10 @@
         <v>2105</v>
       </c>
       <c r="C340" s="22" t="s">
-        <v>3720</v>
+        <v>3718</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>3734</v>
+        <v>3732</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -21480,10 +21493,10 @@
         <v>2116</v>
       </c>
       <c r="C341" s="22" t="s">
-        <v>3721</v>
+        <v>3719</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>3735</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -21494,10 +21507,10 @@
         <v>2106</v>
       </c>
       <c r="C342" s="22" t="s">
-        <v>3726</v>
+        <v>3724</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>3736</v>
+        <v>3734</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -21508,10 +21521,10 @@
         <v>2107</v>
       </c>
       <c r="C343" s="22" t="s">
-        <v>3727</v>
+        <v>3725</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>3737</v>
+        <v>3735</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -21522,10 +21535,10 @@
         <v>2108</v>
       </c>
       <c r="C344" s="22" t="s">
-        <v>3728</v>
+        <v>3726</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>3738</v>
+        <v>3736</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -21536,10 +21549,10 @@
         <v>2109</v>
       </c>
       <c r="C345" s="22" t="s">
-        <v>3729</v>
+        <v>3727</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>3739</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -21550,10 +21563,10 @@
         <v>2110</v>
       </c>
       <c r="C346" s="22" t="s">
-        <v>3730</v>
+        <v>3728</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>3740</v>
+        <v>3738</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -21564,10 +21577,10 @@
         <v>2122</v>
       </c>
       <c r="C347" s="22" t="s">
-        <v>3722</v>
+        <v>3720</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>3741</v>
+        <v>3739</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -21578,10 +21591,10 @@
         <v>2123</v>
       </c>
       <c r="C348" s="22" t="s">
-        <v>3723</v>
+        <v>3721</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>3742</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -21592,10 +21605,10 @@
         <v>2111</v>
       </c>
       <c r="C349" s="22" t="s">
-        <v>3724</v>
+        <v>3722</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>3743</v>
+        <v>3741</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -21606,10 +21619,10 @@
         <v>2169</v>
       </c>
       <c r="C350" s="22" t="s">
-        <v>3725</v>
+        <v>3723</v>
       </c>
       <c r="D350" s="22" t="s">
-        <v>3746</v>
+        <v>3744</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -21623,7 +21636,7 @@
         <v>2179</v>
       </c>
       <c r="D351" s="22" t="s">
-        <v>3510</v>
+        <v>3508</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -21637,7 +21650,7 @@
         <v>2181</v>
       </c>
       <c r="D352" s="22" t="s">
-        <v>3511</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -21819,7 +21832,7 @@
         <v>2173</v>
       </c>
       <c r="D365" s="22" t="s">
-        <v>3747</v>
+        <v>3745</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -21833,7 +21846,7 @@
         <v>2175</v>
       </c>
       <c r="D366" s="22" t="s">
-        <v>3748</v>
+        <v>3746</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -21847,7 +21860,7 @@
         <v>2177</v>
       </c>
       <c r="D367" s="22" t="s">
-        <v>3749</v>
+        <v>3747</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -21875,7 +21888,7 @@
         <v>2186</v>
       </c>
       <c r="D369" s="9" t="s">
-        <v>3744</v>
+        <v>3742</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -21889,7 +21902,7 @@
         <v>2188</v>
       </c>
       <c r="D370" s="9" t="s">
-        <v>3745</v>
+        <v>3743</v>
       </c>
     </row>
   </sheetData>
@@ -21901,10 +21914,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D656"/>
+  <dimension ref="A1:D657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A638" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C661" sqref="C661"/>
+    <sheetView topLeftCell="A638" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B661" sqref="B661"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -22636,10 +22649,10 @@
         <v>1041</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>3774</v>
+        <v>3772</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>3774</v>
+        <v>3772</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -22720,7 +22733,7 @@
         <v>1063</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>3775</v>
+        <v>3773</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>2626</v>
@@ -23893,7 +23906,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>3490</v>
+        <v>3488</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>3235</v>
@@ -23907,7 +23920,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>3491</v>
+        <v>3489</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>3237</v>
@@ -23921,7 +23934,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>3492</v>
+        <v>3490</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>736</v>
@@ -23935,10 +23948,10 @@
         <v>144</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>3493</v>
+        <v>3491</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>3494</v>
+        <v>3492</v>
       </c>
       <c r="D145" s="9" t="s">
         <v>3288</v>
@@ -25957,7 +25970,7 @@
         <v>1472</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>3509</v>
+        <v>3507</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -27939,13 +27952,13 @@
         <v>430</v>
       </c>
       <c r="B431" s="5" t="s">
+        <v>3493</v>
+      </c>
+      <c r="C431" s="9" t="s">
+        <v>3494</v>
+      </c>
+      <c r="D431" s="1" t="s">
         <v>3495</v>
-      </c>
-      <c r="C431" s="9" t="s">
-        <v>3496</v>
-      </c>
-      <c r="D431" s="1" t="s">
-        <v>3497</v>
       </c>
     </row>
     <row r="432" spans="1:4">
@@ -29759,13 +29772,13 @@
         <v>560</v>
       </c>
       <c r="B561" s="5" t="s">
-        <v>3489</v>
+        <v>3487</v>
       </c>
       <c r="C561" s="18" t="s">
-        <v>3487</v>
+        <v>3485</v>
       </c>
       <c r="D561" s="9" t="s">
-        <v>3488</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="562" spans="1:4">
@@ -31047,13 +31060,13 @@
         <v>652</v>
       </c>
       <c r="B653" s="5" t="s">
-        <v>3756</v>
+        <v>3754</v>
       </c>
       <c r="C653" s="18" t="s">
-        <v>3754</v>
+        <v>3752</v>
       </c>
       <c r="D653" s="9" t="s">
-        <v>3755</v>
+        <v>3753</v>
       </c>
     </row>
     <row r="654" spans="1:4">
@@ -31061,10 +31074,10 @@
         <v>653</v>
       </c>
       <c r="B654" s="5" t="s">
-        <v>3767</v>
+        <v>3765</v>
       </c>
       <c r="C654" s="18" t="s">
-        <v>3766</v>
+        <v>3764</v>
       </c>
       <c r="D654" s="9" t="s">
         <v>851</v>
@@ -31075,13 +31088,13 @@
         <v>654</v>
       </c>
       <c r="B655" s="5" t="s">
+        <v>3769</v>
+      </c>
+      <c r="C655" s="18" t="s">
+        <v>3770</v>
+      </c>
+      <c r="D655" s="9" t="s">
         <v>3771</v>
-      </c>
-      <c r="C655" s="18" t="s">
-        <v>3772</v>
-      </c>
-      <c r="D655" s="9" t="s">
-        <v>3773</v>
       </c>
     </row>
     <row r="656" spans="1:4">
@@ -31089,12 +31102,26 @@
         <v>655</v>
       </c>
       <c r="B656" s="5" t="s">
+        <v>3774</v>
+      </c>
+      <c r="C656" s="18" t="s">
+        <v>3775</v>
+      </c>
+      <c r="D656" s="9" t="s">
         <v>3776</v>
       </c>
-      <c r="C656" s="18" t="s">
+    </row>
+    <row r="657" spans="1:4">
+      <c r="A657" s="15">
+        <v>656</v>
+      </c>
+      <c r="B657" s="5" t="s">
+        <v>3779</v>
+      </c>
+      <c r="C657" s="18" t="s">
         <v>3777</v>
       </c>
-      <c r="D656" s="9" t="s">
+      <c r="D657" s="9" t="s">
         <v>3778</v>
       </c>
     </row>
@@ -31109,8 +31136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -32079,10 +32106,10 @@
         <v>3438</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>3754</v>
+        <v>3752</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>3755</v>
+        <v>3753</v>
       </c>
       <c r="E48" s="1">
         <v>5</v>
@@ -32099,10 +32126,10 @@
         <v>3483</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>3484</v>
+        <v>3780</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>3486</v>
+        <v>3781</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
@@ -32119,7 +32146,7 @@
         <v>3483</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>3188</v>
@@ -32156,13 +32183,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>3757</v>
+        <v>3755</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>3758</v>
+        <v>3756</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>3765</v>
+        <v>3763</v>
       </c>
       <c r="E52" s="1">
         <v>1</v>
@@ -32176,13 +32203,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>3755</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>3757</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>3759</v>
-      </c>
       <c r="D53" s="9" t="s">
-        <v>3762</v>
+        <v>3760</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
@@ -32196,13 +32223,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>3757</v>
+        <v>3755</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>3760</v>
+        <v>3758</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>3763</v>
+        <v>3761</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -32216,13 +32243,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>3757</v>
+        <v>3755</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>3761</v>
+        <v>3759</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>3764</v>
+        <v>3762</v>
       </c>
       <c r="E55" s="1">
         <v>4</v>
@@ -32236,7 +32263,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>3768</v>
+        <v>3766</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>2710</v>
@@ -32256,13 +32283,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>3766</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>3767</v>
+      </c>
+      <c r="D57" s="9" t="s">
         <v>3768</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>3769</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>3770</v>
       </c>
       <c r="E57" s="1">
         <v>1</v>
@@ -32343,7 +32370,7 @@
         <v>1836</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3625</v>
+        <v>3623</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>1885</v>
@@ -32395,7 +32422,7 @@
         <v>1817</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>3626</v>
+        <v>3624</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>1887</v>
@@ -32421,7 +32448,7 @@
         <v>1818</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3627</v>
+        <v>3625</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>1888</v>
@@ -32449,7 +32476,7 @@
         <v>1819</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3628</v>
+        <v>3626</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1889</v>
@@ -32477,7 +32504,7 @@
         <v>1837</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>3629</v>
+        <v>3627</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>1890</v>
@@ -32505,7 +32532,7 @@
         <v>1820</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>3630</v>
+        <v>3628</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>1891</v>
@@ -32533,7 +32560,7 @@
         <v>1821</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>3631</v>
+        <v>3629</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>1892</v>
@@ -32589,7 +32616,7 @@
         <v>1822</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>3632</v>
+        <v>3630</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>1894</v>
@@ -32617,7 +32644,7 @@
         <v>1823</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>3633</v>
+        <v>3631</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>1895</v>
@@ -32645,7 +32672,7 @@
         <v>1824</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>3634</v>
+        <v>3632</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>1896</v>
@@ -32673,7 +32700,7 @@
         <v>1825</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>3635</v>
+        <v>3633</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>1897</v>
@@ -32701,7 +32728,7 @@
         <v>1826</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>3636</v>
+        <v>3634</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>1898</v>
@@ -32729,7 +32756,7 @@
         <v>1827</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>3637</v>
+        <v>3635</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>1899</v>
@@ -32757,7 +32784,7 @@
         <v>1828</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>3638</v>
+        <v>3636</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>1900</v>
@@ -32785,7 +32812,7 @@
         <v>1829</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>3639</v>
+        <v>3637</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>1901</v>
@@ -32813,7 +32840,7 @@
         <v>1839</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>3640</v>
+        <v>3638</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>1902</v>
@@ -32841,7 +32868,7 @@
         <v>1830</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>3641</v>
+        <v>3639</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>1903</v>
@@ -32869,7 +32896,7 @@
         <v>1840</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>3642</v>
+        <v>3640</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>1899</v>
@@ -32897,7 +32924,7 @@
         <v>1831</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>3643</v>
+        <v>3641</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>1904</v>
@@ -32925,7 +32952,7 @@
         <v>1832</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>3644</v>
+        <v>3642</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>1905</v>
@@ -32953,7 +32980,7 @@
         <v>1842</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>3645</v>
+        <v>3643</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>1906</v>
@@ -32981,7 +33008,7 @@
         <v>1993</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>3646</v>
+        <v>3644</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>1907</v>
@@ -33009,7 +33036,7 @@
         <v>1992</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>3647</v>
+        <v>3645</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="1"/>
@@ -33033,7 +33060,7 @@
         <v>1990</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>3648</v>
+        <v>3646</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>1908</v>
@@ -33061,7 +33088,7 @@
         <v>1991</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>3649</v>
+        <v>3647</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="1"/>
@@ -33085,7 +33112,7 @@
         <v>1833</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>3650</v>
+        <v>3648</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>1909</v>
@@ -33113,7 +33140,7 @@
         <v>1834</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>3651</v>
+        <v>3649</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="1"/>
@@ -33137,7 +33164,7 @@
         <v>1835</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>3652</v>
+        <v>3650</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="1"/>

</xml_diff>

<commit_message>
Adjustment of the data maintenance module
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0F7682-01D6-4F58-9484-7D86FF69ACE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505252DE-E175-4E59-AEDA-B19704C7A89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4010" uniqueCount="3785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4013" uniqueCount="3788">
   <si>
     <t>myself</t>
   </si>
@@ -14292,6 +14292,18 @@
   </si>
   <si>
     <t>日汇总计算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>protocolSaveConfirm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称或地址出现重复，保存将会覆盖，是否继续？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If there is a duplicate name or address, the save will be overwritten, do you want to continue?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -21924,10 +21936,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D657"/>
+  <dimension ref="A1:D658"/>
   <sheetViews>
-    <sheetView topLeftCell="A638" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B661" sqref="B661"/>
+    <sheetView tabSelected="1" topLeftCell="C638" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D662" sqref="D662"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -31135,6 +31147,20 @@
         <v>3771</v>
       </c>
     </row>
+    <row r="658" spans="1:4">
+      <c r="A658" s="15">
+        <v>657</v>
+      </c>
+      <c r="B658" s="5" t="s">
+        <v>3785</v>
+      </c>
+      <c r="C658" s="18" t="s">
+        <v>3786</v>
+      </c>
+      <c r="D658" s="9" t="s">
+        <v>3787</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31146,7 +31172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Data export has been improved.
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64610807-CFDA-4426-B57F-CA0836BE4CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9157C01F-44CC-427F-BD2D-806B38C41F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4019" uniqueCount="3794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4034" uniqueCount="3809">
   <si>
     <t>myself</t>
   </si>
@@ -14331,6 +14331,63 @@
   <si>
     <t>Number of records after thinning</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>primaryDdeviceExportFileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auxiliaryDdeviceExportFileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备导出数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Device export data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>辅助设备的导出数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Export data for ancillary devices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>organizationExportFileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>组织导出数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userExportFileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户导出数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roleExportFileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色导出数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Organizations export data</t>
+  </si>
+  <si>
+    <t>User exports data</t>
+  </si>
+  <si>
+    <t>Role export data</t>
   </si>
 </sst>
 </file>
@@ -14822,7 +14879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -21976,10 +22033,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D659"/>
+  <dimension ref="A1:D664"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A646" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C670" sqref="C670"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -31213,6 +31270,76 @@
       </c>
       <c r="D659" s="9" t="s">
         <v>3785</v>
+      </c>
+    </row>
+    <row r="660" spans="1:4">
+      <c r="A660" s="15">
+        <v>659</v>
+      </c>
+      <c r="B660" s="5" t="s">
+        <v>3794</v>
+      </c>
+      <c r="C660" s="18" t="s">
+        <v>3796</v>
+      </c>
+      <c r="D660" s="9" t="s">
+        <v>3797</v>
+      </c>
+    </row>
+    <row r="661" spans="1:4">
+      <c r="A661" s="15">
+        <v>660</v>
+      </c>
+      <c r="B661" s="5" t="s">
+        <v>3795</v>
+      </c>
+      <c r="C661" s="18" t="s">
+        <v>3798</v>
+      </c>
+      <c r="D661" s="9" t="s">
+        <v>3799</v>
+      </c>
+    </row>
+    <row r="662" spans="1:4">
+      <c r="A662" s="15">
+        <v>661</v>
+      </c>
+      <c r="B662" s="5" t="s">
+        <v>3800</v>
+      </c>
+      <c r="C662" s="18" t="s">
+        <v>3801</v>
+      </c>
+      <c r="D662" s="18" t="s">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="663" spans="1:4">
+      <c r="A663" s="15">
+        <v>662</v>
+      </c>
+      <c r="B663" s="5" t="s">
+        <v>3802</v>
+      </c>
+      <c r="C663" s="18" t="s">
+        <v>3803</v>
+      </c>
+      <c r="D663" s="18" t="s">
+        <v>3807</v>
+      </c>
+    </row>
+    <row r="664" spans="1:4">
+      <c r="A664" s="15">
+        <v>663</v>
+      </c>
+      <c r="B664" s="5" t="s">
+        <v>3804</v>
+      </c>
+      <c r="C664" s="18" t="s">
+        <v>3805</v>
+      </c>
+      <c r="D664" s="18" t="s">
+        <v>3808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Module import/export, historical data query, table space maintenance and other functions have been adjusted.
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1475FE-0DDB-4894-8E7C-BECDC708D750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D950FC45-8C48-4A36-8D03-61917A769DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4061" uniqueCount="3836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4073" uniqueCount="3848">
   <si>
     <t>myself</t>
   </si>
@@ -14553,6 +14553,50 @@
   <si>
     <t>importRole</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataDictionaryList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字典列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>importDictionaryList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导入数据字典</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moduleExportFileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模块导出数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>importModule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导入模块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dictionary list</t>
+  </si>
+  <si>
+    <t>Import data dictionary</t>
+  </si>
+  <si>
+    <t>module exports data</t>
+  </si>
+  <si>
+    <t>Import modules</t>
   </si>
 </sst>
 </file>
@@ -22226,8 +22270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
   <dimension ref="A1:D683"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A657" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B673" sqref="B673"/>
+    <sheetView tabSelected="1" topLeftCell="D657" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I679" sqref="I679"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -31660,28 +31704,60 @@
       </c>
     </row>
     <row r="674" spans="1:4">
-      <c r="A674" s="14"/>
-      <c r="B674" s="4"/>
-      <c r="C674" s="17"/>
-      <c r="D674" s="24"/>
+      <c r="A674" s="14">
+        <v>673</v>
+      </c>
+      <c r="B674" s="4" t="s">
+        <v>3836</v>
+      </c>
+      <c r="C674" s="17" t="s">
+        <v>3837</v>
+      </c>
+      <c r="D674" s="24" t="s">
+        <v>3844</v>
+      </c>
     </row>
     <row r="675" spans="1:4">
-      <c r="A675" s="14"/>
-      <c r="B675" s="4"/>
-      <c r="C675" s="17"/>
-      <c r="D675" s="24"/>
+      <c r="A675" s="14">
+        <v>674</v>
+      </c>
+      <c r="B675" s="4" t="s">
+        <v>3838</v>
+      </c>
+      <c r="C675" s="17" t="s">
+        <v>3839</v>
+      </c>
+      <c r="D675" s="24" t="s">
+        <v>3845</v>
+      </c>
     </row>
     <row r="676" spans="1:4">
-      <c r="A676" s="14"/>
-      <c r="B676" s="4"/>
-      <c r="C676" s="17"/>
-      <c r="D676" s="24"/>
+      <c r="A676" s="14">
+        <v>675</v>
+      </c>
+      <c r="B676" s="4" t="s">
+        <v>3840</v>
+      </c>
+      <c r="C676" s="17" t="s">
+        <v>3841</v>
+      </c>
+      <c r="D676" s="24" t="s">
+        <v>3846</v>
+      </c>
     </row>
     <row r="677" spans="1:4">
-      <c r="A677" s="14"/>
-      <c r="B677" s="4"/>
-      <c r="C677" s="17"/>
-      <c r="D677" s="24"/>
+      <c r="A677" s="14">
+        <v>676</v>
+      </c>
+      <c r="B677" s="4" t="s">
+        <v>3842</v>
+      </c>
+      <c r="C677" s="17" t="s">
+        <v>3843</v>
+      </c>
+      <c r="D677" s="24" t="s">
+        <v>3847</v>
+      </c>
     </row>
     <row r="678" spans="1:4">
       <c r="A678" s="14"/>

</xml_diff>

<commit_message>
Instance cascading relationship implementation
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D950FC45-8C48-4A36-8D03-61917A769DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF16D57C-83D8-4476-82C4-832EF0568E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4073" uniqueCount="3848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4219" uniqueCount="3993">
   <si>
     <t>myself</t>
   </si>
@@ -13150,14 +13150,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Intelligent monitoring system V9.6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intelligent monitoring system V9.6 mainly focuses on oil well intelligent analysis on the basis of collection and control. The module includes real-time monitoring, historical query, production report, fault query, log query, computing maintenance, driver configuration, rights management, device management, and system configuration. The system applies big data analysis method to carry out statistical analysis on key production indicators such as working conditions, output, liquid level, balance and energy consumption, so as to find abnormal production Wells in time, tap potential production Wells, and improve the control ability of target blocks and individual Wells.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>The type of calculation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -14116,14 +14108,6 @@
   </si>
   <si>
     <t>Dynamometer construction data-ground efficiency</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>智能监控系统 V9.6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>《智能监控系统 V9.6》主要在采集、控制的基础上，侧重油井智能分析。模块主要包括实时监控、历史查询、生产报表、故障查询、日志查询、计算维护、驱动配置、权限管理、设备管理、系统配置等。系统应用大数据分析方法，对工况、产量、液面、平衡、能耗等生产关键指标进行统计分析，及时发现生产不正常井，挖掘生产潜力井，提升对目标区块和单井的管控能力。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -14597,6 +14581,554 @@
   </si>
   <si>
     <t>Import modules</t>
+  </si>
+  <si>
+    <t>运维配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O&amp;M configuration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basicInformation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>backupAndRecovery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备份与恢复</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginInterfaceLanguage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录界面语言</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timeEfficiencyUnit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时率单位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sendSimulationData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送模拟数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>displayTheLogo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示logo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resourceMonitoringLimit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源监测记录数限值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simulateDataSendingCycles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟数据发送周期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>printLogs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打印日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exportDataLimits</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导出数据限值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>historicalDataMaintenance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>历史数据维护</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>executionCycle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>执行周期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>historicalDataTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>历史数据表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sourceDataTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>源数据表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alarmHistoryTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>报警历史表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dailyTotalCalculateTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日累计计算表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dailyCalculationTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汇总表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timingCalculationTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定时汇总表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>acqdataVacuateTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据抽稀表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>executionTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>执行时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataRetentionTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据保留时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>endTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结束时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataSparseness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据抽稀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sparseRecordCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽稀记录数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vacuateSaveIntervalWaveRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽稀数据保存周期波动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vacuateSaveInterval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽稀数据保存间隔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vacuateThreshold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽稀表启用时的记录数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>recordsGreaterThan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记录数大于</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>submit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oneKeyBackup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一键导出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>featureList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>backupDataImport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备份数据导入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>previous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上一步</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>next</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下一步</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Basic information</t>
+  </si>
+  <si>
+    <t>Backup and recovery</t>
+  </si>
+  <si>
+    <t>Login interface language</t>
+  </si>
+  <si>
+    <t>Hourly rate unit</t>
+  </si>
+  <si>
+    <t>Send simulation data</t>
+  </si>
+  <si>
+    <t>Display the logo</t>
+  </si>
+  <si>
+    <t>Limit of the number of resource monitoring records</t>
+  </si>
+  <si>
+    <t>Simulate data sending cycles</t>
+  </si>
+  <si>
+    <t>Print logs</t>
+  </si>
+  <si>
+    <t>Export data limits</t>
+  </si>
+  <si>
+    <t>Historical data maintenance</t>
+  </si>
+  <si>
+    <t>Execution cycle</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>Historical data table</t>
+  </si>
+  <si>
+    <t>Source data table</t>
+  </si>
+  <si>
+    <t>Alarm history table</t>
+  </si>
+  <si>
+    <t>Daily cumulative calculation table</t>
+  </si>
+  <si>
+    <t>Summary table</t>
+  </si>
+  <si>
+    <t>Timing summary table</t>
+  </si>
+  <si>
+    <t>Data sparse table</t>
+  </si>
+  <si>
+    <t>Execution time</t>
+  </si>
+  <si>
+    <t>Data retention time</t>
+  </si>
+  <si>
+    <t>End time</t>
+  </si>
+  <si>
+    <t>Data sparseness</t>
+  </si>
+  <si>
+    <t>Number of sparse records</t>
+  </si>
+  <si>
+    <t>The storage period of sampling data fluctuates</t>
+  </si>
+  <si>
+    <t>Sampling data storage interval</t>
+  </si>
+  <si>
+    <t>The number of records when the sparse table is enabled</t>
+  </si>
+  <si>
+    <t>The number of records is greater than</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>One-click export</t>
+  </si>
+  <si>
+    <t>Feature list</t>
+  </si>
+  <si>
+    <t>Backup data import</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>智能监控系统 V9.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《智能监控系统 V9.7》主要在采集、控制的基础上，侧重油井智能分析。模块主要包括实时监控、历史查询、生产报表、故障查询、日志查询、计算维护、驱动配置、权限管理、设备管理、系统配置等。系统应用大数据分析方法，对工况、产量、液面、平衡、能耗等生产关键指标进行统计分析，及时发现生产不正常井，挖掘生产潜力井，提升对目标区块和单井的管控能力。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intelligent monitoring system V9.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intelligent monitoring system V9.7 mainly focuses on oil well intelligent analysis on the basis of collection and control. The module includes real-time monitoring, historical query, production report, fault query, log query, computing maintenance, driver configuration, rights management, device management, and system configuration. The system applies big data analysis method to carry out statistical analysis on key production indicators such as working conditions, output, liquid level, balance and energy consumption, so as to find abnormal production Wells in time, tap potential production Wells, and improve the control ability of target blocks and individual Wells.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataDictionary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据字典</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>organization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>组织</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>primaryDevice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pleaseImportModuleData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先导入模块数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pleaseImportOrgAndRoleData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先导入组织数据和角色数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pleaseImportOrgAndDriverData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先导入组织数据和驱动数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pleaseImportProtocolData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先导入协议数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pleaseImportAcqUnitData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先导入采控单元数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pleaseImportDisplayUnitData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先导入显示单元数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pleaseImportAlarmUnitData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先导入报警单元数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pleaseImportReportUnitData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先导入报表单元数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>Data Dictionary</t>
+  </si>
+  <si>
+    <t>organization</t>
+  </si>
+  <si>
+    <t>Main equipment</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Import the module data first</t>
+  </si>
+  <si>
+    <t>Import your organization data and role data first</t>
+  </si>
+  <si>
+    <t>Import organizational data and driver data first</t>
+  </si>
+  <si>
+    <t>Please import the protocol data first</t>
+  </si>
+  <si>
+    <t>Import the data of the control unit first</t>
+  </si>
+  <si>
+    <t>Please import the display unit data first</t>
+  </si>
+  <si>
+    <t>Please import the alarm unit data first</t>
+  </si>
+  <si>
+    <t>Please import the report unit data first</t>
   </si>
 </sst>
 </file>
@@ -15383,13 +15915,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3788</v>
+        <v>3784</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>3789</v>
+        <v>3785</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>3790</v>
+        <v>3786</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -16846,7 +17378,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16879,10 +17411,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>3738</v>
+        <v>3951</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>3493</v>
+        <v>3953</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -16893,10 +17425,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>3739</v>
+        <v>3952</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>3494</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -18022,13 +18554,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>3654</v>
+        <v>3652</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>3649</v>
+        <v>3647</v>
       </c>
       <c r="D68" s="24" t="s">
-        <v>3659</v>
+        <v>3657</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -18036,13 +18568,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>3655</v>
+        <v>3653</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>3650</v>
+        <v>3648</v>
       </c>
       <c r="D69" s="24" t="s">
-        <v>3660</v>
+        <v>3658</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -18050,13 +18582,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>3656</v>
+        <v>3654</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>3651</v>
+        <v>3649</v>
       </c>
       <c r="D70" s="24" t="s">
-        <v>3661</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -18064,13 +18596,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>3657</v>
+        <v>3655</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>3652</v>
+        <v>3650</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>3662</v>
+        <v>3660</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -18078,13 +18610,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>3658</v>
+        <v>3656</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>3653</v>
+        <v>3651</v>
       </c>
       <c r="D72" s="24" t="s">
-        <v>3663</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -19974,7 +20506,7 @@
         <v>1279</v>
       </c>
       <c r="D207" s="24" t="s">
-        <v>3498</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -19988,7 +20520,7 @@
         <v>1280</v>
       </c>
       <c r="D208" s="24" t="s">
-        <v>3499</v>
+        <v>3497</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -20002,7 +20534,7 @@
         <v>1281</v>
       </c>
       <c r="D209" s="24" t="s">
-        <v>3500</v>
+        <v>3498</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -20016,7 +20548,7 @@
         <v>1282</v>
       </c>
       <c r="D210" s="24" t="s">
-        <v>3501</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -20030,7 +20562,7 @@
         <v>1283</v>
       </c>
       <c r="D211" s="24" t="s">
-        <v>3502</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -20044,7 +20576,7 @@
         <v>1284</v>
       </c>
       <c r="D212" s="24" t="s">
-        <v>3503</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -20058,7 +20590,7 @@
         <v>1285</v>
       </c>
       <c r="D213" s="24" t="s">
-        <v>3504</v>
+        <v>3502</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -20072,7 +20604,7 @@
         <v>1286</v>
       </c>
       <c r="D214" s="24" t="s">
-        <v>3505</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -20100,7 +20632,7 @@
         <v>1287</v>
       </c>
       <c r="D216" s="24" t="s">
-        <v>3506</v>
+        <v>3504</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -20114,7 +20646,7 @@
         <v>1288</v>
       </c>
       <c r="D217" s="24" t="s">
-        <v>3507</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -20212,7 +20744,7 @@
         <v>1840</v>
       </c>
       <c r="D224" s="24" t="s">
-        <v>3508</v>
+        <v>3506</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -20226,7 +20758,7 @@
         <v>1841</v>
       </c>
       <c r="D225" s="24" t="s">
-        <v>3509</v>
+        <v>3507</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -20254,7 +20786,7 @@
         <v>1843</v>
       </c>
       <c r="D227" s="24" t="s">
-        <v>3510</v>
+        <v>3508</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -20262,13 +20794,13 @@
         <v>227</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>3516</v>
+        <v>3514</v>
       </c>
       <c r="C228" s="8" t="s">
-        <v>3511</v>
+        <v>3509</v>
       </c>
       <c r="D228" s="24" t="s">
-        <v>3514</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -20276,13 +20808,13 @@
         <v>228</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>3517</v>
+        <v>3515</v>
       </c>
       <c r="C229" s="8" t="s">
-        <v>3512</v>
+        <v>3510</v>
       </c>
       <c r="D229" s="24" t="s">
-        <v>3553</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -20290,13 +20822,13 @@
         <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>3515</v>
+        <v>3513</v>
       </c>
       <c r="C230" s="8" t="s">
-        <v>3609</v>
+        <v>3607</v>
       </c>
       <c r="D230" s="24" t="s">
-        <v>3610</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -20304,13 +20836,13 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>3518</v>
+        <v>3516</v>
       </c>
       <c r="C231" s="8" t="s">
-        <v>3609</v>
+        <v>3607</v>
       </c>
       <c r="D231" s="24" t="s">
-        <v>3610</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -20318,13 +20850,13 @@
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>3519</v>
+        <v>3517</v>
       </c>
       <c r="C232" s="8" t="s">
-        <v>3513</v>
+        <v>3511</v>
       </c>
       <c r="D232" s="24" t="s">
-        <v>3554</v>
+        <v>3552</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15" customHeight="1">
@@ -20332,13 +20864,13 @@
         <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>3520</v>
+        <v>3518</v>
       </c>
       <c r="C233" s="8" t="s">
-        <v>3551</v>
+        <v>3549</v>
       </c>
       <c r="D233" s="24" t="s">
-        <v>3555</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -20346,13 +20878,13 @@
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>3522</v>
+        <v>3520</v>
       </c>
       <c r="C234" s="8" t="s">
-        <v>3556</v>
+        <v>3554</v>
       </c>
       <c r="D234" s="24" t="s">
-        <v>3557</v>
+        <v>3555</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -20360,13 +20892,13 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>3521</v>
+        <v>3519</v>
       </c>
       <c r="C235" s="8" t="s">
-        <v>3558</v>
+        <v>3556</v>
       </c>
       <c r="D235" s="24" t="s">
-        <v>3559</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -20374,13 +20906,13 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>3523</v>
+        <v>3521</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>3560</v>
+        <v>3558</v>
       </c>
       <c r="D236" s="24" t="s">
-        <v>3561</v>
+        <v>3559</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -20388,13 +20920,13 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>3524</v>
+        <v>3522</v>
       </c>
       <c r="C237" s="8" t="s">
-        <v>3562</v>
+        <v>3560</v>
       </c>
       <c r="D237" s="24" t="s">
-        <v>3563</v>
+        <v>3561</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -20402,13 +20934,13 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>3525</v>
+        <v>3523</v>
       </c>
       <c r="C238" s="8" t="s">
-        <v>3564</v>
+        <v>3562</v>
       </c>
       <c r="D238" s="24" t="s">
-        <v>3565</v>
+        <v>3563</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -20416,13 +20948,13 @@
         <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>3526</v>
+        <v>3524</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>3566</v>
+        <v>3564</v>
       </c>
       <c r="D239" s="24" t="s">
-        <v>3567</v>
+        <v>3565</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -20430,13 +20962,13 @@
         <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>3527</v>
+        <v>3525</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>3568</v>
+        <v>3566</v>
       </c>
       <c r="D240" s="24" t="s">
-        <v>3569</v>
+        <v>3567</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -20444,13 +20976,13 @@
         <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>3528</v>
+        <v>3526</v>
       </c>
       <c r="C241" s="8" t="s">
-        <v>3570</v>
+        <v>3568</v>
       </c>
       <c r="D241" s="24" t="s">
-        <v>3571</v>
+        <v>3569</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -20458,13 +20990,13 @@
         <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>3529</v>
+        <v>3527</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>3552</v>
+        <v>3550</v>
       </c>
       <c r="D242" s="24" t="s">
-        <v>3572</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -20472,13 +21004,13 @@
         <v>242</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>3530</v>
+        <v>3528</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>3573</v>
+        <v>3571</v>
       </c>
       <c r="D243" s="24" t="s">
-        <v>3574</v>
+        <v>3572</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -20486,13 +21018,13 @@
         <v>243</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>3531</v>
+        <v>3529</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>3575</v>
+        <v>3573</v>
       </c>
       <c r="D244" s="24" t="s">
-        <v>3576</v>
+        <v>3574</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -20500,13 +21032,13 @@
         <v>244</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>3532</v>
+        <v>3530</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>3533</v>
+        <v>3531</v>
       </c>
       <c r="D245" s="24" t="s">
-        <v>3577</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -20514,13 +21046,13 @@
         <v>245</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>3534</v>
+        <v>3532</v>
       </c>
       <c r="C246" s="8" t="s">
-        <v>3578</v>
+        <v>3576</v>
       </c>
       <c r="D246" s="24" t="s">
-        <v>3579</v>
+        <v>3577</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -20528,13 +21060,13 @@
         <v>246</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>3535</v>
+        <v>3533</v>
       </c>
       <c r="C247" s="8" t="s">
-        <v>3580</v>
+        <v>3578</v>
       </c>
       <c r="D247" s="24" t="s">
-        <v>3581</v>
+        <v>3579</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -20542,13 +21074,13 @@
         <v>247</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
       <c r="C248" s="8" t="s">
-        <v>3582</v>
+        <v>3580</v>
       </c>
       <c r="D248" s="24" t="s">
-        <v>3583</v>
+        <v>3581</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -20556,13 +21088,13 @@
         <v>248</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>3537</v>
+        <v>3535</v>
       </c>
       <c r="C249" s="8" t="s">
-        <v>3584</v>
+        <v>3582</v>
       </c>
       <c r="D249" s="24" t="s">
-        <v>3585</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -20570,13 +21102,13 @@
         <v>249</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>3538</v>
+        <v>3536</v>
       </c>
       <c r="C250" s="8" t="s">
-        <v>3586</v>
+        <v>3584</v>
       </c>
       <c r="D250" s="24" t="s">
-        <v>3587</v>
+        <v>3585</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -20584,13 +21116,13 @@
         <v>250</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>3539</v>
+        <v>3537</v>
       </c>
       <c r="C251" s="8" t="s">
-        <v>3588</v>
+        <v>3586</v>
       </c>
       <c r="D251" s="24" t="s">
-        <v>3589</v>
+        <v>3587</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -20598,13 +21130,13 @@
         <v>251</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>3540</v>
+        <v>3538</v>
       </c>
       <c r="C252" s="8" t="s">
-        <v>3590</v>
+        <v>3588</v>
       </c>
       <c r="D252" s="24" t="s">
-        <v>3591</v>
+        <v>3589</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -20612,13 +21144,13 @@
         <v>252</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>3541</v>
+        <v>3539</v>
       </c>
       <c r="C253" s="8" t="s">
-        <v>3592</v>
+        <v>3590</v>
       </c>
       <c r="D253" s="24" t="s">
-        <v>3593</v>
+        <v>3591</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -20626,13 +21158,13 @@
         <v>253</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>3542</v>
+        <v>3540</v>
       </c>
       <c r="C254" s="8" t="s">
-        <v>3594</v>
+        <v>3592</v>
       </c>
       <c r="D254" s="24" t="s">
-        <v>3595</v>
+        <v>3593</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -20640,13 +21172,13 @@
         <v>254</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>3543</v>
+        <v>3541</v>
       </c>
       <c r="C255" s="8" t="s">
-        <v>3596</v>
+        <v>3594</v>
       </c>
       <c r="D255" s="24" t="s">
-        <v>3597</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -20654,13 +21186,13 @@
         <v>255</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>3544</v>
+        <v>3542</v>
       </c>
       <c r="C256" s="8" t="s">
-        <v>3545</v>
+        <v>3543</v>
       </c>
       <c r="D256" s="24" t="s">
-        <v>3598</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -20668,13 +21200,13 @@
         <v>256</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>3546</v>
+        <v>3544</v>
       </c>
       <c r="C257" s="8" t="s">
-        <v>3599</v>
+        <v>3597</v>
       </c>
       <c r="D257" s="24" t="s">
-        <v>3600</v>
+        <v>3598</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -20682,13 +21214,13 @@
         <v>257</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>3547</v>
+        <v>3545</v>
       </c>
       <c r="C258" s="8" t="s">
-        <v>3601</v>
+        <v>3599</v>
       </c>
       <c r="D258" s="24" t="s">
-        <v>3602</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -20696,13 +21228,13 @@
         <v>258</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>3548</v>
+        <v>3546</v>
       </c>
       <c r="C259" s="8" t="s">
-        <v>3603</v>
+        <v>3601</v>
       </c>
       <c r="D259" s="24" t="s">
-        <v>3604</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -20710,13 +21242,13 @@
         <v>259</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>3549</v>
+        <v>3547</v>
       </c>
       <c r="C260" s="8" t="s">
-        <v>3605</v>
+        <v>3603</v>
       </c>
       <c r="D260" s="24" t="s">
-        <v>3606</v>
+        <v>3604</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -20724,13 +21256,13 @@
         <v>260</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>3550</v>
+        <v>3548</v>
       </c>
       <c r="C261" s="8" t="s">
-        <v>3607</v>
+        <v>3605</v>
       </c>
       <c r="D261" s="24" t="s">
-        <v>3608</v>
+        <v>3606</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -20744,7 +21276,7 @@
         <v>2477</v>
       </c>
       <c r="D262" s="24" t="s">
-        <v>3639</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -20772,7 +21304,7 @@
         <v>2478</v>
       </c>
       <c r="D264" s="24" t="s">
-        <v>3640</v>
+        <v>3638</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -20786,7 +21318,7 @@
         <v>2479</v>
       </c>
       <c r="D265" s="24" t="s">
-        <v>3641</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -20856,7 +21388,7 @@
         <v>2480</v>
       </c>
       <c r="D270" s="24" t="s">
-        <v>3642</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -20884,7 +21416,7 @@
         <v>2482</v>
       </c>
       <c r="D272" s="24" t="s">
-        <v>3643</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -20898,7 +21430,7 @@
         <v>2483</v>
       </c>
       <c r="D273" s="24" t="s">
-        <v>3644</v>
+        <v>3642</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -20912,7 +21444,7 @@
         <v>2484</v>
       </c>
       <c r="D274" s="24" t="s">
-        <v>3645</v>
+        <v>3643</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -20926,7 +21458,7 @@
         <v>2485</v>
       </c>
       <c r="D275" s="24" t="s">
-        <v>3646</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -20968,7 +21500,7 @@
         <v>2486</v>
       </c>
       <c r="D278" s="24" t="s">
-        <v>3647</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -20982,7 +21514,7 @@
         <v>2487</v>
       </c>
       <c r="D279" s="24" t="s">
-        <v>3648</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -21010,7 +21542,7 @@
         <v>2488</v>
       </c>
       <c r="D281" s="24" t="s">
-        <v>3664</v>
+        <v>3662</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -21024,7 +21556,7 @@
         <v>2489</v>
       </c>
       <c r="D282" s="24" t="s">
-        <v>3665</v>
+        <v>3663</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -21038,7 +21570,7 @@
         <v>2490</v>
       </c>
       <c r="D283" s="24" t="s">
-        <v>3666</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -21052,7 +21584,7 @@
         <v>2554</v>
       </c>
       <c r="D284" s="24" t="s">
-        <v>3667</v>
+        <v>3665</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -21066,7 +21598,7 @@
         <v>2555</v>
       </c>
       <c r="D285" s="24" t="s">
-        <v>3668</v>
+        <v>3666</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -21080,7 +21612,7 @@
         <v>2556</v>
       </c>
       <c r="D286" s="24" t="s">
-        <v>3669</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -21094,7 +21626,7 @@
         <v>2557</v>
       </c>
       <c r="D287" s="24" t="s">
-        <v>3670</v>
+        <v>3668</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -21108,7 +21640,7 @@
         <v>2558</v>
       </c>
       <c r="D288" s="24" t="s">
-        <v>3671</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -21122,7 +21654,7 @@
         <v>2559</v>
       </c>
       <c r="D289" s="24" t="s">
-        <v>3672</v>
+        <v>3670</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -21136,7 +21668,7 @@
         <v>2560</v>
       </c>
       <c r="D290" s="24" t="s">
-        <v>3673</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -21150,7 +21682,7 @@
         <v>2561</v>
       </c>
       <c r="D291" s="24" t="s">
-        <v>3674</v>
+        <v>3672</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -21164,7 +21696,7 @@
         <v>2562</v>
       </c>
       <c r="D292" s="24" t="s">
-        <v>3675</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -21178,7 +21710,7 @@
         <v>2563</v>
       </c>
       <c r="D293" s="24" t="s">
-        <v>3676</v>
+        <v>3674</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -21192,7 +21724,7 @@
         <v>2564</v>
       </c>
       <c r="D294" s="24" t="s">
-        <v>3677</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -21206,7 +21738,7 @@
         <v>2565</v>
       </c>
       <c r="D295" s="24" t="s">
-        <v>3678</v>
+        <v>3676</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -21220,7 +21752,7 @@
         <v>2566</v>
       </c>
       <c r="D296" s="24" t="s">
-        <v>3679</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -21234,7 +21766,7 @@
         <v>2567</v>
       </c>
       <c r="D297" s="24" t="s">
-        <v>3680</v>
+        <v>3678</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -21248,7 +21780,7 @@
         <v>2568</v>
       </c>
       <c r="D298" s="24" t="s">
-        <v>3681</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -21262,7 +21794,7 @@
         <v>2569</v>
       </c>
       <c r="D299" s="24" t="s">
-        <v>3682</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -21276,7 +21808,7 @@
         <v>2570</v>
       </c>
       <c r="D300" s="24" t="s">
-        <v>3683</v>
+        <v>3681</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -21290,7 +21822,7 @@
         <v>2571</v>
       </c>
       <c r="D301" s="24" t="s">
-        <v>3684</v>
+        <v>3682</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -21304,7 +21836,7 @@
         <v>2572</v>
       </c>
       <c r="D302" s="24" t="s">
-        <v>3685</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -21318,7 +21850,7 @@
         <v>2573</v>
       </c>
       <c r="D303" s="24" t="s">
-        <v>3686</v>
+        <v>3684</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -21346,7 +21878,7 @@
         <v>2491</v>
       </c>
       <c r="D305" s="24" t="s">
-        <v>3687</v>
+        <v>3685</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -21360,7 +21892,7 @@
         <v>2492</v>
       </c>
       <c r="D306" s="24" t="s">
-        <v>3688</v>
+        <v>3686</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -21374,7 +21906,7 @@
         <v>2493</v>
       </c>
       <c r="D307" s="24" t="s">
-        <v>3689</v>
+        <v>3687</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -21388,7 +21920,7 @@
         <v>2494</v>
       </c>
       <c r="D308" s="24" t="s">
-        <v>3690</v>
+        <v>3688</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -21402,7 +21934,7 @@
         <v>2495</v>
       </c>
       <c r="D309" s="24" t="s">
-        <v>3691</v>
+        <v>3689</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -21416,7 +21948,7 @@
         <v>2496</v>
       </c>
       <c r="D310" s="24" t="s">
-        <v>3692</v>
+        <v>3690</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -21430,7 +21962,7 @@
         <v>2497</v>
       </c>
       <c r="D311" s="24" t="s">
-        <v>3693</v>
+        <v>3691</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -21444,7 +21976,7 @@
         <v>2498</v>
       </c>
       <c r="D312" s="24" t="s">
-        <v>3694</v>
+        <v>3692</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -21458,7 +21990,7 @@
         <v>2499</v>
       </c>
       <c r="D313" s="24" t="s">
-        <v>3695</v>
+        <v>3693</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -21472,7 +22004,7 @@
         <v>2500</v>
       </c>
       <c r="D314" s="24" t="s">
-        <v>3696</v>
+        <v>3694</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -21486,7 +22018,7 @@
         <v>2501</v>
       </c>
       <c r="D315" s="24" t="s">
-        <v>3697</v>
+        <v>3695</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -21500,7 +22032,7 @@
         <v>2502</v>
       </c>
       <c r="D316" s="24" t="s">
-        <v>3698</v>
+        <v>3696</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -21612,7 +22144,7 @@
         <v>2510</v>
       </c>
       <c r="D324" s="24" t="s">
-        <v>3699</v>
+        <v>3697</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -21724,7 +22256,7 @@
         <v>2518</v>
       </c>
       <c r="D332" s="24" t="s">
-        <v>3700</v>
+        <v>3698</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -21738,7 +22270,7 @@
         <v>2519</v>
       </c>
       <c r="D333" s="24" t="s">
-        <v>3701</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -21752,7 +22284,7 @@
         <v>2520</v>
       </c>
       <c r="D334" s="24" t="s">
-        <v>3702</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -21766,7 +22298,7 @@
         <v>2521</v>
       </c>
       <c r="D335" s="24" t="s">
-        <v>3703</v>
+        <v>3701</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -21780,7 +22312,7 @@
         <v>2522</v>
       </c>
       <c r="D336" s="24" t="s">
-        <v>3704</v>
+        <v>3702</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -21791,10 +22323,10 @@
         <v>2095</v>
       </c>
       <c r="C337" s="20" t="s">
-        <v>3705</v>
+        <v>3703</v>
       </c>
       <c r="D337" s="24" t="s">
-        <v>3717</v>
+        <v>3715</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -21805,10 +22337,10 @@
         <v>2096</v>
       </c>
       <c r="C338" s="20" t="s">
-        <v>3718</v>
+        <v>3716</v>
       </c>
       <c r="D338" s="24" t="s">
-        <v>3719</v>
+        <v>3717</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -21819,10 +22351,10 @@
         <v>2097</v>
       </c>
       <c r="C339" s="20" t="s">
-        <v>3736</v>
+        <v>3734</v>
       </c>
       <c r="D339" s="24" t="s">
-        <v>3737</v>
+        <v>3735</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -21833,10 +22365,10 @@
         <v>2098</v>
       </c>
       <c r="C340" s="20" t="s">
-        <v>3706</v>
+        <v>3704</v>
       </c>
       <c r="D340" s="24" t="s">
-        <v>3720</v>
+        <v>3718</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -21847,10 +22379,10 @@
         <v>2109</v>
       </c>
       <c r="C341" s="20" t="s">
-        <v>3707</v>
+        <v>3705</v>
       </c>
       <c r="D341" s="24" t="s">
-        <v>3721</v>
+        <v>3719</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -21861,10 +22393,10 @@
         <v>2099</v>
       </c>
       <c r="C342" s="20" t="s">
-        <v>3712</v>
+        <v>3710</v>
       </c>
       <c r="D342" s="24" t="s">
-        <v>3722</v>
+        <v>3720</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -21875,10 +22407,10 @@
         <v>2100</v>
       </c>
       <c r="C343" s="20" t="s">
-        <v>3713</v>
+        <v>3711</v>
       </c>
       <c r="D343" s="24" t="s">
-        <v>3723</v>
+        <v>3721</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -21889,10 +22421,10 @@
         <v>2101</v>
       </c>
       <c r="C344" s="20" t="s">
-        <v>3714</v>
+        <v>3712</v>
       </c>
       <c r="D344" s="24" t="s">
-        <v>3724</v>
+        <v>3722</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -21903,10 +22435,10 @@
         <v>2102</v>
       </c>
       <c r="C345" s="20" t="s">
-        <v>3715</v>
+        <v>3713</v>
       </c>
       <c r="D345" s="24" t="s">
-        <v>3725</v>
+        <v>3723</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -21917,10 +22449,10 @@
         <v>2103</v>
       </c>
       <c r="C346" s="20" t="s">
-        <v>3716</v>
+        <v>3714</v>
       </c>
       <c r="D346" s="24" t="s">
-        <v>3726</v>
+        <v>3724</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -21931,10 +22463,10 @@
         <v>2115</v>
       </c>
       <c r="C347" s="20" t="s">
-        <v>3708</v>
+        <v>3706</v>
       </c>
       <c r="D347" s="24" t="s">
-        <v>3727</v>
+        <v>3725</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -21945,10 +22477,10 @@
         <v>2116</v>
       </c>
       <c r="C348" s="20" t="s">
-        <v>3709</v>
+        <v>3707</v>
       </c>
       <c r="D348" s="24" t="s">
-        <v>3728</v>
+        <v>3726</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -21959,10 +22491,10 @@
         <v>2104</v>
       </c>
       <c r="C349" s="20" t="s">
-        <v>3710</v>
+        <v>3708</v>
       </c>
       <c r="D349" s="24" t="s">
-        <v>3729</v>
+        <v>3727</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -21973,10 +22505,10 @@
         <v>2162</v>
       </c>
       <c r="C350" s="20" t="s">
-        <v>3711</v>
+        <v>3709</v>
       </c>
       <c r="D350" s="31" t="s">
-        <v>3732</v>
+        <v>3730</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -21990,7 +22522,7 @@
         <v>2172</v>
       </c>
       <c r="D351" s="31" t="s">
-        <v>3496</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -22004,7 +22536,7 @@
         <v>2174</v>
       </c>
       <c r="D352" s="31" t="s">
-        <v>3497</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -22186,7 +22718,7 @@
         <v>2166</v>
       </c>
       <c r="D365" s="31" t="s">
-        <v>3733</v>
+        <v>3731</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -22200,7 +22732,7 @@
         <v>2168</v>
       </c>
       <c r="D366" s="31" t="s">
-        <v>3734</v>
+        <v>3732</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -22214,7 +22746,7 @@
         <v>2170</v>
       </c>
       <c r="D367" s="31" t="s">
-        <v>3735</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -22242,7 +22774,7 @@
         <v>2179</v>
       </c>
       <c r="D369" s="24" t="s">
-        <v>3730</v>
+        <v>3728</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -22256,7 +22788,7 @@
         <v>2181</v>
       </c>
       <c r="D370" s="24" t="s">
-        <v>3731</v>
+        <v>3729</v>
       </c>
     </row>
   </sheetData>
@@ -22268,10 +22800,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D683"/>
+  <dimension ref="A1:D725"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D657" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I679" sqref="I679"/>
+    <sheetView tabSelected="1" topLeftCell="A699" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D730" sqref="D730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -23003,10 +23535,10 @@
         <v>1040</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>3760</v>
+        <v>3756</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>3760</v>
+        <v>3756</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -23087,7 +23619,7 @@
         <v>1062</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>3761</v>
+        <v>3757</v>
       </c>
       <c r="D58" s="24" t="s">
         <v>2619</v>
@@ -24316,13 +24848,13 @@
         <v>145</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>3783</v>
+        <v>3779</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>3784</v>
+        <v>3780</v>
       </c>
       <c r="D146" s="24" t="s">
-        <v>3785</v>
+        <v>3781</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -26338,7 +26870,7 @@
         <v>1471</v>
       </c>
       <c r="D290" s="24" t="s">
-        <v>3495</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -29132,13 +29664,13 @@
         <v>489</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>3821</v>
+        <v>3817</v>
       </c>
       <c r="C490" s="17" t="s">
-        <v>3822</v>
+        <v>3818</v>
       </c>
       <c r="D490" s="24" t="s">
-        <v>3823</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="491" spans="1:4">
@@ -31442,13 +31974,13 @@
         <v>654</v>
       </c>
       <c r="B655" s="4" t="s">
-        <v>3742</v>
+        <v>3738</v>
       </c>
       <c r="C655" s="17" t="s">
-        <v>3740</v>
+        <v>3736</v>
       </c>
       <c r="D655" s="24" t="s">
-        <v>3741</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="656" spans="1:4">
@@ -31456,10 +31988,10 @@
         <v>655</v>
       </c>
       <c r="B656" s="4" t="s">
-        <v>3753</v>
+        <v>3749</v>
       </c>
       <c r="C656" s="17" t="s">
-        <v>3752</v>
+        <v>3748</v>
       </c>
       <c r="D656" s="24" t="s">
         <v>850</v>
@@ -31470,13 +32002,13 @@
         <v>656</v>
       </c>
       <c r="B657" s="4" t="s">
-        <v>3757</v>
+        <v>3753</v>
       </c>
       <c r="C657" s="17" t="s">
-        <v>3758</v>
+        <v>3754</v>
       </c>
       <c r="D657" s="24" t="s">
-        <v>3759</v>
+        <v>3755</v>
       </c>
     </row>
     <row r="658" spans="1:4">
@@ -31484,13 +32016,13 @@
         <v>657</v>
       </c>
       <c r="B658" s="4" t="s">
-        <v>3762</v>
+        <v>3758</v>
       </c>
       <c r="C658" s="17" t="s">
-        <v>3763</v>
+        <v>3759</v>
       </c>
       <c r="D658" s="24" t="s">
-        <v>3764</v>
+        <v>3760</v>
       </c>
     </row>
     <row r="659" spans="1:4">
@@ -31498,13 +32030,13 @@
         <v>658</v>
       </c>
       <c r="B659" s="4" t="s">
-        <v>3767</v>
+        <v>3763</v>
       </c>
       <c r="C659" s="17" t="s">
-        <v>3765</v>
+        <v>3761</v>
       </c>
       <c r="D659" s="24" t="s">
-        <v>3766</v>
+        <v>3762</v>
       </c>
     </row>
     <row r="660" spans="1:4">
@@ -31512,13 +32044,13 @@
         <v>659</v>
       </c>
       <c r="B660" s="4" t="s">
-        <v>3780</v>
+        <v>3776</v>
       </c>
       <c r="C660" s="17" t="s">
-        <v>3781</v>
+        <v>3777</v>
       </c>
       <c r="D660" s="24" t="s">
-        <v>3782</v>
+        <v>3778</v>
       </c>
     </row>
     <row r="661" spans="1:4">
@@ -31526,13 +32058,13 @@
         <v>660</v>
       </c>
       <c r="B661" s="4" t="s">
-        <v>3791</v>
+        <v>3787</v>
       </c>
       <c r="C661" s="17" t="s">
-        <v>3793</v>
+        <v>3789</v>
       </c>
       <c r="D661" s="24" t="s">
-        <v>3794</v>
+        <v>3790</v>
       </c>
     </row>
     <row r="662" spans="1:4">
@@ -31540,13 +32072,13 @@
         <v>661</v>
       </c>
       <c r="B662" s="4" t="s">
+        <v>3788</v>
+      </c>
+      <c r="C662" s="17" t="s">
+        <v>3791</v>
+      </c>
+      <c r="D662" s="24" t="s">
         <v>3792</v>
-      </c>
-      <c r="C662" s="17" t="s">
-        <v>3795</v>
-      </c>
-      <c r="D662" s="24" t="s">
-        <v>3796</v>
       </c>
     </row>
     <row r="663" spans="1:4">
@@ -31554,13 +32086,13 @@
         <v>662</v>
       </c>
       <c r="B663" s="4" t="s">
-        <v>3797</v>
+        <v>3793</v>
       </c>
       <c r="C663" s="17" t="s">
-        <v>3798</v>
+        <v>3794</v>
       </c>
       <c r="D663" s="26" t="s">
-        <v>3803</v>
+        <v>3799</v>
       </c>
     </row>
     <row r="664" spans="1:4">
@@ -31568,13 +32100,13 @@
         <v>663</v>
       </c>
       <c r="B664" s="4" t="s">
-        <v>3799</v>
+        <v>3795</v>
       </c>
       <c r="C664" s="17" t="s">
+        <v>3796</v>
+      </c>
+      <c r="D664" s="26" t="s">
         <v>3800</v>
-      </c>
-      <c r="D664" s="26" t="s">
-        <v>3804</v>
       </c>
     </row>
     <row r="665" spans="1:4">
@@ -31582,13 +32114,13 @@
         <v>664</v>
       </c>
       <c r="B665" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="C665" s="17" t="s">
+        <v>3798</v>
+      </c>
+      <c r="D665" s="26" t="s">
         <v>3801</v>
-      </c>
-      <c r="C665" s="17" t="s">
-        <v>3802</v>
-      </c>
-      <c r="D665" s="26" t="s">
-        <v>3805</v>
       </c>
     </row>
     <row r="666" spans="1:4">
@@ -31596,13 +32128,13 @@
         <v>665</v>
       </c>
       <c r="B666" s="4" t="s">
-        <v>3806</v>
+        <v>3802</v>
       </c>
       <c r="C666" s="17" t="s">
-        <v>3807</v>
+        <v>3803</v>
       </c>
       <c r="D666" s="26" t="s">
-        <v>3808</v>
+        <v>3804</v>
       </c>
     </row>
     <row r="667" spans="1:4">
@@ -31610,13 +32142,13 @@
         <v>666</v>
       </c>
       <c r="B667" s="4" t="s">
-        <v>3809</v>
+        <v>3805</v>
       </c>
       <c r="C667" s="17" t="s">
-        <v>3810</v>
+        <v>3806</v>
       </c>
       <c r="D667" s="24" t="s">
-        <v>3811</v>
+        <v>3807</v>
       </c>
     </row>
     <row r="668" spans="1:4">
@@ -31624,13 +32156,13 @@
         <v>667</v>
       </c>
       <c r="B668" s="4" t="s">
-        <v>3812</v>
+        <v>3808</v>
       </c>
       <c r="C668" s="17" t="s">
-        <v>3813</v>
+        <v>3809</v>
       </c>
       <c r="D668" s="24" t="s">
-        <v>3814</v>
+        <v>3810</v>
       </c>
     </row>
     <row r="669" spans="1:4">
@@ -31638,13 +32170,13 @@
         <v>668</v>
       </c>
       <c r="B669" s="4" t="s">
-        <v>3815</v>
+        <v>3811</v>
       </c>
       <c r="C669" s="17" t="s">
-        <v>3816</v>
+        <v>3812</v>
       </c>
       <c r="D669" s="24" t="s">
-        <v>3817</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="670" spans="1:4">
@@ -31652,13 +32184,13 @@
         <v>669</v>
       </c>
       <c r="B670" s="4" t="s">
-        <v>3818</v>
+        <v>3814</v>
       </c>
       <c r="C670" s="17" t="s">
-        <v>3819</v>
+        <v>3815</v>
       </c>
       <c r="D670" s="24" t="s">
-        <v>3820</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="671" spans="1:4">
@@ -31666,13 +32198,13 @@
         <v>670</v>
       </c>
       <c r="B671" s="4" t="s">
-        <v>3824</v>
+        <v>3820</v>
       </c>
       <c r="C671" s="17" t="s">
-        <v>3825</v>
+        <v>3821</v>
       </c>
       <c r="D671" s="24" t="s">
-        <v>3826</v>
+        <v>3822</v>
       </c>
     </row>
     <row r="672" spans="1:4">
@@ -31680,13 +32212,13 @@
         <v>671</v>
       </c>
       <c r="B672" s="4" t="s">
-        <v>3827</v>
+        <v>3823</v>
       </c>
       <c r="C672" s="17" t="s">
-        <v>3828</v>
+        <v>3824</v>
       </c>
       <c r="D672" s="24" t="s">
-        <v>3829</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="673" spans="1:4">
@@ -31694,13 +32226,13 @@
         <v>672</v>
       </c>
       <c r="B673" s="4" t="s">
-        <v>3835</v>
+        <v>3831</v>
       </c>
       <c r="C673" s="17" t="s">
-        <v>3833</v>
+        <v>3829</v>
       </c>
       <c r="D673" s="24" t="s">
-        <v>3834</v>
+        <v>3830</v>
       </c>
     </row>
     <row r="674" spans="1:4">
@@ -31708,13 +32240,13 @@
         <v>673</v>
       </c>
       <c r="B674" s="4" t="s">
-        <v>3836</v>
+        <v>3832</v>
       </c>
       <c r="C674" s="17" t="s">
-        <v>3837</v>
+        <v>3833</v>
       </c>
       <c r="D674" s="24" t="s">
-        <v>3844</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="675" spans="1:4">
@@ -31722,13 +32254,13 @@
         <v>674</v>
       </c>
       <c r="B675" s="4" t="s">
-        <v>3838</v>
+        <v>3834</v>
       </c>
       <c r="C675" s="17" t="s">
-        <v>3839</v>
+        <v>3835</v>
       </c>
       <c r="D675" s="24" t="s">
-        <v>3845</v>
+        <v>3841</v>
       </c>
     </row>
     <row r="676" spans="1:4">
@@ -31736,13 +32268,13 @@
         <v>675</v>
       </c>
       <c r="B676" s="4" t="s">
-        <v>3840</v>
+        <v>3836</v>
       </c>
       <c r="C676" s="17" t="s">
-        <v>3841</v>
+        <v>3837</v>
       </c>
       <c r="D676" s="24" t="s">
-        <v>3846</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="677" spans="1:4">
@@ -31750,50 +32282,686 @@
         <v>676</v>
       </c>
       <c r="B677" s="4" t="s">
-        <v>3842</v>
+        <v>3838</v>
       </c>
       <c r="C677" s="17" t="s">
+        <v>3839</v>
+      </c>
+      <c r="D677" s="24" t="s">
         <v>3843</v>
       </c>
-      <c r="D677" s="24" t="s">
+    </row>
+    <row r="678" spans="1:4">
+      <c r="A678" s="14">
+        <v>677</v>
+      </c>
+      <c r="B678" s="4" t="s">
+        <v>3846</v>
+      </c>
+      <c r="C678" s="17" t="s">
         <v>3847</v>
       </c>
-    </row>
-    <row r="678" spans="1:4">
-      <c r="A678" s="14"/>
-      <c r="B678" s="4"/>
-      <c r="C678" s="17"/>
-      <c r="D678" s="24"/>
+      <c r="D678" s="24" t="s">
+        <v>3916</v>
+      </c>
     </row>
     <row r="679" spans="1:4">
-      <c r="A679" s="14"/>
-      <c r="B679" s="4"/>
-      <c r="C679" s="17"/>
-      <c r="D679" s="24"/>
+      <c r="A679" s="14">
+        <v>678</v>
+      </c>
+      <c r="B679" s="4" t="s">
+        <v>3848</v>
+      </c>
+      <c r="C679" s="17" t="s">
+        <v>3849</v>
+      </c>
+      <c r="D679" s="24" t="s">
+        <v>3917</v>
+      </c>
     </row>
     <row r="680" spans="1:4">
-      <c r="A680" s="14"/>
-      <c r="B680" s="4"/>
-      <c r="C680" s="17"/>
-      <c r="D680" s="24"/>
+      <c r="A680" s="14">
+        <v>679</v>
+      </c>
+      <c r="B680" s="4" t="s">
+        <v>3850</v>
+      </c>
+      <c r="C680" s="17" t="s">
+        <v>3851</v>
+      </c>
+      <c r="D680" s="24" t="s">
+        <v>3918</v>
+      </c>
     </row>
     <row r="681" spans="1:4">
-      <c r="A681" s="14"/>
-      <c r="B681" s="4"/>
-      <c r="C681" s="17"/>
-      <c r="D681" s="24"/>
+      <c r="A681" s="14">
+        <v>680</v>
+      </c>
+      <c r="B681" s="4" t="s">
+        <v>3852</v>
+      </c>
+      <c r="C681" s="17" t="s">
+        <v>3853</v>
+      </c>
+      <c r="D681" s="24" t="s">
+        <v>3919</v>
+      </c>
     </row>
     <row r="682" spans="1:4">
-      <c r="A682" s="14"/>
-      <c r="B682" s="4"/>
-      <c r="C682" s="17"/>
-      <c r="D682" s="24"/>
+      <c r="A682" s="14">
+        <v>681</v>
+      </c>
+      <c r="B682" s="4" t="s">
+        <v>3854</v>
+      </c>
+      <c r="C682" s="17" t="s">
+        <v>3855</v>
+      </c>
+      <c r="D682" s="24" t="s">
+        <v>3920</v>
+      </c>
     </row>
     <row r="683" spans="1:4">
-      <c r="A683" s="14"/>
-      <c r="B683" s="4"/>
-      <c r="C683" s="17"/>
-      <c r="D683" s="24"/>
+      <c r="A683" s="14">
+        <v>682</v>
+      </c>
+      <c r="B683" s="4" t="s">
+        <v>3856</v>
+      </c>
+      <c r="C683" s="17" t="s">
+        <v>3857</v>
+      </c>
+      <c r="D683" s="24" t="s">
+        <v>3921</v>
+      </c>
+    </row>
+    <row r="684" spans="1:4">
+      <c r="A684" s="14">
+        <v>683</v>
+      </c>
+      <c r="B684" s="4" t="s">
+        <v>3858</v>
+      </c>
+      <c r="C684" s="17" t="s">
+        <v>3859</v>
+      </c>
+      <c r="D684" s="24" t="s">
+        <v>3922</v>
+      </c>
+    </row>
+    <row r="685" spans="1:4">
+      <c r="A685" s="14">
+        <v>684</v>
+      </c>
+      <c r="B685" s="4" t="s">
+        <v>3860</v>
+      </c>
+      <c r="C685" s="17" t="s">
+        <v>3861</v>
+      </c>
+      <c r="D685" s="24" t="s">
+        <v>3923</v>
+      </c>
+    </row>
+    <row r="686" spans="1:4">
+      <c r="A686" s="14">
+        <v>685</v>
+      </c>
+      <c r="B686" s="4" t="s">
+        <v>3862</v>
+      </c>
+      <c r="C686" s="17" t="s">
+        <v>3863</v>
+      </c>
+      <c r="D686" s="24" t="s">
+        <v>3924</v>
+      </c>
+    </row>
+    <row r="687" spans="1:4">
+      <c r="A687" s="14">
+        <v>686</v>
+      </c>
+      <c r="B687" s="4" t="s">
+        <v>3864</v>
+      </c>
+      <c r="C687" s="17" t="s">
+        <v>3865</v>
+      </c>
+      <c r="D687" s="24" t="s">
+        <v>3925</v>
+      </c>
+    </row>
+    <row r="688" spans="1:4">
+      <c r="A688" s="14">
+        <v>687</v>
+      </c>
+      <c r="B688" s="4" t="s">
+        <v>3866</v>
+      </c>
+      <c r="C688" s="17" t="s">
+        <v>3867</v>
+      </c>
+      <c r="D688" s="24" t="s">
+        <v>3926</v>
+      </c>
+    </row>
+    <row r="689" spans="1:4">
+      <c r="A689" s="14">
+        <v>688</v>
+      </c>
+      <c r="B689" s="4" t="s">
+        <v>3868</v>
+      </c>
+      <c r="C689" s="17" t="s">
+        <v>3869</v>
+      </c>
+      <c r="D689" s="24" t="s">
+        <v>3927</v>
+      </c>
+    </row>
+    <row r="690" spans="1:4">
+      <c r="A690" s="14">
+        <v>689</v>
+      </c>
+      <c r="B690" s="4" t="s">
+        <v>3870</v>
+      </c>
+      <c r="C690" s="17" t="s">
+        <v>3871</v>
+      </c>
+      <c r="D690" s="24" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="691" spans="1:4">
+      <c r="A691" s="14">
+        <v>690</v>
+      </c>
+      <c r="B691" s="4" t="s">
+        <v>3872</v>
+      </c>
+      <c r="C691" s="17" t="s">
+        <v>3873</v>
+      </c>
+      <c r="D691" s="24" t="s">
+        <v>3929</v>
+      </c>
+    </row>
+    <row r="692" spans="1:4">
+      <c r="A692" s="14">
+        <v>691</v>
+      </c>
+      <c r="B692" s="4" t="s">
+        <v>3874</v>
+      </c>
+      <c r="C692" s="17" t="s">
+        <v>3875</v>
+      </c>
+      <c r="D692" s="24" t="s">
+        <v>3930</v>
+      </c>
+    </row>
+    <row r="693" spans="1:4">
+      <c r="A693" s="14">
+        <v>692</v>
+      </c>
+      <c r="B693" s="4" t="s">
+        <v>3876</v>
+      </c>
+      <c r="C693" s="17" t="s">
+        <v>3877</v>
+      </c>
+      <c r="D693" s="24" t="s">
+        <v>3931</v>
+      </c>
+    </row>
+    <row r="694" spans="1:4">
+      <c r="A694" s="14">
+        <v>693</v>
+      </c>
+      <c r="B694" s="4" t="s">
+        <v>3878</v>
+      </c>
+      <c r="C694" s="17" t="s">
+        <v>3879</v>
+      </c>
+      <c r="D694" s="24" t="s">
+        <v>3932</v>
+      </c>
+    </row>
+    <row r="695" spans="1:4">
+      <c r="A695" s="14">
+        <v>694</v>
+      </c>
+      <c r="B695" s="4" t="s">
+        <v>3880</v>
+      </c>
+      <c r="C695" s="17" t="s">
+        <v>3881</v>
+      </c>
+      <c r="D695" s="24" t="s">
+        <v>3933</v>
+      </c>
+    </row>
+    <row r="696" spans="1:4">
+      <c r="A696" s="14">
+        <v>695</v>
+      </c>
+      <c r="B696" s="4" t="s">
+        <v>3882</v>
+      </c>
+      <c r="C696" s="17" t="s">
+        <v>3883</v>
+      </c>
+      <c r="D696" s="24" t="s">
+        <v>3934</v>
+      </c>
+    </row>
+    <row r="697" spans="1:4">
+      <c r="A697" s="14">
+        <v>696</v>
+      </c>
+      <c r="B697" s="4" t="s">
+        <v>3884</v>
+      </c>
+      <c r="C697" s="17" t="s">
+        <v>3885</v>
+      </c>
+      <c r="D697" s="24" t="s">
+        <v>3935</v>
+      </c>
+    </row>
+    <row r="698" spans="1:4">
+      <c r="A698" s="14">
+        <v>697</v>
+      </c>
+      <c r="B698" s="4" t="s">
+        <v>3886</v>
+      </c>
+      <c r="C698" s="17" t="s">
+        <v>3887</v>
+      </c>
+      <c r="D698" s="24" t="s">
+        <v>3936</v>
+      </c>
+    </row>
+    <row r="699" spans="1:4">
+      <c r="A699" s="14">
+        <v>698</v>
+      </c>
+      <c r="B699" s="4" t="s">
+        <v>3888</v>
+      </c>
+      <c r="C699" s="17" t="s">
+        <v>3889</v>
+      </c>
+      <c r="D699" s="24" t="s">
+        <v>3937</v>
+      </c>
+    </row>
+    <row r="700" spans="1:4">
+      <c r="A700" s="14">
+        <v>699</v>
+      </c>
+      <c r="B700" s="4" t="s">
+        <v>3890</v>
+      </c>
+      <c r="C700" s="17" t="s">
+        <v>3891</v>
+      </c>
+      <c r="D700" s="24" t="s">
+        <v>3938</v>
+      </c>
+    </row>
+    <row r="701" spans="1:4">
+      <c r="A701" s="14">
+        <v>700</v>
+      </c>
+      <c r="B701" s="4" t="s">
+        <v>3892</v>
+      </c>
+      <c r="C701" s="17" t="s">
+        <v>3893</v>
+      </c>
+      <c r="D701" s="24" t="s">
+        <v>3939</v>
+      </c>
+    </row>
+    <row r="702" spans="1:4">
+      <c r="A702" s="14">
+        <v>701</v>
+      </c>
+      <c r="B702" s="4" t="s">
+        <v>3894</v>
+      </c>
+      <c r="C702" s="17" t="s">
+        <v>3895</v>
+      </c>
+      <c r="D702" s="24" t="s">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="703" spans="1:4">
+      <c r="A703" s="14">
+        <v>702</v>
+      </c>
+      <c r="B703" s="4" t="s">
+        <v>3896</v>
+      </c>
+      <c r="C703" s="17" t="s">
+        <v>3897</v>
+      </c>
+      <c r="D703" s="24" t="s">
+        <v>3941</v>
+      </c>
+    </row>
+    <row r="704" spans="1:4">
+      <c r="A704" s="14">
+        <v>703</v>
+      </c>
+      <c r="B704" s="4" t="s">
+        <v>3898</v>
+      </c>
+      <c r="C704" s="17" t="s">
+        <v>3899</v>
+      </c>
+      <c r="D704" s="24" t="s">
+        <v>3942</v>
+      </c>
+    </row>
+    <row r="705" spans="1:4">
+      <c r="A705" s="14">
+        <v>704</v>
+      </c>
+      <c r="B705" s="4" t="s">
+        <v>3900</v>
+      </c>
+      <c r="C705" s="17" t="s">
+        <v>3901</v>
+      </c>
+      <c r="D705" s="24" t="s">
+        <v>3943</v>
+      </c>
+    </row>
+    <row r="706" spans="1:4">
+      <c r="A706" s="14">
+        <v>705</v>
+      </c>
+      <c r="B706" s="4" t="s">
+        <v>3902</v>
+      </c>
+      <c r="C706" s="17" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D706" s="24" t="s">
+        <v>3944</v>
+      </c>
+    </row>
+    <row r="707" spans="1:4">
+      <c r="A707" s="14">
+        <v>706</v>
+      </c>
+      <c r="B707" s="4" t="s">
+        <v>3904</v>
+      </c>
+      <c r="C707" s="17" t="s">
+        <v>3905</v>
+      </c>
+      <c r="D707" s="24" t="s">
+        <v>3945</v>
+      </c>
+    </row>
+    <row r="708" spans="1:4">
+      <c r="A708" s="14">
+        <v>707</v>
+      </c>
+      <c r="B708" s="4" t="s">
+        <v>3906</v>
+      </c>
+      <c r="C708" s="17" t="s">
+        <v>3907</v>
+      </c>
+      <c r="D708" s="24" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="709" spans="1:4">
+      <c r="A709" s="14">
+        <v>708</v>
+      </c>
+      <c r="B709" s="4" t="s">
+        <v>3908</v>
+      </c>
+      <c r="C709" s="17" t="s">
+        <v>3909</v>
+      </c>
+      <c r="D709" s="24" t="s">
+        <v>3947</v>
+      </c>
+    </row>
+    <row r="710" spans="1:4">
+      <c r="A710" s="14">
+        <v>709</v>
+      </c>
+      <c r="B710" s="4" t="s">
+        <v>3910</v>
+      </c>
+      <c r="C710" s="17" t="s">
+        <v>3911</v>
+      </c>
+      <c r="D710" s="24" t="s">
+        <v>3948</v>
+      </c>
+    </row>
+    <row r="711" spans="1:4">
+      <c r="A711" s="14">
+        <v>710</v>
+      </c>
+      <c r="B711" s="4" t="s">
+        <v>3912</v>
+      </c>
+      <c r="C711" s="17" t="s">
+        <v>3913</v>
+      </c>
+      <c r="D711" s="24" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="712" spans="1:4">
+      <c r="A712" s="14">
+        <v>711</v>
+      </c>
+      <c r="B712" s="4" t="s">
+        <v>3914</v>
+      </c>
+      <c r="C712" s="17" t="s">
+        <v>3915</v>
+      </c>
+      <c r="D712" s="24" t="s">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="713" spans="1:4">
+      <c r="A713" s="14">
+        <v>712</v>
+      </c>
+      <c r="B713" s="4" t="s">
+        <v>3955</v>
+      </c>
+      <c r="C713" s="17" t="s">
+        <v>3956</v>
+      </c>
+      <c r="D713" s="24" t="s">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="714" spans="1:4">
+      <c r="A714" s="14">
+        <v>713</v>
+      </c>
+      <c r="B714" s="4" t="s">
+        <v>3957</v>
+      </c>
+      <c r="C714" s="17" t="s">
+        <v>3958</v>
+      </c>
+      <c r="D714" s="24" t="s">
+        <v>3981</v>
+      </c>
+    </row>
+    <row r="715" spans="1:4">
+      <c r="A715" s="14">
+        <v>714</v>
+      </c>
+      <c r="B715" s="4" t="s">
+        <v>3959</v>
+      </c>
+      <c r="C715" s="17" t="s">
+        <v>3960</v>
+      </c>
+      <c r="D715" s="24" t="s">
+        <v>3982</v>
+      </c>
+    </row>
+    <row r="716" spans="1:4">
+      <c r="A716" s="14">
+        <v>715</v>
+      </c>
+      <c r="B716" s="4" t="s">
+        <v>3961</v>
+      </c>
+      <c r="C716" s="17" t="s">
+        <v>3220</v>
+      </c>
+      <c r="D716" s="24" t="s">
+        <v>3983</v>
+      </c>
+    </row>
+    <row r="717" spans="1:4">
+      <c r="A717" s="14">
+        <v>716</v>
+      </c>
+      <c r="B717" s="4" t="s">
+        <v>3962</v>
+      </c>
+      <c r="C717" s="17" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D717" s="24" t="s">
+        <v>3984</v>
+      </c>
+    </row>
+    <row r="718" spans="1:4">
+      <c r="A718" s="14">
+        <v>717</v>
+      </c>
+      <c r="B718" s="4" t="s">
+        <v>3964</v>
+      </c>
+      <c r="C718" s="17" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D718" s="24" t="s">
+        <v>3985</v>
+      </c>
+    </row>
+    <row r="719" spans="1:4">
+      <c r="A719" s="14">
+        <v>718</v>
+      </c>
+      <c r="B719" s="4" t="s">
+        <v>3966</v>
+      </c>
+      <c r="C719" s="17" t="s">
+        <v>3967</v>
+      </c>
+      <c r="D719" s="24" t="s">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="720" spans="1:4">
+      <c r="A720" s="14">
+        <v>719</v>
+      </c>
+      <c r="B720" s="4" t="s">
+        <v>3968</v>
+      </c>
+      <c r="C720" s="17" t="s">
+        <v>3969</v>
+      </c>
+      <c r="D720" s="24" t="s">
+        <v>3987</v>
+      </c>
+    </row>
+    <row r="721" spans="1:4">
+      <c r="A721" s="14">
+        <v>720</v>
+      </c>
+      <c r="B721" s="4" t="s">
+        <v>3970</v>
+      </c>
+      <c r="C721" s="17" t="s">
+        <v>3971</v>
+      </c>
+      <c r="D721" s="24" t="s">
+        <v>3988</v>
+      </c>
+    </row>
+    <row r="722" spans="1:4">
+      <c r="A722" s="14">
+        <v>721</v>
+      </c>
+      <c r="B722" s="4" t="s">
+        <v>3972</v>
+      </c>
+      <c r="C722" s="17" t="s">
+        <v>3973</v>
+      </c>
+      <c r="D722" s="24" t="s">
+        <v>3989</v>
+      </c>
+    </row>
+    <row r="723" spans="1:4">
+      <c r="A723" s="14">
+        <v>722</v>
+      </c>
+      <c r="B723" s="4" t="s">
+        <v>3974</v>
+      </c>
+      <c r="C723" s="17" t="s">
+        <v>3975</v>
+      </c>
+      <c r="D723" s="24" t="s">
+        <v>3990</v>
+      </c>
+    </row>
+    <row r="724" spans="1:4">
+      <c r="A724" s="14">
+        <v>723</v>
+      </c>
+      <c r="B724" s="4" t="s">
+        <v>3976</v>
+      </c>
+      <c r="C724" s="17" t="s">
+        <v>3977</v>
+      </c>
+      <c r="D724" s="24" t="s">
+        <v>3991</v>
+      </c>
+    </row>
+    <row r="725" spans="1:4">
+      <c r="A725" s="14">
+        <v>724</v>
+      </c>
+      <c r="B725" s="4" t="s">
+        <v>3978</v>
+      </c>
+      <c r="C725" s="17" t="s">
+        <v>3979</v>
+      </c>
+      <c r="D725" s="24" t="s">
+        <v>3992</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -32676,10 +33844,10 @@
         <v>3429</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>3770</v>
+        <v>3766</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>3775</v>
+        <v>3771</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
@@ -32696,10 +33864,10 @@
         <v>3429</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>3771</v>
+        <v>3767</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>3776</v>
+        <v>3772</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -32716,10 +33884,10 @@
         <v>3429</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>3772</v>
+        <v>3768</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>3777</v>
+        <v>3773</v>
       </c>
       <c r="E45" s="1">
         <v>2</v>
@@ -32736,7 +33904,7 @@
         <v>3429</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>3773</v>
+        <v>3769</v>
       </c>
       <c r="D46" s="24" t="s">
         <v>3079</v>
@@ -32756,10 +33924,10 @@
         <v>3429</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>3771</v>
+        <v>3767</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>3776</v>
+        <v>3772</v>
       </c>
       <c r="E47" s="1">
         <v>4</v>
@@ -32767,7 +33935,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1" t="s">
-        <v>3779</v>
+        <v>3775</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -32778,10 +33946,10 @@
         <v>3429</v>
       </c>
       <c r="C48" s="8" t="s">
+        <v>3770</v>
+      </c>
+      <c r="D48" s="24" t="s">
         <v>3774</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>3778</v>
       </c>
       <c r="E48" s="1">
         <v>5</v>
@@ -32798,10 +33966,10 @@
         <v>3471</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>3768</v>
+        <v>3764</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>3769</v>
+        <v>3765</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
@@ -32855,13 +34023,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>3743</v>
+        <v>3739</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>3744</v>
+        <v>3740</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>3751</v>
+        <v>3747</v>
       </c>
       <c r="E52" s="1">
         <v>1</v>
@@ -32875,13 +34043,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>3743</v>
+        <v>3739</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>3745</v>
+        <v>3741</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>3748</v>
+        <v>3744</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
@@ -32895,13 +34063,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>3743</v>
+        <v>3739</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>3746</v>
+        <v>3742</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>3749</v>
+        <v>3745</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -32915,13 +34083,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>3739</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>3743</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>3747</v>
-      </c>
       <c r="D55" s="24" t="s">
-        <v>3750</v>
+        <v>3746</v>
       </c>
       <c r="E55" s="1">
         <v>4</v>
@@ -32935,7 +34103,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>3754</v>
+        <v>3750</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>2703</v>
@@ -32955,13 +34123,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>3754</v>
+        <v>3750</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>3755</v>
+        <v>3751</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>3756</v>
+        <v>3752</v>
       </c>
       <c r="E57" s="1">
         <v>1</v>
@@ -33042,7 +34210,7 @@
         <v>1832</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>3611</v>
+        <v>3609</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>1881</v>
@@ -33074,7 +34242,7 @@
         <v>1882</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>3830</v>
+        <v>3826</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="8" t="s">
@@ -33094,13 +34262,13 @@
         <v>1813</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>3612</v>
+        <v>3610</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>1883</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>3831</v>
+        <v>3827</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="8" t="s">
@@ -33120,13 +34288,13 @@
         <v>1814</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>3613</v>
+        <v>3611</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>1884</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>3832</v>
+        <v>3828</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="8" t="s">
@@ -33148,7 +34316,7 @@
         <v>1815</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>3614</v>
+        <v>3612</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>1885</v>
@@ -33176,7 +34344,7 @@
         <v>1833</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>3615</v>
+        <v>3613</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>1886</v>
@@ -33204,7 +34372,7 @@
         <v>1816</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>3616</v>
+        <v>3614</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>1887</v>
@@ -33232,7 +34400,7 @@
         <v>1817</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>3617</v>
+        <v>3615</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>1888</v>
@@ -33288,7 +34456,7 @@
         <v>1818</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>3618</v>
+        <v>3616</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>1890</v>
@@ -33316,7 +34484,7 @@
         <v>1819</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>3619</v>
+        <v>3617</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>1891</v>
@@ -33344,7 +34512,7 @@
         <v>1820</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>3620</v>
+        <v>3618</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>1892</v>
@@ -33372,7 +34540,7 @@
         <v>1821</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>3621</v>
+        <v>3619</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>1893</v>
@@ -33400,7 +34568,7 @@
         <v>1822</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>3622</v>
+        <v>3620</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>1894</v>
@@ -33428,7 +34596,7 @@
         <v>1823</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>3623</v>
+        <v>3621</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>1895</v>
@@ -33456,7 +34624,7 @@
         <v>1824</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>3624</v>
+        <v>3622</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>1896</v>
@@ -33484,7 +34652,7 @@
         <v>1825</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>3625</v>
+        <v>3623</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>1897</v>
@@ -33512,7 +34680,7 @@
         <v>1835</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>3626</v>
+        <v>3624</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>1898</v>
@@ -33540,7 +34708,7 @@
         <v>1826</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>3627</v>
+        <v>3625</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>1899</v>
@@ -33568,7 +34736,7 @@
         <v>1836</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>3628</v>
+        <v>3626</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>1895</v>
@@ -33596,7 +34764,7 @@
         <v>1827</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>3629</v>
+        <v>3627</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>1900</v>
@@ -33624,7 +34792,7 @@
         <v>1828</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>3630</v>
+        <v>3628</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>1901</v>
@@ -33652,7 +34820,7 @@
         <v>1838</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>3631</v>
+        <v>3629</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>1902</v>
@@ -33680,7 +34848,7 @@
         <v>1986</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>3632</v>
+        <v>3630</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>1903</v>
@@ -33708,7 +34876,7 @@
         <v>1985</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>3633</v>
+        <v>3631</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="24"/>
@@ -33732,7 +34900,7 @@
         <v>1983</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>3634</v>
+        <v>3632</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>1904</v>
@@ -33760,7 +34928,7 @@
         <v>1984</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>3635</v>
+        <v>3633</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="24"/>
@@ -33784,7 +34952,7 @@
         <v>1829</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>3636</v>
+        <v>3634</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>1905</v>
@@ -33812,7 +34980,7 @@
         <v>1830</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>3637</v>
+        <v>3635</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="24"/>
@@ -33836,7 +35004,7 @@
         <v>1831</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>3638</v>
+        <v>3636</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="24"/>
@@ -33878,10 +35046,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -33984,10 +35152,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3786</v>
+        <v>3782</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>3787</v>
+        <v>3783</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -34109,6 +35277,17 @@
       </c>
       <c r="C20" s="24" t="s">
         <v>3217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="14">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3844</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>3845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimization of the operation and maintenance module and adjustment of the documentation
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2657F6-E374-4CC1-824D-160486B55491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E97B24-9581-4A4C-B74F-C5791E87D356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14779,26 +14779,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>抽稀记录数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>vacuateSaveIntervalWaveRange</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>抽稀数据保存周期波动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>vacuateSaveInterval</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>抽稀数据保存间隔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>vacuateThreshold</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -14929,15 +14917,6 @@
     <t>Data sparseness</t>
   </si>
   <si>
-    <t>Number of sparse records</t>
-  </si>
-  <si>
-    <t>The storage period of sampling data fluctuates</t>
-  </si>
-  <si>
-    <t>Sampling data storage interval</t>
-  </si>
-  <si>
     <t>The number of records when the sparse table is enabled</t>
   </si>
   <si>
@@ -15131,6 +15110,27 @@
   <si>
     <t>Structural backup and recovery</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记录数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存盘周期波动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存盘周期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of records</t>
+  </si>
+  <si>
+    <t>The deposit cycle fluctuates</t>
+  </si>
+  <si>
+    <t>Storage period</t>
   </si>
 </sst>
 </file>
@@ -17413,10 +17413,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>3947</v>
+        <v>3941</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>3949</v>
+        <v>3943</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -17427,10 +17427,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>3948</v>
+        <v>3942</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>3950</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -22804,8 +22804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
   <dimension ref="A1:D725"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A666" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D679" sqref="D679"/>
+    <sheetView tabSelected="1" topLeftCell="A684" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D702" sqref="D702:D704"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -32301,10 +32301,10 @@
         <v>3846</v>
       </c>
       <c r="C678" s="17" t="s">
-        <v>3990</v>
+        <v>3984</v>
       </c>
       <c r="D678" s="24" t="s">
-        <v>3989</v>
+        <v>3983</v>
       </c>
     </row>
     <row r="679" spans="1:4">
@@ -32315,10 +32315,10 @@
         <v>3847</v>
       </c>
       <c r="C679" s="17" t="s">
-        <v>3991</v>
+        <v>3985</v>
       </c>
       <c r="D679" s="24" t="s">
-        <v>3992</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="680" spans="1:4">
@@ -32332,7 +32332,7 @@
         <v>3849</v>
       </c>
       <c r="D680" s="24" t="s">
-        <v>3914</v>
+        <v>3911</v>
       </c>
     </row>
     <row r="681" spans="1:4">
@@ -32346,7 +32346,7 @@
         <v>3851</v>
       </c>
       <c r="D681" s="24" t="s">
-        <v>3915</v>
+        <v>3912</v>
       </c>
     </row>
     <row r="682" spans="1:4">
@@ -32360,7 +32360,7 @@
         <v>3853</v>
       </c>
       <c r="D682" s="24" t="s">
-        <v>3916</v>
+        <v>3913</v>
       </c>
     </row>
     <row r="683" spans="1:4">
@@ -32374,7 +32374,7 @@
         <v>3855</v>
       </c>
       <c r="D683" s="24" t="s">
-        <v>3917</v>
+        <v>3914</v>
       </c>
     </row>
     <row r="684" spans="1:4">
@@ -32388,7 +32388,7 @@
         <v>3857</v>
       </c>
       <c r="D684" s="24" t="s">
-        <v>3918</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="685" spans="1:4">
@@ -32402,7 +32402,7 @@
         <v>3859</v>
       </c>
       <c r="D685" s="24" t="s">
-        <v>3919</v>
+        <v>3916</v>
       </c>
     </row>
     <row r="686" spans="1:4">
@@ -32416,7 +32416,7 @@
         <v>3861</v>
       </c>
       <c r="D686" s="24" t="s">
-        <v>3920</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="687" spans="1:4">
@@ -32430,7 +32430,7 @@
         <v>3863</v>
       </c>
       <c r="D687" s="24" t="s">
-        <v>3921</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="688" spans="1:4">
@@ -32444,7 +32444,7 @@
         <v>3865</v>
       </c>
       <c r="D688" s="24" t="s">
-        <v>3922</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="689" spans="1:4">
@@ -32458,7 +32458,7 @@
         <v>3867</v>
       </c>
       <c r="D689" s="24" t="s">
-        <v>3923</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="690" spans="1:4">
@@ -32472,7 +32472,7 @@
         <v>3869</v>
       </c>
       <c r="D690" s="24" t="s">
-        <v>3924</v>
+        <v>3921</v>
       </c>
     </row>
     <row r="691" spans="1:4">
@@ -32486,7 +32486,7 @@
         <v>3871</v>
       </c>
       <c r="D691" s="24" t="s">
-        <v>3925</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="692" spans="1:4">
@@ -32500,7 +32500,7 @@
         <v>3873</v>
       </c>
       <c r="D692" s="24" t="s">
-        <v>3926</v>
+        <v>3923</v>
       </c>
     </row>
     <row r="693" spans="1:4">
@@ -32514,7 +32514,7 @@
         <v>3875</v>
       </c>
       <c r="D693" s="24" t="s">
-        <v>3927</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="694" spans="1:4">
@@ -32528,7 +32528,7 @@
         <v>3877</v>
       </c>
       <c r="D694" s="24" t="s">
-        <v>3928</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="695" spans="1:4">
@@ -32542,7 +32542,7 @@
         <v>3879</v>
       </c>
       <c r="D695" s="24" t="s">
-        <v>3929</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="696" spans="1:4">
@@ -32556,7 +32556,7 @@
         <v>3881</v>
       </c>
       <c r="D696" s="24" t="s">
-        <v>3930</v>
+        <v>3927</v>
       </c>
     </row>
     <row r="697" spans="1:4">
@@ -32570,7 +32570,7 @@
         <v>3883</v>
       </c>
       <c r="D697" s="24" t="s">
-        <v>3931</v>
+        <v>3928</v>
       </c>
     </row>
     <row r="698" spans="1:4">
@@ -32584,7 +32584,7 @@
         <v>3885</v>
       </c>
       <c r="D698" s="24" t="s">
-        <v>3932</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="699" spans="1:4">
@@ -32598,7 +32598,7 @@
         <v>3887</v>
       </c>
       <c r="D699" s="24" t="s">
-        <v>3933</v>
+        <v>3930</v>
       </c>
     </row>
     <row r="700" spans="1:4">
@@ -32612,7 +32612,7 @@
         <v>3889</v>
       </c>
       <c r="D700" s="24" t="s">
-        <v>3934</v>
+        <v>3931</v>
       </c>
     </row>
     <row r="701" spans="1:4">
@@ -32626,7 +32626,7 @@
         <v>3891</v>
       </c>
       <c r="D701" s="24" t="s">
-        <v>3935</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="702" spans="1:4">
@@ -32637,10 +32637,10 @@
         <v>3892</v>
       </c>
       <c r="C702" s="17" t="s">
-        <v>3893</v>
+        <v>3987</v>
       </c>
       <c r="D702" s="24" t="s">
-        <v>3936</v>
+        <v>3990</v>
       </c>
     </row>
     <row r="703" spans="1:4">
@@ -32648,13 +32648,13 @@
         <v>702</v>
       </c>
       <c r="B703" s="4" t="s">
-        <v>3894</v>
+        <v>3893</v>
       </c>
       <c r="C703" s="17" t="s">
-        <v>3895</v>
+        <v>3988</v>
       </c>
       <c r="D703" s="24" t="s">
-        <v>3937</v>
+        <v>3991</v>
       </c>
     </row>
     <row r="704" spans="1:4">
@@ -32662,13 +32662,13 @@
         <v>703</v>
       </c>
       <c r="B704" s="4" t="s">
-        <v>3896</v>
+        <v>3894</v>
       </c>
       <c r="C704" s="17" t="s">
-        <v>3897</v>
+        <v>3989</v>
       </c>
       <c r="D704" s="24" t="s">
-        <v>3938</v>
+        <v>3992</v>
       </c>
     </row>
     <row r="705" spans="1:4">
@@ -32676,13 +32676,13 @@
         <v>704</v>
       </c>
       <c r="B705" s="4" t="s">
-        <v>3898</v>
+        <v>3895</v>
       </c>
       <c r="C705" s="17" t="s">
-        <v>3899</v>
+        <v>3896</v>
       </c>
       <c r="D705" s="24" t="s">
-        <v>3939</v>
+        <v>3933</v>
       </c>
     </row>
     <row r="706" spans="1:4">
@@ -32690,13 +32690,13 @@
         <v>705</v>
       </c>
       <c r="B706" s="4" t="s">
-        <v>3900</v>
+        <v>3897</v>
       </c>
       <c r="C706" s="17" t="s">
-        <v>3901</v>
+        <v>3898</v>
       </c>
       <c r="D706" s="24" t="s">
-        <v>3940</v>
+        <v>3934</v>
       </c>
     </row>
     <row r="707" spans="1:4">
@@ -32704,13 +32704,13 @@
         <v>706</v>
       </c>
       <c r="B707" s="4" t="s">
-        <v>3902</v>
+        <v>3899</v>
       </c>
       <c r="C707" s="17" t="s">
-        <v>3903</v>
+        <v>3900</v>
       </c>
       <c r="D707" s="24" t="s">
-        <v>3941</v>
+        <v>3935</v>
       </c>
     </row>
     <row r="708" spans="1:4">
@@ -32718,13 +32718,13 @@
         <v>707</v>
       </c>
       <c r="B708" s="4" t="s">
-        <v>3904</v>
+        <v>3901</v>
       </c>
       <c r="C708" s="17" t="s">
-        <v>3905</v>
+        <v>3902</v>
       </c>
       <c r="D708" s="24" t="s">
-        <v>3942</v>
+        <v>3936</v>
       </c>
     </row>
     <row r="709" spans="1:4">
@@ -32732,13 +32732,13 @@
         <v>708</v>
       </c>
       <c r="B709" s="4" t="s">
-        <v>3906</v>
+        <v>3903</v>
       </c>
       <c r="C709" s="17" t="s">
-        <v>3907</v>
+        <v>3904</v>
       </c>
       <c r="D709" s="24" t="s">
-        <v>3943</v>
+        <v>3937</v>
       </c>
     </row>
     <row r="710" spans="1:4">
@@ -32746,13 +32746,13 @@
         <v>709</v>
       </c>
       <c r="B710" s="4" t="s">
-        <v>3908</v>
+        <v>3905</v>
       </c>
       <c r="C710" s="17" t="s">
-        <v>3909</v>
+        <v>3906</v>
       </c>
       <c r="D710" s="24" t="s">
-        <v>3944</v>
+        <v>3938</v>
       </c>
     </row>
     <row r="711" spans="1:4">
@@ -32760,13 +32760,13 @@
         <v>710</v>
       </c>
       <c r="B711" s="4" t="s">
-        <v>3910</v>
+        <v>3907</v>
       </c>
       <c r="C711" s="17" t="s">
-        <v>3911</v>
+        <v>3908</v>
       </c>
       <c r="D711" s="24" t="s">
-        <v>3945</v>
+        <v>3939</v>
       </c>
     </row>
     <row r="712" spans="1:4">
@@ -32774,13 +32774,13 @@
         <v>711</v>
       </c>
       <c r="B712" s="4" t="s">
-        <v>3912</v>
+        <v>3909</v>
       </c>
       <c r="C712" s="17" t="s">
-        <v>3913</v>
+        <v>3910</v>
       </c>
       <c r="D712" s="24" t="s">
-        <v>3946</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="713" spans="1:4">
@@ -32788,13 +32788,13 @@
         <v>712</v>
       </c>
       <c r="B713" s="4" t="s">
-        <v>3951</v>
+        <v>3945</v>
       </c>
       <c r="C713" s="17" t="s">
-        <v>3952</v>
+        <v>3946</v>
       </c>
       <c r="D713" s="24" t="s">
-        <v>3976</v>
+        <v>3970</v>
       </c>
     </row>
     <row r="714" spans="1:4">
@@ -32802,13 +32802,13 @@
         <v>713</v>
       </c>
       <c r="B714" s="4" t="s">
-        <v>3953</v>
+        <v>3947</v>
       </c>
       <c r="C714" s="17" t="s">
-        <v>3954</v>
+        <v>3948</v>
       </c>
       <c r="D714" s="24" t="s">
-        <v>3977</v>
+        <v>3971</v>
       </c>
     </row>
     <row r="715" spans="1:4">
@@ -32816,13 +32816,13 @@
         <v>714</v>
       </c>
       <c r="B715" s="4" t="s">
-        <v>3955</v>
+        <v>3949</v>
       </c>
       <c r="C715" s="17" t="s">
-        <v>3956</v>
+        <v>3950</v>
       </c>
       <c r="D715" s="24" t="s">
-        <v>3978</v>
+        <v>3972</v>
       </c>
     </row>
     <row r="716" spans="1:4">
@@ -32830,13 +32830,13 @@
         <v>715</v>
       </c>
       <c r="B716" s="4" t="s">
-        <v>3957</v>
+        <v>3951</v>
       </c>
       <c r="C716" s="17" t="s">
         <v>3220</v>
       </c>
       <c r="D716" s="24" t="s">
-        <v>3979</v>
+        <v>3973</v>
       </c>
     </row>
     <row r="717" spans="1:4">
@@ -32844,13 +32844,13 @@
         <v>716</v>
       </c>
       <c r="B717" s="4" t="s">
-        <v>3958</v>
+        <v>3952</v>
       </c>
       <c r="C717" s="17" t="s">
-        <v>3959</v>
+        <v>3953</v>
       </c>
       <c r="D717" s="24" t="s">
-        <v>3980</v>
+        <v>3974</v>
       </c>
     </row>
     <row r="718" spans="1:4">
@@ -32858,13 +32858,13 @@
         <v>717</v>
       </c>
       <c r="B718" s="4" t="s">
-        <v>3960</v>
+        <v>3954</v>
       </c>
       <c r="C718" s="17" t="s">
-        <v>3961</v>
+        <v>3955</v>
       </c>
       <c r="D718" s="24" t="s">
-        <v>3981</v>
+        <v>3975</v>
       </c>
     </row>
     <row r="719" spans="1:4">
@@ -32872,13 +32872,13 @@
         <v>718</v>
       </c>
       <c r="B719" s="4" t="s">
-        <v>3962</v>
+        <v>3956</v>
       </c>
       <c r="C719" s="17" t="s">
-        <v>3963</v>
+        <v>3957</v>
       </c>
       <c r="D719" s="24" t="s">
-        <v>3982</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="720" spans="1:4">
@@ -32886,13 +32886,13 @@
         <v>719</v>
       </c>
       <c r="B720" s="4" t="s">
-        <v>3964</v>
+        <v>3958</v>
       </c>
       <c r="C720" s="17" t="s">
-        <v>3965</v>
+        <v>3959</v>
       </c>
       <c r="D720" s="24" t="s">
-        <v>3983</v>
+        <v>3977</v>
       </c>
     </row>
     <row r="721" spans="1:4">
@@ -32900,13 +32900,13 @@
         <v>720</v>
       </c>
       <c r="B721" s="4" t="s">
-        <v>3966</v>
+        <v>3960</v>
       </c>
       <c r="C721" s="17" t="s">
-        <v>3967</v>
+        <v>3961</v>
       </c>
       <c r="D721" s="24" t="s">
-        <v>3984</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="722" spans="1:4">
@@ -32914,13 +32914,13 @@
         <v>721</v>
       </c>
       <c r="B722" s="4" t="s">
-        <v>3968</v>
+        <v>3962</v>
       </c>
       <c r="C722" s="17" t="s">
-        <v>3969</v>
+        <v>3963</v>
       </c>
       <c r="D722" s="24" t="s">
-        <v>3985</v>
+        <v>3979</v>
       </c>
     </row>
     <row r="723" spans="1:4">
@@ -32928,13 +32928,13 @@
         <v>722</v>
       </c>
       <c r="B723" s="4" t="s">
-        <v>3970</v>
+        <v>3964</v>
       </c>
       <c r="C723" s="17" t="s">
-        <v>3971</v>
+        <v>3965</v>
       </c>
       <c r="D723" s="24" t="s">
-        <v>3986</v>
+        <v>3980</v>
       </c>
     </row>
     <row r="724" spans="1:4">
@@ -32942,13 +32942,13 @@
         <v>723</v>
       </c>
       <c r="B724" s="4" t="s">
-        <v>3972</v>
+        <v>3966</v>
       </c>
       <c r="C724" s="17" t="s">
-        <v>3973</v>
+        <v>3967</v>
       </c>
       <c r="D724" s="24" t="s">
-        <v>3987</v>
+        <v>3981</v>
       </c>
     </row>
     <row r="725" spans="1:4">
@@ -32956,13 +32956,13 @@
         <v>724</v>
       </c>
       <c r="B725" s="4" t="s">
-        <v>3974</v>
+        <v>3968</v>
       </c>
       <c r="C725" s="17" t="s">
-        <v>3975</v>
+        <v>3969</v>
       </c>
       <c r="D725" s="24" t="s">
-        <v>3988</v>
+        <v>3982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Detail optimization and memory curve adjustment
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697A56DE-CEAA-422F-B5AA-1B8A4917EBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57060F29-1863-4F43-873E-4160475F4AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4222" uniqueCount="3996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4228" uniqueCount="4002">
   <si>
     <t>myself</t>
   </si>
@@ -15143,6 +15143,28 @@
   <si>
     <t>Basic information</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oemConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OEM配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collisionDevice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲突的设备</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OEM configuration</t>
+  </si>
+  <si>
+    <t>Conflicting equipment</t>
   </si>
 </sst>
 </file>
@@ -22814,10 +22836,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D726"/>
+  <dimension ref="A1:D728"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A708" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D733" sqref="D733"/>
+      <selection activeCell="D735" sqref="D735"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -32989,6 +33011,34 @@
       </c>
       <c r="D726" s="24" t="s">
         <v>3995</v>
+      </c>
+    </row>
+    <row r="727" spans="1:4">
+      <c r="A727" s="14">
+        <v>726</v>
+      </c>
+      <c r="B727" s="4" t="s">
+        <v>3996</v>
+      </c>
+      <c r="C727" s="17" t="s">
+        <v>3997</v>
+      </c>
+      <c r="D727" s="24" t="s">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="728" spans="1:4">
+      <c r="A728" s="14">
+        <v>727</v>
+      </c>
+      <c r="B728" s="4" t="s">
+        <v>3998</v>
+      </c>
+      <c r="C728" s="17" t="s">
+        <v>3999</v>
+      </c>
+      <c r="D728" s="24" t="s">
+        <v>4001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Function optimization and improvement of memory monitoring curve
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57060F29-1863-4F43-873E-4160475F4AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD7A2D6-6890-4038-8B32-D8535C7050F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4228" uniqueCount="4002">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4252" uniqueCount="4024">
   <si>
     <t>myself</t>
   </si>
@@ -15165,6 +15165,87 @@
   </si>
   <si>
     <t>Conflicting equipment</t>
+  </si>
+  <si>
+    <t>affiliatedOrg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memoryCurve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内存曲线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>totalMemoryUsage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总内存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tomcatPhysicalMemory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tomcat物理内存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JVMMemory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JVM内存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JVMHeapMemory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JVM堆内存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JVMNonHeapMemory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JVM非堆内存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oraclePhysicalMemory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库物理内存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memory curve</t>
+  </si>
+  <si>
+    <t>Total memory</t>
+  </si>
+  <si>
+    <t>Tomcat physical memory</t>
+  </si>
+  <si>
+    <t>JVM memory</t>
+  </si>
+  <si>
+    <t>JVM heap memory</t>
+  </si>
+  <si>
+    <t>JVM is not heap memory</t>
+  </si>
+  <si>
+    <t>Database physical memory</t>
   </si>
 </sst>
 </file>
@@ -22836,10 +22917,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D728"/>
+  <dimension ref="A1:D739"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A708" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D735" sqref="D735"/>
+    <sheetView tabSelected="1" topLeftCell="A705" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D739" sqref="D739"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -33040,6 +33121,136 @@
       <c r="D728" s="24" t="s">
         <v>4001</v>
       </c>
+    </row>
+    <row r="729" spans="1:4">
+      <c r="A729" s="14">
+        <v>728</v>
+      </c>
+      <c r="B729" s="4" t="s">
+        <v>4002</v>
+      </c>
+      <c r="C729" s="17" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D729" s="24" t="s">
+        <v>3322</v>
+      </c>
+    </row>
+    <row r="730" spans="1:4">
+      <c r="A730" s="14">
+        <v>729</v>
+      </c>
+      <c r="B730" s="4" t="s">
+        <v>4003</v>
+      </c>
+      <c r="C730" s="17" t="s">
+        <v>4004</v>
+      </c>
+      <c r="D730" s="24" t="s">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="731" spans="1:4">
+      <c r="A731" s="14">
+        <v>730</v>
+      </c>
+      <c r="B731" s="4" t="s">
+        <v>4005</v>
+      </c>
+      <c r="C731" s="17" t="s">
+        <v>4006</v>
+      </c>
+      <c r="D731" s="24" t="s">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="732" spans="1:4">
+      <c r="A732" s="14">
+        <v>731</v>
+      </c>
+      <c r="B732" s="4" t="s">
+        <v>4007</v>
+      </c>
+      <c r="C732" s="17" t="s">
+        <v>4008</v>
+      </c>
+      <c r="D732" s="24" t="s">
+        <v>4019</v>
+      </c>
+    </row>
+    <row r="733" spans="1:4">
+      <c r="A733" s="14">
+        <v>732</v>
+      </c>
+      <c r="B733" s="4" t="s">
+        <v>4009</v>
+      </c>
+      <c r="C733" s="17" t="s">
+        <v>4010</v>
+      </c>
+      <c r="D733" s="24" t="s">
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="734" spans="1:4">
+      <c r="A734" s="14">
+        <v>733</v>
+      </c>
+      <c r="B734" s="4" t="s">
+        <v>4011</v>
+      </c>
+      <c r="C734" s="17" t="s">
+        <v>4012</v>
+      </c>
+      <c r="D734" s="24" t="s">
+        <v>4021</v>
+      </c>
+    </row>
+    <row r="735" spans="1:4">
+      <c r="A735" s="14">
+        <v>734</v>
+      </c>
+      <c r="B735" s="4" t="s">
+        <v>4013</v>
+      </c>
+      <c r="C735" s="17" t="s">
+        <v>4014</v>
+      </c>
+      <c r="D735" s="24" t="s">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="736" spans="1:4">
+      <c r="A736" s="14">
+        <v>735</v>
+      </c>
+      <c r="B736" s="4" t="s">
+        <v>4015</v>
+      </c>
+      <c r="C736" s="17" t="s">
+        <v>4016</v>
+      </c>
+      <c r="D736" s="24" t="s">
+        <v>4023</v>
+      </c>
+    </row>
+    <row r="737" spans="1:4">
+      <c r="A737" s="14"/>
+      <c r="B737" s="4"/>
+      <c r="C737" s="17"/>
+      <c r="D737" s="24"/>
+    </row>
+    <row r="738" spans="1:4">
+      <c r="A738" s="14"/>
+      <c r="B738" s="4"/>
+      <c r="C738" s="17"/>
+      <c r="D738" s="24"/>
+    </row>
+    <row r="739" spans="1:4">
+      <c r="A739" s="14"/>
+      <c r="B739" s="4"/>
+      <c r="C739" s="17"/>
+      <c r="D739" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -35378,8 +35589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Adjust the control window
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD7A2D6-6890-4038-8B32-D8535C7050F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103CC6CB-73FD-400F-B9AC-3EBD11386036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4252" uniqueCount="4024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4258" uniqueCount="4029">
   <si>
     <t>myself</t>
   </si>
@@ -15246,6 +15246,26 @@
   </si>
   <si>
     <t>Database physical memory</t>
+  </si>
+  <si>
+    <t>批量下行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Downlink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batch down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>downwardCommand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batchDownwardCommand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -22919,8 +22939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
   <dimension ref="A1:D739"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A705" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D739" sqref="D739"/>
+    <sheetView tabSelected="1" topLeftCell="A707" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B742" sqref="B742"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -33235,16 +33255,32 @@
       </c>
     </row>
     <row r="737" spans="1:4">
-      <c r="A737" s="14"/>
-      <c r="B737" s="4"/>
-      <c r="C737" s="17"/>
-      <c r="D737" s="24"/>
+      <c r="A737" s="14">
+        <v>736</v>
+      </c>
+      <c r="B737" s="4" t="s">
+        <v>4027</v>
+      </c>
+      <c r="C737" s="17" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D737" s="17" t="s">
+        <v>4025</v>
+      </c>
     </row>
     <row r="738" spans="1:4">
-      <c r="A738" s="14"/>
-      <c r="B738" s="4"/>
-      <c r="C738" s="17"/>
-      <c r="D738" s="24"/>
+      <c r="A738" s="14">
+        <v>737</v>
+      </c>
+      <c r="B738" s="4" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C738" s="17" t="s">
+        <v>4024</v>
+      </c>
+      <c r="D738" s="17" t="s">
+        <v>4026</v>
+      </c>
     </row>
     <row r="739" spans="1:4">
       <c r="A739" s="14"/>

</xml_diff>

<commit_message>
Adjustment of tab maintenance function
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5010C4D-0FC7-4727-9ED3-8193957E6192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195A3707-BCEE-4E4B-9F17-077407F7915C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294" uniqueCount="4065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4297" uniqueCount="4068">
   <si>
     <t>myself</t>
   </si>
@@ -15411,6 +15411,18 @@
   </si>
   <si>
     <t>The role is associated with information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tagManagement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标签管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tag management</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -23086,7 +23098,7 @@
   <dimension ref="A1:D761"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A723" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C755" sqref="C755"/>
+      <selection activeCell="C756" sqref="C756"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -33597,10 +33609,18 @@
       </c>
     </row>
     <row r="751" spans="1:4">
-      <c r="A751" s="14"/>
-      <c r="B751" s="4"/>
-      <c r="C751" s="17"/>
-      <c r="D751" s="24"/>
+      <c r="A751" s="14">
+        <v>750</v>
+      </c>
+      <c r="B751" s="4" t="s">
+        <v>4065</v>
+      </c>
+      <c r="C751" s="17" t="s">
+        <v>4066</v>
+      </c>
+      <c r="D751" s="24" t="s">
+        <v>4067</v>
+      </c>
     </row>
     <row r="752" spans="1:4">
       <c r="A752" s="14"/>

</xml_diff>

<commit_message>
Detailed optimization and adjustment
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D12F3F-D6A2-42AC-94B7-0E1E4AC7CAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F01AE4F-B277-42D4-B1A9-D96F3890D9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14621,10 +14621,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>打印日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>exportDataLimits</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -14839,9 +14835,6 @@
     <t>Simulate data sending cycles</t>
   </si>
   <si>
-    <t>Print logs</t>
-  </si>
-  <si>
     <t>Export data limits</t>
   </si>
   <si>
@@ -15426,14 +15419,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>打印通信服务交互日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Print the communication service interaction log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>printAdLogs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -15442,12 +15427,25 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>打印异常信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Print the exception information</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>打印调试日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打印交互日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打印异常日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Print the debug log</t>
+  </si>
+  <si>
+    <t>Print the interaction log</t>
+  </si>
+  <si>
+    <t>Print the exception log</t>
   </si>
 </sst>
 </file>
@@ -17730,10 +17728,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>4017</v>
+        <v>4015</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4018</v>
+        <v>4016</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -17744,10 +17742,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>4019</v>
+        <v>4017</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4020</v>
+        <v>4018</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -23122,7 +23120,7 @@
   <dimension ref="A1:D763"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A672" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D690" sqref="D690"/>
+      <selection activeCell="D688" sqref="D688:D690"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -25856,10 +25854,10 @@
         <v>183</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>4021</v>
+        <v>4019</v>
       </c>
       <c r="D195" s="24" t="s">
-        <v>4022</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -25881,13 +25879,13 @@
         <v>196</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>4023</v>
+        <v>4021</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>4047</v>
+        <v>4045</v>
       </c>
       <c r="D197" s="24" t="s">
-        <v>4048</v>
+        <v>4046</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -25898,10 +25896,10 @@
         <v>185</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>4054</v>
+        <v>4052</v>
       </c>
       <c r="D198" s="24" t="s">
-        <v>4055</v>
+        <v>4053</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -26360,10 +26358,10 @@
         <v>231</v>
       </c>
       <c r="C231" s="8" t="s">
-        <v>4029</v>
+        <v>4027</v>
       </c>
       <c r="D231" s="24" t="s">
-        <v>4030</v>
+        <v>4028</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -26371,13 +26369,13 @@
         <v>231</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>4027</v>
+        <v>4025</v>
       </c>
       <c r="C232" s="17" t="s">
-        <v>4028</v>
+        <v>4026</v>
       </c>
       <c r="D232" s="24" t="s">
-        <v>4031</v>
+        <v>4029</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -30770,10 +30768,10 @@
         <v>484</v>
       </c>
       <c r="C546" s="8" t="s">
-        <v>4052</v>
+        <v>4050</v>
       </c>
       <c r="D546" s="24" t="s">
-        <v>4053</v>
+        <v>4051</v>
       </c>
     </row>
     <row r="547" spans="1:4">
@@ -32643,13 +32641,13 @@
         <v>679</v>
       </c>
       <c r="B680" s="4" t="s">
-        <v>3981</v>
+        <v>3979</v>
       </c>
       <c r="C680" s="17" t="s">
-        <v>3972</v>
+        <v>3970</v>
       </c>
       <c r="D680" s="24" t="s">
-        <v>3971</v>
+        <v>3969</v>
       </c>
     </row>
     <row r="681" spans="1:4">
@@ -32660,10 +32658,10 @@
         <v>3839</v>
       </c>
       <c r="C681" s="17" t="s">
-        <v>3973</v>
+        <v>3971</v>
       </c>
       <c r="D681" s="24" t="s">
-        <v>3974</v>
+        <v>3972</v>
       </c>
     </row>
     <row r="682" spans="1:4">
@@ -32677,7 +32675,7 @@
         <v>3841</v>
       </c>
       <c r="D682" s="24" t="s">
-        <v>3903</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="683" spans="1:4">
@@ -32691,7 +32689,7 @@
         <v>3843</v>
       </c>
       <c r="D683" s="24" t="s">
-        <v>3904</v>
+        <v>3903</v>
       </c>
     </row>
     <row r="684" spans="1:4">
@@ -32705,7 +32703,7 @@
         <v>3845</v>
       </c>
       <c r="D684" s="24" t="s">
-        <v>3905</v>
+        <v>3904</v>
       </c>
     </row>
     <row r="685" spans="1:4">
@@ -32719,7 +32717,7 @@
         <v>3847</v>
       </c>
       <c r="D685" s="24" t="s">
-        <v>3906</v>
+        <v>3905</v>
       </c>
     </row>
     <row r="686" spans="1:4">
@@ -32733,7 +32731,7 @@
         <v>3849</v>
       </c>
       <c r="D686" s="24" t="s">
-        <v>3907</v>
+        <v>3906</v>
       </c>
     </row>
     <row r="687" spans="1:4">
@@ -32747,7 +32745,7 @@
         <v>3851</v>
       </c>
       <c r="D687" s="24" t="s">
-        <v>3908</v>
+        <v>3907</v>
       </c>
     </row>
     <row r="688" spans="1:4">
@@ -32758,10 +32756,10 @@
         <v>3852</v>
       </c>
       <c r="C688" s="17" t="s">
-        <v>3853</v>
+        <v>4068</v>
       </c>
       <c r="D688" s="24" t="s">
-        <v>3909</v>
+        <v>4071</v>
       </c>
     </row>
     <row r="689" spans="1:4">
@@ -32769,13 +32767,13 @@
         <v>688</v>
       </c>
       <c r="B689" s="4" t="s">
-        <v>4070</v>
+        <v>4066</v>
       </c>
       <c r="C689" s="17" t="s">
-        <v>4068</v>
+        <v>4069</v>
       </c>
       <c r="D689" s="26" t="s">
-        <v>4069</v>
+        <v>4072</v>
       </c>
     </row>
     <row r="690" spans="1:4">
@@ -32783,10 +32781,10 @@
         <v>689</v>
       </c>
       <c r="B690" s="4" t="s">
-        <v>4071</v>
+        <v>4067</v>
       </c>
       <c r="C690" s="17" t="s">
-        <v>4072</v>
+        <v>4070</v>
       </c>
       <c r="D690" s="26" t="s">
         <v>4073</v>
@@ -32797,13 +32795,13 @@
         <v>690</v>
       </c>
       <c r="B691" s="4" t="s">
+        <v>3853</v>
+      </c>
+      <c r="C691" s="17" t="s">
         <v>3854</v>
       </c>
-      <c r="C691" s="17" t="s">
-        <v>3855</v>
-      </c>
       <c r="D691" s="24" t="s">
-        <v>3910</v>
+        <v>3908</v>
       </c>
     </row>
     <row r="692" spans="1:4">
@@ -32811,13 +32809,13 @@
         <v>691</v>
       </c>
       <c r="B692" s="4" t="s">
+        <v>3855</v>
+      </c>
+      <c r="C692" s="17" t="s">
         <v>3856</v>
       </c>
-      <c r="C692" s="17" t="s">
-        <v>3857</v>
-      </c>
       <c r="D692" s="24" t="s">
-        <v>3911</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="693" spans="1:4">
@@ -32825,13 +32823,13 @@
         <v>692</v>
       </c>
       <c r="B693" s="4" t="s">
+        <v>3857</v>
+      </c>
+      <c r="C693" s="17" t="s">
         <v>3858</v>
       </c>
-      <c r="C693" s="17" t="s">
-        <v>3859</v>
-      </c>
       <c r="D693" s="24" t="s">
-        <v>3912</v>
+        <v>3910</v>
       </c>
     </row>
     <row r="694" spans="1:4">
@@ -32839,13 +32837,13 @@
         <v>693</v>
       </c>
       <c r="B694" s="4" t="s">
+        <v>3859</v>
+      </c>
+      <c r="C694" s="17" t="s">
         <v>3860</v>
       </c>
-      <c r="C694" s="17" t="s">
-        <v>3861</v>
-      </c>
       <c r="D694" s="24" t="s">
-        <v>3913</v>
+        <v>3911</v>
       </c>
     </row>
     <row r="695" spans="1:4">
@@ -32853,13 +32851,13 @@
         <v>694</v>
       </c>
       <c r="B695" s="4" t="s">
+        <v>3861</v>
+      </c>
+      <c r="C695" s="17" t="s">
         <v>3862</v>
       </c>
-      <c r="C695" s="17" t="s">
-        <v>3863</v>
-      </c>
       <c r="D695" s="24" t="s">
-        <v>3914</v>
+        <v>3912</v>
       </c>
     </row>
     <row r="696" spans="1:4">
@@ -32867,13 +32865,13 @@
         <v>695</v>
       </c>
       <c r="B696" s="4" t="s">
+        <v>3863</v>
+      </c>
+      <c r="C696" s="17" t="s">
         <v>3864</v>
       </c>
-      <c r="C696" s="17" t="s">
-        <v>3865</v>
-      </c>
       <c r="D696" s="24" t="s">
-        <v>3915</v>
+        <v>3913</v>
       </c>
     </row>
     <row r="697" spans="1:4">
@@ -32881,13 +32879,13 @@
         <v>696</v>
       </c>
       <c r="B697" s="4" t="s">
+        <v>3865</v>
+      </c>
+      <c r="C697" s="17" t="s">
         <v>3866</v>
       </c>
-      <c r="C697" s="17" t="s">
-        <v>3867</v>
-      </c>
       <c r="D697" s="24" t="s">
-        <v>3916</v>
+        <v>3914</v>
       </c>
     </row>
     <row r="698" spans="1:4">
@@ -32895,13 +32893,13 @@
         <v>697</v>
       </c>
       <c r="B698" s="4" t="s">
+        <v>3867</v>
+      </c>
+      <c r="C698" s="17" t="s">
         <v>3868</v>
       </c>
-      <c r="C698" s="17" t="s">
-        <v>3869</v>
-      </c>
       <c r="D698" s="24" t="s">
-        <v>3917</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="699" spans="1:4">
@@ -32909,13 +32907,13 @@
         <v>698</v>
       </c>
       <c r="B699" s="4" t="s">
+        <v>3869</v>
+      </c>
+      <c r="C699" s="17" t="s">
         <v>3870</v>
       </c>
-      <c r="C699" s="17" t="s">
-        <v>3871</v>
-      </c>
       <c r="D699" s="24" t="s">
-        <v>3918</v>
+        <v>3916</v>
       </c>
     </row>
     <row r="700" spans="1:4">
@@ -32923,13 +32921,13 @@
         <v>699</v>
       </c>
       <c r="B700" s="4" t="s">
+        <v>3871</v>
+      </c>
+      <c r="C700" s="17" t="s">
         <v>3872</v>
       </c>
-      <c r="C700" s="17" t="s">
-        <v>3873</v>
-      </c>
       <c r="D700" s="24" t="s">
-        <v>3919</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="701" spans="1:4">
@@ -32937,13 +32935,13 @@
         <v>700</v>
       </c>
       <c r="B701" s="4" t="s">
+        <v>3873</v>
+      </c>
+      <c r="C701" s="17" t="s">
         <v>3874</v>
       </c>
-      <c r="C701" s="17" t="s">
-        <v>3875</v>
-      </c>
       <c r="D701" s="24" t="s">
-        <v>3920</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="702" spans="1:4">
@@ -32951,13 +32949,13 @@
         <v>701</v>
       </c>
       <c r="B702" s="4" t="s">
+        <v>3875</v>
+      </c>
+      <c r="C702" s="17" t="s">
         <v>3876</v>
       </c>
-      <c r="C702" s="17" t="s">
-        <v>3877</v>
-      </c>
       <c r="D702" s="24" t="s">
-        <v>3921</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="703" spans="1:4">
@@ -32965,13 +32963,13 @@
         <v>702</v>
       </c>
       <c r="B703" s="4" t="s">
+        <v>3877</v>
+      </c>
+      <c r="C703" s="17" t="s">
         <v>3878</v>
       </c>
-      <c r="C703" s="17" t="s">
-        <v>3879</v>
-      </c>
       <c r="D703" s="24" t="s">
-        <v>3922</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="704" spans="1:4">
@@ -32979,13 +32977,13 @@
         <v>703</v>
       </c>
       <c r="B704" s="4" t="s">
+        <v>3879</v>
+      </c>
+      <c r="C704" s="17" t="s">
         <v>3880</v>
       </c>
-      <c r="C704" s="17" t="s">
-        <v>3881</v>
-      </c>
       <c r="D704" s="24" t="s">
-        <v>3923</v>
+        <v>3921</v>
       </c>
     </row>
     <row r="705" spans="1:4">
@@ -32993,13 +32991,13 @@
         <v>704</v>
       </c>
       <c r="B705" s="4" t="s">
+        <v>3881</v>
+      </c>
+      <c r="C705" s="17" t="s">
         <v>3882</v>
       </c>
-      <c r="C705" s="17" t="s">
-        <v>3883</v>
-      </c>
       <c r="D705" s="24" t="s">
-        <v>3924</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="706" spans="1:4">
@@ -33007,13 +33005,13 @@
         <v>705</v>
       </c>
       <c r="B706" s="4" t="s">
-        <v>3884</v>
+        <v>3883</v>
       </c>
       <c r="C706" s="17" t="s">
-        <v>3975</v>
+        <v>3973</v>
       </c>
       <c r="D706" s="24" t="s">
-        <v>3978</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="707" spans="1:4">
@@ -33021,13 +33019,13 @@
         <v>706</v>
       </c>
       <c r="B707" s="4" t="s">
-        <v>3885</v>
+        <v>3884</v>
       </c>
       <c r="C707" s="17" t="s">
-        <v>3976</v>
+        <v>3974</v>
       </c>
       <c r="D707" s="24" t="s">
-        <v>3979</v>
+        <v>3977</v>
       </c>
     </row>
     <row r="708" spans="1:4">
@@ -33035,13 +33033,13 @@
         <v>707</v>
       </c>
       <c r="B708" s="4" t="s">
-        <v>3886</v>
+        <v>3885</v>
       </c>
       <c r="C708" s="17" t="s">
-        <v>3977</v>
+        <v>3975</v>
       </c>
       <c r="D708" s="24" t="s">
-        <v>3980</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="709" spans="1:4">
@@ -33049,13 +33047,13 @@
         <v>708</v>
       </c>
       <c r="B709" s="4" t="s">
+        <v>3886</v>
+      </c>
+      <c r="C709" s="17" t="s">
         <v>3887</v>
       </c>
-      <c r="C709" s="17" t="s">
-        <v>3888</v>
-      </c>
       <c r="D709" s="24" t="s">
-        <v>3925</v>
+        <v>3923</v>
       </c>
     </row>
     <row r="710" spans="1:4">
@@ -33063,13 +33061,13 @@
         <v>709</v>
       </c>
       <c r="B710" s="4" t="s">
+        <v>3888</v>
+      </c>
+      <c r="C710" s="17" t="s">
         <v>3889</v>
       </c>
-      <c r="C710" s="17" t="s">
-        <v>3890</v>
-      </c>
       <c r="D710" s="24" t="s">
-        <v>3926</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="711" spans="1:4">
@@ -33077,13 +33075,13 @@
         <v>710</v>
       </c>
       <c r="B711" s="4" t="s">
+        <v>3890</v>
+      </c>
+      <c r="C711" s="17" t="s">
         <v>3891</v>
       </c>
-      <c r="C711" s="17" t="s">
-        <v>3892</v>
-      </c>
       <c r="D711" s="24" t="s">
-        <v>3927</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="712" spans="1:4">
@@ -33091,13 +33089,13 @@
         <v>711</v>
       </c>
       <c r="B712" s="4" t="s">
+        <v>3892</v>
+      </c>
+      <c r="C712" s="17" t="s">
         <v>3893</v>
       </c>
-      <c r="C712" s="17" t="s">
-        <v>3894</v>
-      </c>
       <c r="D712" s="24" t="s">
-        <v>3928</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="713" spans="1:4">
@@ -33105,13 +33103,13 @@
         <v>712</v>
       </c>
       <c r="B713" s="4" t="s">
+        <v>3894</v>
+      </c>
+      <c r="C713" s="17" t="s">
         <v>3895</v>
       </c>
-      <c r="C713" s="17" t="s">
-        <v>3896</v>
-      </c>
       <c r="D713" s="24" t="s">
-        <v>3929</v>
+        <v>3927</v>
       </c>
     </row>
     <row r="714" spans="1:4">
@@ -33119,13 +33117,13 @@
         <v>713</v>
       </c>
       <c r="B714" s="4" t="s">
+        <v>3896</v>
+      </c>
+      <c r="C714" s="17" t="s">
         <v>3897</v>
       </c>
-      <c r="C714" s="17" t="s">
-        <v>3898</v>
-      </c>
       <c r="D714" s="24" t="s">
-        <v>3930</v>
+        <v>3928</v>
       </c>
     </row>
     <row r="715" spans="1:4">
@@ -33133,13 +33131,13 @@
         <v>714</v>
       </c>
       <c r="B715" s="4" t="s">
+        <v>3898</v>
+      </c>
+      <c r="C715" s="17" t="s">
         <v>3899</v>
       </c>
-      <c r="C715" s="17" t="s">
-        <v>3900</v>
-      </c>
       <c r="D715" s="24" t="s">
-        <v>3931</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="716" spans="1:4">
@@ -33147,13 +33145,13 @@
         <v>715</v>
       </c>
       <c r="B716" s="4" t="s">
+        <v>3900</v>
+      </c>
+      <c r="C716" s="17" t="s">
         <v>3901</v>
       </c>
-      <c r="C716" s="17" t="s">
-        <v>3902</v>
-      </c>
       <c r="D716" s="24" t="s">
-        <v>3932</v>
+        <v>3930</v>
       </c>
     </row>
     <row r="717" spans="1:4">
@@ -33161,13 +33159,13 @@
         <v>716</v>
       </c>
       <c r="B717" s="4" t="s">
-        <v>3933</v>
+        <v>3931</v>
       </c>
       <c r="C717" s="17" t="s">
-        <v>3934</v>
+        <v>3932</v>
       </c>
       <c r="D717" s="24" t="s">
-        <v>3958</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="718" spans="1:4">
@@ -33175,13 +33173,13 @@
         <v>717</v>
       </c>
       <c r="B718" s="4" t="s">
-        <v>3935</v>
+        <v>3933</v>
       </c>
       <c r="C718" s="17" t="s">
-        <v>3936</v>
+        <v>3934</v>
       </c>
       <c r="D718" s="24" t="s">
-        <v>3959</v>
+        <v>3957</v>
       </c>
     </row>
     <row r="719" spans="1:4">
@@ -33189,13 +33187,13 @@
         <v>718</v>
       </c>
       <c r="B719" s="4" t="s">
-        <v>3937</v>
+        <v>3935</v>
       </c>
       <c r="C719" s="17" t="s">
-        <v>3938</v>
+        <v>3936</v>
       </c>
       <c r="D719" s="24" t="s">
-        <v>3960</v>
+        <v>3958</v>
       </c>
     </row>
     <row r="720" spans="1:4">
@@ -33203,13 +33201,13 @@
         <v>719</v>
       </c>
       <c r="B720" s="4" t="s">
-        <v>3939</v>
+        <v>3937</v>
       </c>
       <c r="C720" s="17" t="s">
         <v>3212</v>
       </c>
       <c r="D720" s="24" t="s">
-        <v>3961</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="721" spans="1:4">
@@ -33217,13 +33215,13 @@
         <v>720</v>
       </c>
       <c r="B721" s="4" t="s">
-        <v>3940</v>
+        <v>3938</v>
       </c>
       <c r="C721" s="17" t="s">
-        <v>3941</v>
+        <v>3939</v>
       </c>
       <c r="D721" s="24" t="s">
-        <v>3962</v>
+        <v>3960</v>
       </c>
     </row>
     <row r="722" spans="1:4">
@@ -33231,13 +33229,13 @@
         <v>721</v>
       </c>
       <c r="B722" s="4" t="s">
-        <v>3942</v>
+        <v>3940</v>
       </c>
       <c r="C722" s="17" t="s">
-        <v>3943</v>
+        <v>3941</v>
       </c>
       <c r="D722" s="24" t="s">
-        <v>3963</v>
+        <v>3961</v>
       </c>
     </row>
     <row r="723" spans="1:4">
@@ -33245,13 +33243,13 @@
         <v>722</v>
       </c>
       <c r="B723" s="4" t="s">
-        <v>3944</v>
+        <v>3942</v>
       </c>
       <c r="C723" s="17" t="s">
-        <v>3945</v>
+        <v>3943</v>
       </c>
       <c r="D723" s="24" t="s">
-        <v>3964</v>
+        <v>3962</v>
       </c>
     </row>
     <row r="724" spans="1:4">
@@ -33259,13 +33257,13 @@
         <v>723</v>
       </c>
       <c r="B724" s="4" t="s">
-        <v>3946</v>
+        <v>3944</v>
       </c>
       <c r="C724" s="17" t="s">
-        <v>3947</v>
+        <v>3945</v>
       </c>
       <c r="D724" s="24" t="s">
-        <v>3965</v>
+        <v>3963</v>
       </c>
     </row>
     <row r="725" spans="1:4">
@@ -33273,13 +33271,13 @@
         <v>724</v>
       </c>
       <c r="B725" s="4" t="s">
-        <v>3948</v>
+        <v>3946</v>
       </c>
       <c r="C725" s="17" t="s">
-        <v>3949</v>
+        <v>3947</v>
       </c>
       <c r="D725" s="24" t="s">
-        <v>3966</v>
+        <v>3964</v>
       </c>
     </row>
     <row r="726" spans="1:4">
@@ -33287,13 +33285,13 @@
         <v>725</v>
       </c>
       <c r="B726" s="4" t="s">
-        <v>3950</v>
+        <v>3948</v>
       </c>
       <c r="C726" s="17" t="s">
-        <v>3951</v>
+        <v>3949</v>
       </c>
       <c r="D726" s="24" t="s">
-        <v>3967</v>
+        <v>3965</v>
       </c>
     </row>
     <row r="727" spans="1:4">
@@ -33301,13 +33299,13 @@
         <v>726</v>
       </c>
       <c r="B727" s="4" t="s">
-        <v>3952</v>
+        <v>3950</v>
       </c>
       <c r="C727" s="17" t="s">
-        <v>3953</v>
+        <v>3951</v>
       </c>
       <c r="D727" s="24" t="s">
-        <v>3968</v>
+        <v>3966</v>
       </c>
     </row>
     <row r="728" spans="1:4">
@@ -33315,13 +33313,13 @@
         <v>727</v>
       </c>
       <c r="B728" s="4" t="s">
-        <v>3954</v>
+        <v>3952</v>
       </c>
       <c r="C728" s="17" t="s">
-        <v>3955</v>
+        <v>3953</v>
       </c>
       <c r="D728" s="24" t="s">
-        <v>3969</v>
+        <v>3967</v>
       </c>
     </row>
     <row r="729" spans="1:4">
@@ -33329,13 +33327,13 @@
         <v>728</v>
       </c>
       <c r="B729" s="4" t="s">
-        <v>3956</v>
+        <v>3954</v>
       </c>
       <c r="C729" s="17" t="s">
-        <v>3957</v>
+        <v>3955</v>
       </c>
       <c r="D729" s="24" t="s">
-        <v>3970</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="730" spans="1:4">
@@ -33346,10 +33344,10 @@
         <v>3838</v>
       </c>
       <c r="C730" s="17" t="s">
-        <v>3982</v>
+        <v>3980</v>
       </c>
       <c r="D730" s="24" t="s">
-        <v>3983</v>
+        <v>3981</v>
       </c>
     </row>
     <row r="731" spans="1:4">
@@ -33357,13 +33355,13 @@
         <v>730</v>
       </c>
       <c r="B731" s="4" t="s">
-        <v>3984</v>
+        <v>3982</v>
       </c>
       <c r="C731" s="17" t="s">
-        <v>3985</v>
+        <v>3983</v>
       </c>
       <c r="D731" s="24" t="s">
-        <v>3988</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="732" spans="1:4">
@@ -33371,13 +33369,13 @@
         <v>731</v>
       </c>
       <c r="B732" s="4" t="s">
-        <v>3986</v>
+        <v>3984</v>
       </c>
       <c r="C732" s="17" t="s">
+        <v>3985</v>
+      </c>
+      <c r="D732" s="24" t="s">
         <v>3987</v>
-      </c>
-      <c r="D732" s="24" t="s">
-        <v>3989</v>
       </c>
     </row>
     <row r="733" spans="1:4">
@@ -33385,7 +33383,7 @@
         <v>732</v>
       </c>
       <c r="B733" s="4" t="s">
-        <v>3990</v>
+        <v>3988</v>
       </c>
       <c r="C733" s="17" t="s">
         <v>1116</v>
@@ -33399,13 +33397,13 @@
         <v>733</v>
       </c>
       <c r="B734" s="4" t="s">
-        <v>3991</v>
+        <v>3989</v>
       </c>
       <c r="C734" s="17" t="s">
-        <v>3992</v>
+        <v>3990</v>
       </c>
       <c r="D734" s="24" t="s">
-        <v>4005</v>
+        <v>4003</v>
       </c>
     </row>
     <row r="735" spans="1:4">
@@ -33413,13 +33411,13 @@
         <v>734</v>
       </c>
       <c r="B735" s="4" t="s">
-        <v>3993</v>
+        <v>3991</v>
       </c>
       <c r="C735" s="17" t="s">
-        <v>3994</v>
+        <v>3992</v>
       </c>
       <c r="D735" s="24" t="s">
-        <v>4006</v>
+        <v>4004</v>
       </c>
     </row>
     <row r="736" spans="1:4">
@@ -33427,13 +33425,13 @@
         <v>735</v>
       </c>
       <c r="B736" s="4" t="s">
-        <v>3995</v>
+        <v>3993</v>
       </c>
       <c r="C736" s="17" t="s">
-        <v>3996</v>
+        <v>3994</v>
       </c>
       <c r="D736" s="24" t="s">
-        <v>4007</v>
+        <v>4005</v>
       </c>
     </row>
     <row r="737" spans="1:4">
@@ -33441,13 +33439,13 @@
         <v>736</v>
       </c>
       <c r="B737" s="4" t="s">
-        <v>3997</v>
+        <v>3995</v>
       </c>
       <c r="C737" s="17" t="s">
-        <v>3998</v>
+        <v>3996</v>
       </c>
       <c r="D737" s="24" t="s">
-        <v>4008</v>
+        <v>4006</v>
       </c>
     </row>
     <row r="738" spans="1:4">
@@ -33455,13 +33453,13 @@
         <v>737</v>
       </c>
       <c r="B738" s="4" t="s">
-        <v>3999</v>
+        <v>3997</v>
       </c>
       <c r="C738" s="17" t="s">
-        <v>4000</v>
+        <v>3998</v>
       </c>
       <c r="D738" s="24" t="s">
-        <v>4009</v>
+        <v>4007</v>
       </c>
     </row>
     <row r="739" spans="1:4">
@@ -33469,13 +33467,13 @@
         <v>738</v>
       </c>
       <c r="B739" s="4" t="s">
-        <v>4001</v>
+        <v>3999</v>
       </c>
       <c r="C739" s="17" t="s">
-        <v>4002</v>
+        <v>4000</v>
       </c>
       <c r="D739" s="24" t="s">
-        <v>4010</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="740" spans="1:4">
@@ -33483,13 +33481,13 @@
         <v>739</v>
       </c>
       <c r="B740" s="4" t="s">
-        <v>4003</v>
+        <v>4001</v>
       </c>
       <c r="C740" s="17" t="s">
-        <v>4004</v>
+        <v>4002</v>
       </c>
       <c r="D740" s="24" t="s">
-        <v>4011</v>
+        <v>4009</v>
       </c>
     </row>
     <row r="741" spans="1:4">
@@ -33497,13 +33495,13 @@
         <v>740</v>
       </c>
       <c r="B741" s="4" t="s">
-        <v>4015</v>
+        <v>4013</v>
       </c>
       <c r="C741" s="17" t="s">
         <v>2029</v>
       </c>
       <c r="D741" s="17" t="s">
-        <v>4013</v>
+        <v>4011</v>
       </c>
     </row>
     <row r="742" spans="1:4">
@@ -33511,13 +33509,13 @@
         <v>741</v>
       </c>
       <c r="B742" s="4" t="s">
-        <v>4016</v>
+        <v>4014</v>
       </c>
       <c r="C742" s="17" t="s">
+        <v>4010</v>
+      </c>
+      <c r="D742" s="17" t="s">
         <v>4012</v>
-      </c>
-      <c r="D742" s="17" t="s">
-        <v>4014</v>
       </c>
     </row>
     <row r="743" spans="1:4">
@@ -33525,13 +33523,13 @@
         <v>742</v>
       </c>
       <c r="B743" s="4" t="s">
+        <v>4022</v>
+      </c>
+      <c r="C743" s="17" t="s">
+        <v>4023</v>
+      </c>
+      <c r="D743" s="24" t="s">
         <v>4024</v>
-      </c>
-      <c r="C743" s="17" t="s">
-        <v>4025</v>
-      </c>
-      <c r="D743" s="24" t="s">
-        <v>4026</v>
       </c>
     </row>
     <row r="744" spans="1:4">
@@ -33539,13 +33537,13 @@
         <v>743</v>
       </c>
       <c r="B744" s="4" t="s">
+        <v>4030</v>
+      </c>
+      <c r="C744" s="17" t="s">
+        <v>4031</v>
+      </c>
+      <c r="D744" s="24" t="s">
         <v>4032</v>
-      </c>
-      <c r="C744" s="17" t="s">
-        <v>4033</v>
-      </c>
-      <c r="D744" s="24" t="s">
-        <v>4034</v>
       </c>
     </row>
     <row r="745" spans="1:4">
@@ -33553,13 +33551,13 @@
         <v>744</v>
       </c>
       <c r="B745" s="4" t="s">
-        <v>4037</v>
+        <v>4035</v>
       </c>
       <c r="C745" s="17" t="s">
-        <v>4035</v>
+        <v>4033</v>
       </c>
       <c r="D745" s="24" t="s">
-        <v>4036</v>
+        <v>4034</v>
       </c>
     </row>
     <row r="746" spans="1:4">
@@ -33567,13 +33565,13 @@
         <v>745</v>
       </c>
       <c r="B746" s="4" t="s">
-        <v>4046</v>
+        <v>4044</v>
       </c>
       <c r="C746" s="17" t="s">
-        <v>4038</v>
+        <v>4036</v>
       </c>
       <c r="D746" s="24" t="s">
-        <v>4039</v>
+        <v>4037</v>
       </c>
     </row>
     <row r="747" spans="1:4">
@@ -33581,13 +33579,13 @@
         <v>746</v>
       </c>
       <c r="B747" s="4" t="s">
-        <v>4042</v>
+        <v>4040</v>
       </c>
       <c r="C747" s="17" t="s">
-        <v>4040</v>
+        <v>4038</v>
       </c>
       <c r="D747" s="24" t="s">
-        <v>4041</v>
+        <v>4039</v>
       </c>
     </row>
     <row r="748" spans="1:4">
@@ -33595,13 +33593,13 @@
         <v>747</v>
       </c>
       <c r="B748" s="4" t="s">
+        <v>4041</v>
+      </c>
+      <c r="C748" s="17" t="s">
+        <v>4042</v>
+      </c>
+      <c r="D748" s="24" t="s">
         <v>4043</v>
-      </c>
-      <c r="C748" s="17" t="s">
-        <v>4044</v>
-      </c>
-      <c r="D748" s="24" t="s">
-        <v>4045</v>
       </c>
     </row>
     <row r="749" spans="1:4">
@@ -33609,13 +33607,13 @@
         <v>748</v>
       </c>
       <c r="B749" s="4" t="s">
-        <v>4051</v>
+        <v>4049</v>
       </c>
       <c r="C749" s="17" t="s">
-        <v>4049</v>
+        <v>4047</v>
       </c>
       <c r="D749" s="24" t="s">
-        <v>4050</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="750" spans="1:4">
@@ -33623,13 +33621,13 @@
         <v>749</v>
       </c>
       <c r="B750" s="4" t="s">
+        <v>4054</v>
+      </c>
+      <c r="C750" s="17" t="s">
+        <v>4055</v>
+      </c>
+      <c r="D750" s="24" t="s">
         <v>4056</v>
-      </c>
-      <c r="C750" s="17" t="s">
-        <v>4057</v>
-      </c>
-      <c r="D750" s="24" t="s">
-        <v>4058</v>
       </c>
     </row>
     <row r="751" spans="1:4">
@@ -33637,13 +33635,13 @@
         <v>750</v>
       </c>
       <c r="B751" s="4" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C751" s="17" t="s">
+        <v>4058</v>
+      </c>
+      <c r="D751" s="24" t="s">
         <v>4059</v>
-      </c>
-      <c r="C751" s="17" t="s">
-        <v>4060</v>
-      </c>
-      <c r="D751" s="24" t="s">
-        <v>4061</v>
       </c>
     </row>
     <row r="752" spans="1:4">
@@ -33651,13 +33649,13 @@
         <v>751</v>
       </c>
       <c r="B752" s="4" t="s">
+        <v>4060</v>
+      </c>
+      <c r="C752" s="17" t="s">
+        <v>4061</v>
+      </c>
+      <c r="D752" s="24" t="s">
         <v>4062</v>
-      </c>
-      <c r="C752" s="17" t="s">
-        <v>4063</v>
-      </c>
-      <c r="D752" s="24" t="s">
-        <v>4064</v>
       </c>
     </row>
     <row r="753" spans="1:4">
@@ -33665,13 +33663,13 @@
         <v>752</v>
       </c>
       <c r="B753" s="4" t="s">
+        <v>4063</v>
+      </c>
+      <c r="C753" s="17" t="s">
+        <v>4064</v>
+      </c>
+      <c r="D753" s="24" t="s">
         <v>4065</v>
-      </c>
-      <c r="C753" s="17" t="s">
-        <v>4066</v>
-      </c>
-      <c r="D753" s="24" t="s">
-        <v>4067</v>
       </c>
     </row>
     <row r="754" spans="1:4">

</xml_diff>

<commit_message>
System testing and bug fixing
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F01AE4F-B277-42D4-B1A9-D96F3890D9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F285720-A90D-4031-A6A9-D2402FCB453A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4303" uniqueCount="4074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4333" uniqueCount="4104">
   <si>
     <t>myself</t>
   </si>
@@ -15446,6 +15446,120 @@
   </si>
   <si>
     <t>Print the exception log</t>
+  </si>
+  <si>
+    <t>projectTag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deviceTag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>displayContentConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示内容配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>realtimeMonitoringModule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实时监控模块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FESResultStatisticsPieChart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工况诊断统计饼图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commStatusStatisticsPieChart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通信状态统计饼图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>runStatusStatisticsPieChart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运行状态统计饼图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>historyQueryModule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>历史查询模块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alarmQueryModule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display content configuration</t>
+  </si>
+  <si>
+    <t>Real-time monitoring module</t>
+  </si>
+  <si>
+    <t>Condition Diagnosis Statistics Pie Chart</t>
+  </si>
+  <si>
+    <t>Communication status statistics pie chart</t>
+  </si>
+  <si>
+    <t>Run state statistics pie chart</t>
+  </si>
+  <si>
+    <t>History query module</t>
+  </si>
+  <si>
+    <t>报警查询模块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alarm query module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>primaryDeviceModule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主设备模块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Primary device module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project tags</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Device tags</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -23117,10 +23231,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D763"/>
+  <dimension ref="A1:D783"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A672" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D688" sqref="D688:D690"/>
+    <sheetView tabSelected="1" topLeftCell="A744" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D768" sqref="D768"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -33673,64 +33787,264 @@
       </c>
     </row>
     <row r="754" spans="1:4">
-      <c r="A754" s="14"/>
-      <c r="B754" s="4"/>
-      <c r="C754" s="17"/>
-      <c r="D754" s="24"/>
+      <c r="A754" s="14">
+        <v>753</v>
+      </c>
+      <c r="B754" s="4" t="s">
+        <v>4074</v>
+      </c>
+      <c r="C754" s="17" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D754" s="24" t="s">
+        <v>4102</v>
+      </c>
     </row>
     <row r="755" spans="1:4">
-      <c r="A755" s="14"/>
-      <c r="B755" s="4"/>
-      <c r="C755" s="17"/>
-      <c r="D755" s="24"/>
+      <c r="A755" s="14">
+        <v>754</v>
+      </c>
+      <c r="B755" s="4" t="s">
+        <v>4076</v>
+      </c>
+      <c r="C755" s="17" t="s">
+        <v>4077</v>
+      </c>
+      <c r="D755" s="24" t="s">
+        <v>4103</v>
+      </c>
     </row>
     <row r="756" spans="1:4">
-      <c r="A756" s="14"/>
-      <c r="B756" s="4"/>
-      <c r="C756" s="17"/>
-      <c r="D756" s="24"/>
+      <c r="A756" s="14">
+        <v>755</v>
+      </c>
+      <c r="B756" s="4" t="s">
+        <v>4078</v>
+      </c>
+      <c r="C756" s="17" t="s">
+        <v>4079</v>
+      </c>
+      <c r="D756" s="24" t="s">
+        <v>4091</v>
+      </c>
     </row>
     <row r="757" spans="1:4">
-      <c r="A757" s="14"/>
-      <c r="B757" s="4"/>
-      <c r="C757" s="17"/>
-      <c r="D757" s="24"/>
+      <c r="A757" s="14">
+        <v>756</v>
+      </c>
+      <c r="B757" s="4" t="s">
+        <v>4080</v>
+      </c>
+      <c r="C757" s="17" t="s">
+        <v>4081</v>
+      </c>
+      <c r="D757" s="24" t="s">
+        <v>4092</v>
+      </c>
     </row>
     <row r="758" spans="1:4">
-      <c r="A758" s="14"/>
-      <c r="B758" s="4"/>
-      <c r="C758" s="17"/>
-      <c r="D758" s="24"/>
+      <c r="A758" s="14">
+        <v>757</v>
+      </c>
+      <c r="B758" s="4" t="s">
+        <v>4082</v>
+      </c>
+      <c r="C758" s="17" t="s">
+        <v>4083</v>
+      </c>
+      <c r="D758" s="24" t="s">
+        <v>4093</v>
+      </c>
     </row>
     <row r="759" spans="1:4">
-      <c r="A759" s="14"/>
-      <c r="B759" s="4"/>
-      <c r="C759" s="17"/>
-      <c r="D759" s="24"/>
+      <c r="A759" s="14">
+        <v>758</v>
+      </c>
+      <c r="B759" s="4" t="s">
+        <v>4084</v>
+      </c>
+      <c r="C759" s="17" t="s">
+        <v>4085</v>
+      </c>
+      <c r="D759" s="24" t="s">
+        <v>4094</v>
+      </c>
     </row>
     <row r="760" spans="1:4">
-      <c r="A760" s="14"/>
-      <c r="B760" s="4"/>
-      <c r="C760" s="17"/>
-      <c r="D760" s="24"/>
+      <c r="A760" s="14">
+        <v>759</v>
+      </c>
+      <c r="B760" s="4" t="s">
+        <v>4086</v>
+      </c>
+      <c r="C760" s="17" t="s">
+        <v>4087</v>
+      </c>
+      <c r="D760" s="24" t="s">
+        <v>4095</v>
+      </c>
     </row>
     <row r="761" spans="1:4">
-      <c r="A761" s="14"/>
-      <c r="B761" s="4"/>
-      <c r="C761" s="17"/>
-      <c r="D761" s="24"/>
+      <c r="A761" s="14">
+        <v>760</v>
+      </c>
+      <c r="B761" s="4" t="s">
+        <v>4088</v>
+      </c>
+      <c r="C761" s="17" t="s">
+        <v>4089</v>
+      </c>
+      <c r="D761" s="24" t="s">
+        <v>4096</v>
+      </c>
     </row>
     <row r="762" spans="1:4">
-      <c r="A762" s="14"/>
-      <c r="B762" s="4"/>
-      <c r="C762" s="17"/>
-      <c r="D762" s="24"/>
+      <c r="A762" s="14">
+        <v>761</v>
+      </c>
+      <c r="B762" s="4" t="s">
+        <v>4090</v>
+      </c>
+      <c r="C762" s="17" t="s">
+        <v>4097</v>
+      </c>
+      <c r="D762" s="24" t="s">
+        <v>4098</v>
+      </c>
     </row>
     <row r="763" spans="1:4">
-      <c r="A763" s="14"/>
-      <c r="B763" s="4"/>
-      <c r="C763" s="17"/>
-      <c r="D763" s="24"/>
+      <c r="A763" s="14">
+        <v>762</v>
+      </c>
+      <c r="B763" s="4" t="s">
+        <v>4099</v>
+      </c>
+      <c r="C763" s="17" t="s">
+        <v>4100</v>
+      </c>
+      <c r="D763" s="24" t="s">
+        <v>4101</v>
+      </c>
+    </row>
+    <row r="764" spans="1:4">
+      <c r="A764" s="14"/>
+      <c r="B764" s="4"/>
+      <c r="C764" s="17"/>
+      <c r="D764" s="24"/>
+    </row>
+    <row r="765" spans="1:4">
+      <c r="A765" s="14"/>
+      <c r="B765" s="4"/>
+      <c r="C765" s="17"/>
+      <c r="D765" s="24"/>
+    </row>
+    <row r="766" spans="1:4">
+      <c r="A766" s="14"/>
+      <c r="B766" s="4"/>
+      <c r="C766" s="17"/>
+      <c r="D766" s="24"/>
+    </row>
+    <row r="767" spans="1:4">
+      <c r="A767" s="14"/>
+      <c r="B767" s="4"/>
+      <c r="C767" s="17"/>
+      <c r="D767" s="24"/>
+    </row>
+    <row r="768" spans="1:4">
+      <c r="A768" s="14"/>
+      <c r="B768" s="4"/>
+      <c r="C768" s="17"/>
+      <c r="D768" s="24"/>
+    </row>
+    <row r="769" spans="1:4">
+      <c r="A769" s="14"/>
+      <c r="B769" s="4"/>
+      <c r="C769" s="17"/>
+      <c r="D769" s="24"/>
+    </row>
+    <row r="770" spans="1:4">
+      <c r="A770" s="14"/>
+      <c r="B770" s="4"/>
+      <c r="C770" s="17"/>
+      <c r="D770" s="24"/>
+    </row>
+    <row r="771" spans="1:4">
+      <c r="A771" s="14"/>
+      <c r="B771" s="4"/>
+      <c r="C771" s="17"/>
+      <c r="D771" s="24"/>
+    </row>
+    <row r="772" spans="1:4">
+      <c r="A772" s="14"/>
+      <c r="B772" s="4"/>
+      <c r="C772" s="17"/>
+      <c r="D772" s="24"/>
+    </row>
+    <row r="773" spans="1:4">
+      <c r="A773" s="14"/>
+      <c r="B773" s="4"/>
+      <c r="C773" s="17"/>
+      <c r="D773" s="24"/>
+    </row>
+    <row r="774" spans="1:4">
+      <c r="A774" s="14"/>
+      <c r="B774" s="4"/>
+      <c r="C774" s="17"/>
+      <c r="D774" s="24"/>
+    </row>
+    <row r="775" spans="1:4">
+      <c r="A775" s="14"/>
+      <c r="B775" s="4"/>
+      <c r="C775" s="17"/>
+      <c r="D775" s="24"/>
+    </row>
+    <row r="776" spans="1:4">
+      <c r="A776" s="14"/>
+      <c r="B776" s="4"/>
+      <c r="C776" s="17"/>
+      <c r="D776" s="24"/>
+    </row>
+    <row r="777" spans="1:4">
+      <c r="A777" s="14"/>
+      <c r="B777" s="4"/>
+      <c r="C777" s="17"/>
+      <c r="D777" s="24"/>
+    </row>
+    <row r="778" spans="1:4">
+      <c r="A778" s="14"/>
+      <c r="B778" s="4"/>
+      <c r="C778" s="17"/>
+      <c r="D778" s="24"/>
+    </row>
+    <row r="779" spans="1:4">
+      <c r="A779" s="14"/>
+      <c r="B779" s="4"/>
+      <c r="C779" s="17"/>
+      <c r="D779" s="24"/>
+    </row>
+    <row r="780" spans="1:4">
+      <c r="A780" s="14"/>
+      <c r="B780" s="4"/>
+      <c r="C780" s="17"/>
+      <c r="D780" s="24"/>
+    </row>
+    <row r="781" spans="1:4">
+      <c r="A781" s="14"/>
+      <c r="B781" s="4"/>
+      <c r="C781" s="17"/>
+      <c r="D781" s="24"/>
+    </row>
+    <row r="782" spans="1:4">
+      <c r="A782" s="14"/>
+      <c r="B782" s="4"/>
+      <c r="C782" s="17"/>
+      <c r="D782" s="24"/>
+    </row>
+    <row r="783" spans="1:4">
+      <c r="A783" s="14"/>
+      <c r="B783" s="4"/>
+      <c r="C783" s="17"/>
+      <c r="D783" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Expand field data parsing and adjustment
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnooc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnooc/locale/locale-en.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05BA514-B12C-43CB-8CB5-CF6167E6A2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5103996E-85EA-4399-BDBA-67C5F22D20E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,20 @@
     <sheet name="role" sheetId="9" r:id="rId9"/>
     <sheet name="video" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -15223,14 +15236,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>《智能化监控系统》 主要针对泵设备和管设备系列产品，通过驱动配置，实现采集、控制与报警等功能。模块包括实时监控、历史查询、生产报表、故障查询、设备日志、系统日志、计算维护、驱动配置、权限管理（组织用户、角色管理）、设备管理（设备信息、辅件设备、短信设备）和系统配置（模块配置、字典配置）等功能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intelligent Monitoring System is mainly aimed at pump equipment and pipe equipment series products, through the drive configuration, to achieve collection, control and alarm functions. The module includes real-time monitoring, historical query, production report, fault query, device log, system log, computing and maintenance, driver configuration, permission management (organization user and role management), device management (device information, accessory devices, SMS devices), and system configuration (module configuration, dictionary configuration) and other functions.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>计算字段关联表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -15570,14 +15575,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>数值状态统计饼图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Numerical state statistics pie chart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>报警数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -15630,6 +15627,22 @@
   </si>
   <si>
     <t>Alarm status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>报警状态统计饼图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alarm status statistics pie chart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《智能化监控系统》 主要针对泵设备和管设备系列产品，通过驱动配置，实现采集、控制与报警等功能。模块包括实时监控、历史查询、生产报表、报警查询、设备日志、系统日志、计算维护、驱动配置、权限管理（组织用户、角色管理）、设备管理（设备信息、辅件设备、短信设备）和系统配置（模块配置、字典配置）等功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intelligent Monitoring System is mainly aimed at pump equipment and pipe equipment series products, and realizes the functions of collection, control and alarm through drive configuration. The module includes real-time monitoring, historical query, production report, alarm query, device log, system log, calculation and maintenance, driver configuration, permission management (organization user, role management), device management (device information, auxiliary device, SMS device) and system configuration (module configuration, dictionary configuration) and other functions.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -17879,8 +17892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -17927,10 +17940,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>4017</v>
+        <v>4120</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4018</v>
+        <v>4121</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -23304,8 +23317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
   <dimension ref="A1:D785"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A745" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C762" sqref="C762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -23516,13 +23529,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>4104</v>
+        <v>4102</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>4120</v>
+        <v>4116</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>4121</v>
+        <v>4117</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -26053,10 +26066,10 @@
         <v>183</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>4019</v>
+        <v>4017</v>
       </c>
       <c r="D196" s="24" t="s">
-        <v>4020</v>
+        <v>4018</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -26078,13 +26091,13 @@
         <v>197</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>4021</v>
+        <v>4019</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>4045</v>
+        <v>4043</v>
       </c>
       <c r="D198" s="24" t="s">
-        <v>4046</v>
+        <v>4044</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -26095,10 +26108,10 @@
         <v>185</v>
       </c>
       <c r="C199" s="8" t="s">
-        <v>4052</v>
+        <v>4050</v>
       </c>
       <c r="D199" s="24" t="s">
-        <v>4053</v>
+        <v>4051</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -26557,10 +26570,10 @@
         <v>231</v>
       </c>
       <c r="C232" s="8" t="s">
-        <v>4027</v>
+        <v>4025</v>
       </c>
       <c r="D232" s="24" t="s">
-        <v>4028</v>
+        <v>4026</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -26568,13 +26581,13 @@
         <v>232</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>4025</v>
+        <v>4023</v>
       </c>
       <c r="C233" s="17" t="s">
-        <v>4026</v>
+        <v>4024</v>
       </c>
       <c r="D233" s="24" t="s">
-        <v>4029</v>
+        <v>4027</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -30967,10 +30980,10 @@
         <v>484</v>
       </c>
       <c r="C547" s="8" t="s">
-        <v>4050</v>
+        <v>4048</v>
       </c>
       <c r="D547" s="24" t="s">
-        <v>4051</v>
+        <v>4049</v>
       </c>
     </row>
     <row r="548" spans="1:4">
@@ -32955,10 +32968,10 @@
         <v>3852</v>
       </c>
       <c r="C689" s="17" t="s">
-        <v>4068</v>
+        <v>4066</v>
       </c>
       <c r="D689" s="24" t="s">
-        <v>4071</v>
+        <v>4069</v>
       </c>
     </row>
     <row r="690" spans="1:4">
@@ -32966,13 +32979,13 @@
         <v>689</v>
       </c>
       <c r="B690" s="4" t="s">
-        <v>4066</v>
+        <v>4064</v>
       </c>
       <c r="C690" s="17" t="s">
-        <v>4069</v>
+        <v>4067</v>
       </c>
       <c r="D690" s="26" t="s">
-        <v>4072</v>
+        <v>4070</v>
       </c>
     </row>
     <row r="691" spans="1:4">
@@ -32980,13 +32993,13 @@
         <v>690</v>
       </c>
       <c r="B691" s="4" t="s">
-        <v>4067</v>
+        <v>4065</v>
       </c>
       <c r="C691" s="17" t="s">
-        <v>4070</v>
+        <v>4068</v>
       </c>
       <c r="D691" s="26" t="s">
-        <v>4073</v>
+        <v>4071</v>
       </c>
     </row>
     <row r="692" spans="1:4">
@@ -33722,13 +33735,13 @@
         <v>743</v>
       </c>
       <c r="B744" s="4" t="s">
+        <v>4020</v>
+      </c>
+      <c r="C744" s="17" t="s">
+        <v>4021</v>
+      </c>
+      <c r="D744" s="24" t="s">
         <v>4022</v>
-      </c>
-      <c r="C744" s="17" t="s">
-        <v>4023</v>
-      </c>
-      <c r="D744" s="24" t="s">
-        <v>4024</v>
       </c>
     </row>
     <row r="745" spans="1:4">
@@ -33736,13 +33749,13 @@
         <v>744</v>
       </c>
       <c r="B745" s="4" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C745" s="17" t="s">
+        <v>4029</v>
+      </c>
+      <c r="D745" s="24" t="s">
         <v>4030</v>
-      </c>
-      <c r="C745" s="17" t="s">
-        <v>4031</v>
-      </c>
-      <c r="D745" s="24" t="s">
-        <v>4032</v>
       </c>
     </row>
     <row r="746" spans="1:4">
@@ -33750,13 +33763,13 @@
         <v>745</v>
       </c>
       <c r="B746" s="4" t="s">
-        <v>4035</v>
+        <v>4033</v>
       </c>
       <c r="C746" s="17" t="s">
-        <v>4033</v>
+        <v>4031</v>
       </c>
       <c r="D746" s="24" t="s">
-        <v>4034</v>
+        <v>4032</v>
       </c>
     </row>
     <row r="747" spans="1:4">
@@ -33764,13 +33777,13 @@
         <v>746</v>
       </c>
       <c r="B747" s="4" t="s">
-        <v>4044</v>
+        <v>4042</v>
       </c>
       <c r="C747" s="17" t="s">
-        <v>4036</v>
+        <v>4034</v>
       </c>
       <c r="D747" s="24" t="s">
-        <v>4037</v>
+        <v>4035</v>
       </c>
     </row>
     <row r="748" spans="1:4">
@@ -33778,13 +33791,13 @@
         <v>747</v>
       </c>
       <c r="B748" s="4" t="s">
-        <v>4040</v>
+        <v>4038</v>
       </c>
       <c r="C748" s="17" t="s">
-        <v>4038</v>
+        <v>4036</v>
       </c>
       <c r="D748" s="24" t="s">
-        <v>4039</v>
+        <v>4037</v>
       </c>
     </row>
     <row r="749" spans="1:4">
@@ -33792,13 +33805,13 @@
         <v>748</v>
       </c>
       <c r="B749" s="4" t="s">
+        <v>4039</v>
+      </c>
+      <c r="C749" s="17" t="s">
+        <v>4040</v>
+      </c>
+      <c r="D749" s="24" t="s">
         <v>4041</v>
-      </c>
-      <c r="C749" s="17" t="s">
-        <v>4042</v>
-      </c>
-      <c r="D749" s="24" t="s">
-        <v>4043</v>
       </c>
     </row>
     <row r="750" spans="1:4">
@@ -33806,13 +33819,13 @@
         <v>749</v>
       </c>
       <c r="B750" s="4" t="s">
-        <v>4049</v>
+        <v>4047</v>
       </c>
       <c r="C750" s="17" t="s">
-        <v>4047</v>
+        <v>4045</v>
       </c>
       <c r="D750" s="24" t="s">
-        <v>4048</v>
+        <v>4046</v>
       </c>
     </row>
     <row r="751" spans="1:4">
@@ -33820,13 +33833,13 @@
         <v>750</v>
       </c>
       <c r="B751" s="4" t="s">
+        <v>4052</v>
+      </c>
+      <c r="C751" s="17" t="s">
+        <v>4053</v>
+      </c>
+      <c r="D751" s="24" t="s">
         <v>4054</v>
-      </c>
-      <c r="C751" s="17" t="s">
-        <v>4055</v>
-      </c>
-      <c r="D751" s="24" t="s">
-        <v>4056</v>
       </c>
     </row>
     <row r="752" spans="1:4">
@@ -33834,13 +33847,13 @@
         <v>751</v>
       </c>
       <c r="B752" s="4" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C752" s="17" t="s">
+        <v>4056</v>
+      </c>
+      <c r="D752" s="24" t="s">
         <v>4057</v>
-      </c>
-      <c r="C752" s="17" t="s">
-        <v>4058</v>
-      </c>
-      <c r="D752" s="24" t="s">
-        <v>4059</v>
       </c>
     </row>
     <row r="753" spans="1:4">
@@ -33848,13 +33861,13 @@
         <v>752</v>
       </c>
       <c r="B753" s="4" t="s">
+        <v>4058</v>
+      </c>
+      <c r="C753" s="17" t="s">
+        <v>4059</v>
+      </c>
+      <c r="D753" s="24" t="s">
         <v>4060</v>
-      </c>
-      <c r="C753" s="17" t="s">
-        <v>4061</v>
-      </c>
-      <c r="D753" s="24" t="s">
-        <v>4062</v>
       </c>
     </row>
     <row r="754" spans="1:4">
@@ -33862,13 +33875,13 @@
         <v>753</v>
       </c>
       <c r="B754" s="4" t="s">
+        <v>4061</v>
+      </c>
+      <c r="C754" s="17" t="s">
+        <v>4062</v>
+      </c>
+      <c r="D754" s="24" t="s">
         <v>4063</v>
-      </c>
-      <c r="C754" s="17" t="s">
-        <v>4064</v>
-      </c>
-      <c r="D754" s="24" t="s">
-        <v>4065</v>
       </c>
     </row>
     <row r="755" spans="1:4">
@@ -33876,13 +33889,13 @@
         <v>754</v>
       </c>
       <c r="B755" s="4" t="s">
-        <v>4074</v>
+        <v>4072</v>
       </c>
       <c r="C755" s="17" t="s">
-        <v>4075</v>
+        <v>4073</v>
       </c>
       <c r="D755" s="24" t="s">
-        <v>4102</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="756" spans="1:4">
@@ -33890,13 +33903,13 @@
         <v>755</v>
       </c>
       <c r="B756" s="4" t="s">
-        <v>4076</v>
+        <v>4074</v>
       </c>
       <c r="C756" s="17" t="s">
-        <v>4077</v>
+        <v>4075</v>
       </c>
       <c r="D756" s="24" t="s">
-        <v>4103</v>
+        <v>4101</v>
       </c>
     </row>
     <row r="757" spans="1:4">
@@ -33904,13 +33917,13 @@
         <v>756</v>
       </c>
       <c r="B757" s="4" t="s">
-        <v>4078</v>
+        <v>4076</v>
       </c>
       <c r="C757" s="17" t="s">
-        <v>4079</v>
+        <v>4077</v>
       </c>
       <c r="D757" s="24" t="s">
-        <v>4091</v>
+        <v>4089</v>
       </c>
     </row>
     <row r="758" spans="1:4">
@@ -33918,13 +33931,13 @@
         <v>757</v>
       </c>
       <c r="B758" s="4" t="s">
-        <v>4080</v>
+        <v>4078</v>
       </c>
       <c r="C758" s="17" t="s">
-        <v>4081</v>
+        <v>4079</v>
       </c>
       <c r="D758" s="24" t="s">
-        <v>4092</v>
+        <v>4090</v>
       </c>
     </row>
     <row r="759" spans="1:4">
@@ -33932,13 +33945,13 @@
         <v>758</v>
       </c>
       <c r="B759" s="4" t="s">
-        <v>4082</v>
+        <v>4080</v>
       </c>
       <c r="C759" s="17" t="s">
-        <v>4083</v>
+        <v>4081</v>
       </c>
       <c r="D759" s="24" t="s">
-        <v>4093</v>
+        <v>4091</v>
       </c>
     </row>
     <row r="760" spans="1:4">
@@ -33946,13 +33959,13 @@
         <v>759</v>
       </c>
       <c r="B760" s="4" t="s">
-        <v>4084</v>
+        <v>4082</v>
       </c>
       <c r="C760" s="17" t="s">
-        <v>4085</v>
+        <v>4083</v>
       </c>
       <c r="D760" s="24" t="s">
-        <v>4094</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="761" spans="1:4">
@@ -33960,13 +33973,13 @@
         <v>760</v>
       </c>
       <c r="B761" s="4" t="s">
-        <v>4086</v>
+        <v>4084</v>
       </c>
       <c r="C761" s="17" t="s">
-        <v>4087</v>
+        <v>4085</v>
       </c>
       <c r="D761" s="24" t="s">
-        <v>4095</v>
+        <v>4093</v>
       </c>
     </row>
     <row r="762" spans="1:4">
@@ -33974,13 +33987,13 @@
         <v>761</v>
       </c>
       <c r="B762" s="4" t="s">
-        <v>4105</v>
+        <v>4103</v>
       </c>
       <c r="C762" s="17" t="s">
-        <v>4106</v>
+        <v>4118</v>
       </c>
       <c r="D762" s="24" t="s">
-        <v>4107</v>
+        <v>4119</v>
       </c>
     </row>
     <row r="763" spans="1:4">
@@ -33988,13 +34001,13 @@
         <v>762</v>
       </c>
       <c r="B763" s="4" t="s">
-        <v>4088</v>
+        <v>4086</v>
       </c>
       <c r="C763" s="17" t="s">
-        <v>4089</v>
+        <v>4087</v>
       </c>
       <c r="D763" s="24" t="s">
-        <v>4096</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="764" spans="1:4">
@@ -34002,13 +34015,13 @@
         <v>763</v>
       </c>
       <c r="B764" s="4" t="s">
-        <v>4090</v>
+        <v>4088</v>
       </c>
       <c r="C764" s="17" t="s">
-        <v>4097</v>
+        <v>4095</v>
       </c>
       <c r="D764" s="24" t="s">
-        <v>4098</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="765" spans="1:4">
@@ -34016,13 +34029,13 @@
         <v>764</v>
       </c>
       <c r="B765" s="4" t="s">
+        <v>4097</v>
+      </c>
+      <c r="C765" s="17" t="s">
+        <v>4098</v>
+      </c>
+      <c r="D765" s="24" t="s">
         <v>4099</v>
-      </c>
-      <c r="C765" s="17" t="s">
-        <v>4100</v>
-      </c>
-      <c r="D765" s="24" t="s">
-        <v>4101</v>
       </c>
     </row>
     <row r="766" spans="1:4">
@@ -34030,13 +34043,13 @@
         <v>765</v>
       </c>
       <c r="B766" s="4" t="s">
-        <v>4110</v>
+        <v>4106</v>
       </c>
       <c r="C766" s="17" t="s">
-        <v>4108</v>
+        <v>4104</v>
       </c>
       <c r="D766" s="24" t="s">
-        <v>4109</v>
+        <v>4105</v>
       </c>
     </row>
     <row r="767" spans="1:4">
@@ -34044,13 +34057,13 @@
         <v>766</v>
       </c>
       <c r="B767" s="4" t="s">
-        <v>4111</v>
+        <v>4107</v>
       </c>
       <c r="C767" s="17" t="s">
-        <v>4112</v>
+        <v>4108</v>
       </c>
       <c r="D767" s="24" t="s">
-        <v>4114</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="768" spans="1:4">
@@ -34058,13 +34071,13 @@
         <v>767</v>
       </c>
       <c r="B768" s="4" t="s">
-        <v>4113</v>
+        <v>4109</v>
       </c>
       <c r="C768" s="17" t="s">
-        <v>4115</v>
+        <v>4111</v>
       </c>
       <c r="D768" s="24" t="s">
-        <v>4116</v>
+        <v>4112</v>
       </c>
     </row>
     <row r="769" spans="1:4">
@@ -34072,13 +34085,13 @@
         <v>768</v>
       </c>
       <c r="B769" s="4" t="s">
-        <v>4119</v>
+        <v>4115</v>
       </c>
       <c r="C769" s="17" t="s">
-        <v>4117</v>
+        <v>4113</v>
       </c>
       <c r="D769" s="24" t="s">
-        <v>4118</v>
+        <v>4114</v>
       </c>
     </row>
     <row r="770" spans="1:4">

</xml_diff>